<commit_message>
update Vocabulary Statistic Chart for TOEFL.xlsx
</commit_message>
<xml_diff>
--- a/english_learning/Vocabulary Statistic Chart for TOEFL.xlsx
+++ b/english_learning/Vocabulary Statistic Chart for TOEFL.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="136">
   <si>
     <t>Expression</t>
   </si>
@@ -368,9 +368,6 @@
     <t>障碍课程</t>
   </si>
   <si>
-    <t>将死</t>
-  </si>
-  <si>
     <t>足球场</t>
   </si>
   <si>
@@ -380,9 +377,6 @@
     <t>连锁</t>
   </si>
   <si>
-    <t>凸起和凹陷</t>
-  </si>
-  <si>
     <t>太空球</t>
   </si>
   <si>
@@ -410,9 +404,6 @@
     <t>城堡</t>
   </si>
   <si>
-    <t>魁地奇</t>
-  </si>
-  <si>
     <t>扫帚</t>
   </si>
   <si>
@@ -423,6 +414,24 @@
   </si>
   <si>
     <t>球</t>
+  </si>
+  <si>
+    <t>鬼脸</t>
+  </si>
+  <si>
+    <t>水下曲棍球</t>
+  </si>
+  <si>
+    <t>凸起和凹陷（拼图）</t>
+  </si>
+  <si>
+    <t>魁地奇（Harry Porter女巫游戏）</t>
+  </si>
+  <si>
+    <t>（象棋）将死</t>
+  </si>
+  <si>
+    <t>pitch: 场</t>
   </si>
 </sst>
 </file>
@@ -870,8 +879,8 @@
   <dimension ref="B1:M264"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E66" sqref="E66"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
@@ -2091,7 +2100,7 @@
       </c>
       <c r="F45" s="5"/>
       <c r="G45" s="5" t="s">
-        <v>114</v>
+        <v>134</v>
       </c>
       <c r="H45" s="5"/>
       <c r="I45" s="5"/>
@@ -2119,9 +2128,11 @@
       </c>
       <c r="F46" s="5"/>
       <c r="G46" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="H46" s="5"/>
+        <v>114</v>
+      </c>
+      <c r="H46" s="5" t="s">
+        <v>135</v>
+      </c>
       <c r="I46" s="5"/>
       <c r="J46" s="5"/>
       <c r="K46" s="5">
@@ -2147,7 +2158,7 @@
       </c>
       <c r="F47" s="5"/>
       <c r="G47" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H47" s="5"/>
       <c r="I47" s="5"/>
@@ -2175,7 +2186,7 @@
       </c>
       <c r="F48" s="5"/>
       <c r="G48" s="5" t="s">
-        <v>92</v>
+        <v>131</v>
       </c>
       <c r="H48" s="5"/>
       <c r="I48" s="5"/>
@@ -2203,7 +2214,7 @@
       </c>
       <c r="F49" s="5"/>
       <c r="G49" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H49" s="5"/>
       <c r="I49" s="5"/>
@@ -2231,7 +2242,7 @@
       </c>
       <c r="F50" s="5"/>
       <c r="G50" s="5" t="s">
-        <v>118</v>
+        <v>132</v>
       </c>
       <c r="H50" s="5"/>
       <c r="I50" s="5"/>
@@ -2259,7 +2270,7 @@
       </c>
       <c r="F51" s="5"/>
       <c r="G51" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H51" s="5"/>
       <c r="I51" s="5"/>
@@ -2287,7 +2298,7 @@
       </c>
       <c r="F52" s="5"/>
       <c r="G52" s="5" t="s">
-        <v>96</v>
+        <v>130</v>
       </c>
       <c r="H52" s="5"/>
       <c r="I52" s="5"/>
@@ -2315,7 +2326,7 @@
       </c>
       <c r="F53" s="5"/>
       <c r="G53" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H53" s="5"/>
       <c r="I53" s="5"/>
@@ -2343,7 +2354,7 @@
       </c>
       <c r="F54" s="5"/>
       <c r="G54" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H54" s="5"/>
       <c r="I54" s="5"/>
@@ -2371,7 +2382,7 @@
       </c>
       <c r="F55" s="5"/>
       <c r="G55" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="H55" s="5"/>
       <c r="I55" s="5"/>
@@ -2399,7 +2410,7 @@
       </c>
       <c r="F56" s="5"/>
       <c r="G56" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H56" s="5"/>
       <c r="I56" s="5"/>
@@ -2427,7 +2438,7 @@
       </c>
       <c r="F57" s="5"/>
       <c r="G57" s="5" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H57" s="5"/>
       <c r="I57" s="5"/>
@@ -2455,7 +2466,7 @@
       </c>
       <c r="F58" s="5"/>
       <c r="G58" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H58" s="5"/>
       <c r="I58" s="5"/>
@@ -2483,7 +2494,7 @@
       </c>
       <c r="F59" s="5"/>
       <c r="G59" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="H59" s="5"/>
       <c r="I59" s="5"/>
@@ -2511,7 +2522,7 @@
       </c>
       <c r="F60" s="5"/>
       <c r="G60" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H60" s="5"/>
       <c r="I60" s="5"/>
@@ -2539,7 +2550,7 @@
       </c>
       <c r="F61" s="5"/>
       <c r="G61" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="H61" s="5"/>
       <c r="I61" s="5"/>
@@ -2567,7 +2578,7 @@
       </c>
       <c r="F62" s="5"/>
       <c r="G62" s="5" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="H62" s="5"/>
       <c r="I62" s="5"/>
@@ -2595,7 +2606,7 @@
       </c>
       <c r="F63" s="5"/>
       <c r="G63" s="5" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="H63" s="5"/>
       <c r="I63" s="5"/>
@@ -2623,7 +2634,7 @@
       </c>
       <c r="F64" s="5"/>
       <c r="G64" s="5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H64" s="5"/>
       <c r="I64" s="5"/>
@@ -2651,7 +2662,7 @@
       </c>
       <c r="F65" s="5"/>
       <c r="G65" s="5" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="H65" s="5"/>
       <c r="I65" s="5"/>

</xml_diff>

<commit_message>
english_learning/Vocabulary Statistic Chart for TOEFL.xlsx
</commit_message>
<xml_diff>
--- a/english_learning/Vocabulary Statistic Chart for TOEFL.xlsx
+++ b/english_learning/Vocabulary Statistic Chart for TOEFL.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19301" windowHeight="8007" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19301" windowHeight="8007"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
     <sheet name="TOEFL" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">main!$B$4:$M$104</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">main!$B$4:$M$175</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">TOEFL!$B$4:$M$4</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1725" uniqueCount="839">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1866" uniqueCount="910">
   <si>
     <t>Expression</t>
   </si>
@@ -2547,6 +2547,219 @@
   </si>
   <si>
     <t>20mins</t>
+  </si>
+  <si>
+    <t>extracurricular</t>
+  </si>
+  <si>
+    <t>distinctive</t>
+  </si>
+  <si>
+    <t>dean</t>
+  </si>
+  <si>
+    <t>camaraderie</t>
+  </si>
+  <si>
+    <t>intramural</t>
+  </si>
+  <si>
+    <t>confinement</t>
+  </si>
+  <si>
+    <t>partake</t>
+  </si>
+  <si>
+    <t>guts</t>
+  </si>
+  <si>
+    <t>conviction</t>
+  </si>
+  <si>
+    <t>introverted</t>
+  </si>
+  <si>
+    <t>come out of one's shell</t>
+  </si>
+  <si>
+    <t>profound impact</t>
+  </si>
+  <si>
+    <t>broaden your horizon</t>
+  </si>
+  <si>
+    <t>bite the bullet</t>
+  </si>
+  <si>
+    <t>varsity athlete</t>
+  </si>
+  <si>
+    <t>varsity sport</t>
+  </si>
+  <si>
+    <t>varsity athletics</t>
+  </si>
+  <si>
+    <t>service-leaning activity</t>
+  </si>
+  <si>
+    <t>musketeer</t>
+  </si>
+  <si>
+    <t>课外</t>
+  </si>
+  <si>
+    <t>独特</t>
+  </si>
+  <si>
+    <t>院长</t>
+  </si>
+  <si>
+    <t>友情</t>
+  </si>
+  <si>
+    <t>坐月子</t>
+  </si>
+  <si>
+    <t>参加</t>
+  </si>
+  <si>
+    <t>胆量</t>
+  </si>
+  <si>
+    <t>信念</t>
+  </si>
+  <si>
+    <t>内敛</t>
+  </si>
+  <si>
+    <t>从一个人的壳里出来</t>
+  </si>
+  <si>
+    <t>深远影响</t>
+  </si>
+  <si>
+    <t>拓宽视野</t>
+  </si>
+  <si>
+    <t>硬着头皮</t>
+  </si>
+  <si>
+    <t>大学运动员</t>
+  </si>
+  <si>
+    <t>大学运动</t>
+  </si>
+  <si>
+    <t>大学竞技</t>
+  </si>
+  <si>
+    <t>服务倾向活动</t>
+  </si>
+  <si>
+    <t>火枪手</t>
+  </si>
+  <si>
+    <t>bit: past tense</t>
+  </si>
+  <si>
+    <t>wallflower</t>
+  </si>
+  <si>
+    <t>局外人 (用来描述girl)</t>
+  </si>
+  <si>
+    <t>壁间(indoor)</t>
+  </si>
+  <si>
+    <t>sing your heart out</t>
+  </si>
+  <si>
+    <t>唱出你的心</t>
+  </si>
+  <si>
+    <t>gusto and bravado</t>
+  </si>
+  <si>
+    <t>有滋有味, 虚张声势</t>
+  </si>
+  <si>
+    <t>demoralize</t>
+  </si>
+  <si>
+    <t>idiom</t>
+  </si>
+  <si>
+    <t>boredom</t>
+  </si>
+  <si>
+    <t>lack of empowerment</t>
+  </si>
+  <si>
+    <t>lack of progress</t>
+  </si>
+  <si>
+    <t>put his heart and soul into</t>
+  </si>
+  <si>
+    <t>steal the thunder</t>
+  </si>
+  <si>
+    <t>keep up the good work</t>
+  </si>
+  <si>
+    <t>going to extra mile</t>
+  </si>
+  <si>
+    <t>guiding spirit</t>
+  </si>
+  <si>
+    <t>have an eye for</t>
+  </si>
+  <si>
+    <t>Sarah is in over her head at work.</t>
+  </si>
+  <si>
+    <t>cash flow</t>
+  </si>
+  <si>
+    <t>士气低落</t>
+  </si>
+  <si>
+    <t>成语</t>
+  </si>
+  <si>
+    <t>无聊</t>
+  </si>
+  <si>
+    <t>缺乏赋权</t>
+  </si>
+  <si>
+    <t>缺乏进展</t>
+  </si>
+  <si>
+    <t>把他的心灵和灵魂融入其中</t>
+  </si>
+  <si>
+    <t>偷了雷</t>
+  </si>
+  <si>
+    <t>保持良好的工作</t>
+  </si>
+  <si>
+    <t>加倍努力</t>
+  </si>
+  <si>
+    <t>指导精神</t>
+  </si>
+  <si>
+    <t>关注</t>
+  </si>
+  <si>
+    <t>莎拉正在工作。</t>
+  </si>
+  <si>
+    <t>现金周转</t>
   </si>
 </sst>
 </file>
@@ -2999,11 +3212,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:M523"/>
+  <dimension ref="B1:M521"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F148" sqref="F148"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A174" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J183" sqref="J183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
@@ -6611,7 +6824,7 @@
         <v>124</v>
       </c>
       <c r="C128" s="3">
-        <v>43515</v>
+        <v>43516</v>
       </c>
       <c r="D128" s="5" t="s">
         <v>213</v>
@@ -6639,7 +6852,7 @@
         <v>125</v>
       </c>
       <c r="C129" s="3">
-        <v>43515</v>
+        <v>43516</v>
       </c>
       <c r="D129" s="5" t="s">
         <v>213</v>
@@ -6667,7 +6880,7 @@
         <v>126</v>
       </c>
       <c r="C130" s="3">
-        <v>43515</v>
+        <v>43516</v>
       </c>
       <c r="D130" s="5" t="s">
         <v>213</v>
@@ -6695,7 +6908,7 @@
         <v>127</v>
       </c>
       <c r="C131" s="3">
-        <v>43515</v>
+        <v>43516</v>
       </c>
       <c r="D131" s="5" t="s">
         <v>213</v>
@@ -6723,7 +6936,7 @@
         <v>128</v>
       </c>
       <c r="C132" s="3">
-        <v>43515</v>
+        <v>43516</v>
       </c>
       <c r="D132" s="5" t="s">
         <v>213</v>
@@ -6751,7 +6964,7 @@
         <v>129</v>
       </c>
       <c r="C133" s="3">
-        <v>43515</v>
+        <v>43516</v>
       </c>
       <c r="D133" s="5" t="s">
         <v>213</v>
@@ -6779,7 +6992,7 @@
         <v>130</v>
       </c>
       <c r="C134" s="3">
-        <v>43515</v>
+        <v>43516</v>
       </c>
       <c r="D134" s="5" t="s">
         <v>213</v>
@@ -6807,7 +7020,7 @@
         <v>131</v>
       </c>
       <c r="C135" s="3">
-        <v>43515</v>
+        <v>43516</v>
       </c>
       <c r="D135" s="5" t="s">
         <v>213</v>
@@ -6835,7 +7048,7 @@
         <v>132</v>
       </c>
       <c r="C136" s="3">
-        <v>43515</v>
+        <v>43516</v>
       </c>
       <c r="D136" s="5" t="s">
         <v>213</v>
@@ -6863,7 +7076,7 @@
         <v>133</v>
       </c>
       <c r="C137" s="3">
-        <v>43515</v>
+        <v>43516</v>
       </c>
       <c r="D137" s="5" t="s">
         <v>213</v>
@@ -6891,7 +7104,7 @@
         <v>134</v>
       </c>
       <c r="C138" s="3">
-        <v>43515</v>
+        <v>43516</v>
       </c>
       <c r="D138" s="5" t="s">
         <v>213</v>
@@ -6919,7 +7132,7 @@
         <v>135</v>
       </c>
       <c r="C139" s="3">
-        <v>43515</v>
+        <v>43516</v>
       </c>
       <c r="D139" s="5" t="s">
         <v>213</v>
@@ -6947,7 +7160,7 @@
         <v>136</v>
       </c>
       <c r="C140" s="3">
-        <v>43515</v>
+        <v>43516</v>
       </c>
       <c r="D140" s="5" t="s">
         <v>213</v>
@@ -6975,7 +7188,7 @@
         <v>137</v>
       </c>
       <c r="C141" s="3">
-        <v>43515</v>
+        <v>43516</v>
       </c>
       <c r="D141" s="5" t="s">
         <v>213</v>
@@ -7003,7 +7216,7 @@
         <v>138</v>
       </c>
       <c r="C142" s="3">
-        <v>43515</v>
+        <v>43516</v>
       </c>
       <c r="D142" s="5" t="s">
         <v>213</v>
@@ -7031,7 +7244,7 @@
         <v>139</v>
       </c>
       <c r="C143" s="3">
-        <v>43515</v>
+        <v>43516</v>
       </c>
       <c r="D143" s="5" t="s">
         <v>213</v>
@@ -7059,7 +7272,7 @@
         <v>140</v>
       </c>
       <c r="C144" s="3">
-        <v>43515</v>
+        <v>43516</v>
       </c>
       <c r="D144" s="5" t="s">
         <v>213</v>
@@ -7087,7 +7300,7 @@
         <v>141</v>
       </c>
       <c r="C145" s="3">
-        <v>43515</v>
+        <v>43516</v>
       </c>
       <c r="D145" s="5" t="s">
         <v>213</v>
@@ -7115,7 +7328,7 @@
         <v>142</v>
       </c>
       <c r="C146" s="3">
-        <v>43516</v>
+        <v>43517</v>
       </c>
       <c r="D146" s="5" t="s">
         <v>213</v>
@@ -7143,7 +7356,7 @@
         <v>143</v>
       </c>
       <c r="C147" s="3">
-        <v>43516</v>
+        <v>43517</v>
       </c>
       <c r="D147" s="5" t="s">
         <v>213</v>
@@ -7171,7 +7384,7 @@
         <v>144</v>
       </c>
       <c r="C148" s="3">
-        <v>43516</v>
+        <v>43517</v>
       </c>
       <c r="D148" s="5" t="s">
         <v>213</v>
@@ -7199,7 +7412,7 @@
         <v>145</v>
       </c>
       <c r="C149" s="3">
-        <v>43516</v>
+        <v>43517</v>
       </c>
       <c r="D149" s="5" t="s">
         <v>213</v>
@@ -7227,7 +7440,7 @@
         <v>146</v>
       </c>
       <c r="C150" s="3">
-        <v>43516</v>
+        <v>43517</v>
       </c>
       <c r="D150" s="5" t="s">
         <v>213</v>
@@ -7255,7 +7468,7 @@
         <v>147</v>
       </c>
       <c r="C151" s="3">
-        <v>43516</v>
+        <v>43517</v>
       </c>
       <c r="D151" s="5" t="s">
         <v>213</v>
@@ -7283,7 +7496,7 @@
         <v>148</v>
       </c>
       <c r="C152" s="3">
-        <v>43516</v>
+        <v>43517</v>
       </c>
       <c r="D152" s="5" t="s">
         <v>213</v>
@@ -7311,7 +7524,7 @@
         <v>149</v>
       </c>
       <c r="C153" s="3">
-        <v>43516</v>
+        <v>43517</v>
       </c>
       <c r="D153" s="5" t="s">
         <v>213</v>
@@ -7335,493 +7548,985 @@
       <c r="M153" s="5"/>
     </row>
     <row r="154" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B154" s="2"/>
-      <c r="C154" s="3"/>
-      <c r="D154" s="5"/>
-      <c r="E154" s="5"/>
+      <c r="B154" s="2">
+        <v>150</v>
+      </c>
+      <c r="C154" s="3">
+        <v>43518</v>
+      </c>
+      <c r="D154" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E154" s="5" t="s">
+        <v>839</v>
+      </c>
       <c r="F154" s="5"/>
-      <c r="G154" s="5"/>
+      <c r="G154" s="5" t="s">
+        <v>858</v>
+      </c>
       <c r="H154" s="5"/>
       <c r="I154" s="5"/>
       <c r="J154" s="5"/>
-      <c r="K154" s="5"/>
-      <c r="L154" s="5"/>
+      <c r="K154" s="5">
+        <v>1</v>
+      </c>
+      <c r="L154" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M154" s="5"/>
     </row>
     <row r="155" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B155" s="2"/>
-      <c r="C155" s="3"/>
-      <c r="D155" s="5"/>
-      <c r="E155" s="5"/>
+      <c r="B155" s="2">
+        <v>151</v>
+      </c>
+      <c r="C155" s="3">
+        <v>43518</v>
+      </c>
+      <c r="D155" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E155" s="5" t="s">
+        <v>840</v>
+      </c>
       <c r="F155" s="5"/>
-      <c r="G155" s="5"/>
+      <c r="G155" s="5" t="s">
+        <v>859</v>
+      </c>
       <c r="H155" s="5"/>
       <c r="I155" s="5"/>
       <c r="J155" s="5"/>
-      <c r="K155" s="5"/>
-      <c r="L155" s="5"/>
+      <c r="K155" s="5">
+        <v>1</v>
+      </c>
+      <c r="L155" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M155" s="5"/>
     </row>
     <row r="156" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B156" s="2"/>
-      <c r="C156" s="3"/>
-      <c r="D156" s="5"/>
-      <c r="E156" s="5"/>
+      <c r="B156" s="2">
+        <v>152</v>
+      </c>
+      <c r="C156" s="3">
+        <v>43518</v>
+      </c>
+      <c r="D156" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E156" s="5" t="s">
+        <v>841</v>
+      </c>
       <c r="F156" s="5"/>
-      <c r="G156" s="5"/>
+      <c r="G156" s="5" t="s">
+        <v>860</v>
+      </c>
       <c r="H156" s="5"/>
       <c r="I156" s="5"/>
       <c r="J156" s="5"/>
-      <c r="K156" s="5"/>
-      <c r="L156" s="5"/>
+      <c r="K156" s="5">
+        <v>1</v>
+      </c>
+      <c r="L156" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M156" s="5"/>
     </row>
     <row r="157" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B157" s="2"/>
-      <c r="C157" s="3"/>
-      <c r="D157" s="5"/>
-      <c r="E157" s="5"/>
+      <c r="B157" s="2">
+        <v>153</v>
+      </c>
+      <c r="C157" s="3">
+        <v>43518</v>
+      </c>
+      <c r="D157" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E157" s="5" t="s">
+        <v>842</v>
+      </c>
       <c r="F157" s="5"/>
-      <c r="G157" s="5"/>
+      <c r="G157" s="5" t="s">
+        <v>861</v>
+      </c>
       <c r="H157" s="5"/>
       <c r="I157" s="5"/>
       <c r="J157" s="5"/>
-      <c r="K157" s="5"/>
-      <c r="L157" s="5"/>
+      <c r="K157" s="5">
+        <v>1</v>
+      </c>
+      <c r="L157" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M157" s="5"/>
     </row>
     <row r="158" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B158" s="2"/>
-      <c r="C158" s="3"/>
-      <c r="D158" s="5"/>
-      <c r="E158" s="5"/>
+      <c r="B158" s="2">
+        <v>154</v>
+      </c>
+      <c r="C158" s="3">
+        <v>43518</v>
+      </c>
+      <c r="D158" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E158" s="5" t="s">
+        <v>843</v>
+      </c>
       <c r="F158" s="5"/>
-      <c r="G158" s="5"/>
+      <c r="G158" s="5" t="s">
+        <v>879</v>
+      </c>
       <c r="H158" s="5"/>
       <c r="I158" s="5"/>
       <c r="J158" s="5"/>
-      <c r="K158" s="5"/>
-      <c r="L158" s="5"/>
+      <c r="K158" s="5">
+        <v>1</v>
+      </c>
+      <c r="L158" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M158" s="5"/>
     </row>
     <row r="159" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B159" s="2"/>
-      <c r="C159" s="3"/>
-      <c r="D159" s="5"/>
-      <c r="E159" s="5"/>
+      <c r="B159" s="2">
+        <v>155</v>
+      </c>
+      <c r="C159" s="3">
+        <v>43518</v>
+      </c>
+      <c r="D159" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E159" s="5" t="s">
+        <v>844</v>
+      </c>
       <c r="F159" s="5"/>
-      <c r="G159" s="5"/>
+      <c r="G159" s="5" t="s">
+        <v>862</v>
+      </c>
       <c r="H159" s="5"/>
       <c r="I159" s="5"/>
       <c r="J159" s="5"/>
-      <c r="K159" s="5"/>
-      <c r="L159" s="5"/>
+      <c r="K159" s="5">
+        <v>1</v>
+      </c>
+      <c r="L159" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M159" s="5"/>
     </row>
     <row r="160" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B160" s="2"/>
-      <c r="C160" s="3"/>
-      <c r="D160" s="5"/>
-      <c r="E160" s="5"/>
+      <c r="B160" s="2">
+        <v>156</v>
+      </c>
+      <c r="C160" s="3">
+        <v>43518</v>
+      </c>
+      <c r="D160" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E160" s="5" t="s">
+        <v>845</v>
+      </c>
       <c r="F160" s="5"/>
-      <c r="G160" s="5"/>
+      <c r="G160" s="5" t="s">
+        <v>863</v>
+      </c>
       <c r="H160" s="5"/>
       <c r="I160" s="5"/>
       <c r="J160" s="5"/>
-      <c r="K160" s="5"/>
-      <c r="L160" s="5"/>
+      <c r="K160" s="5">
+        <v>1</v>
+      </c>
+      <c r="L160" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M160" s="5"/>
     </row>
     <row r="161" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B161" s="2"/>
-      <c r="C161" s="3"/>
-      <c r="D161" s="5"/>
-      <c r="E161" s="5"/>
+      <c r="B161" s="2">
+        <v>157</v>
+      </c>
+      <c r="C161" s="3">
+        <v>43518</v>
+      </c>
+      <c r="D161" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E161" s="5" t="s">
+        <v>846</v>
+      </c>
       <c r="F161" s="5"/>
-      <c r="G161" s="5"/>
+      <c r="G161" s="5" t="s">
+        <v>864</v>
+      </c>
       <c r="H161" s="5"/>
       <c r="I161" s="5"/>
       <c r="J161" s="5"/>
-      <c r="K161" s="5"/>
-      <c r="L161" s="5"/>
+      <c r="K161" s="5">
+        <v>1</v>
+      </c>
+      <c r="L161" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M161" s="5"/>
     </row>
     <row r="162" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B162" s="2"/>
-      <c r="C162" s="3"/>
-      <c r="D162" s="5"/>
-      <c r="E162" s="5"/>
+      <c r="B162" s="2">
+        <v>158</v>
+      </c>
+      <c r="C162" s="3">
+        <v>43518</v>
+      </c>
+      <c r="D162" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E162" s="5" t="s">
+        <v>880</v>
+      </c>
       <c r="F162" s="5"/>
-      <c r="G162" s="5"/>
+      <c r="G162" s="5" t="s">
+        <v>881</v>
+      </c>
       <c r="H162" s="5"/>
       <c r="I162" s="5"/>
       <c r="J162" s="5"/>
-      <c r="K162" s="5"/>
-      <c r="L162" s="5"/>
+      <c r="K162" s="5">
+        <v>1</v>
+      </c>
+      <c r="L162" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M162" s="5"/>
     </row>
     <row r="163" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B163" s="2"/>
-      <c r="C163" s="3"/>
-      <c r="D163" s="5"/>
-      <c r="E163" s="5"/>
+      <c r="B163" s="2">
+        <v>159</v>
+      </c>
+      <c r="C163" s="3">
+        <v>43518</v>
+      </c>
+      <c r="D163" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E163" s="5" t="s">
+        <v>847</v>
+      </c>
       <c r="F163" s="5"/>
-      <c r="G163" s="5"/>
+      <c r="G163" s="5" t="s">
+        <v>865</v>
+      </c>
       <c r="H163" s="5"/>
       <c r="I163" s="5"/>
       <c r="J163" s="5"/>
-      <c r="K163" s="5"/>
-      <c r="L163" s="5"/>
+      <c r="K163" s="5">
+        <v>1</v>
+      </c>
+      <c r="L163" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M163" s="5"/>
     </row>
     <row r="164" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B164" s="2"/>
-      <c r="C164" s="3"/>
-      <c r="D164" s="5"/>
-      <c r="E164" s="5"/>
+      <c r="B164" s="2">
+        <v>160</v>
+      </c>
+      <c r="C164" s="3">
+        <v>43518</v>
+      </c>
+      <c r="D164" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E164" s="5" t="s">
+        <v>882</v>
+      </c>
       <c r="F164" s="5"/>
-      <c r="G164" s="5"/>
+      <c r="G164" s="5" t="s">
+        <v>883</v>
+      </c>
       <c r="H164" s="5"/>
       <c r="I164" s="5"/>
       <c r="J164" s="5"/>
-      <c r="K164" s="5"/>
-      <c r="L164" s="5"/>
+      <c r="K164" s="5">
+        <v>1</v>
+      </c>
+      <c r="L164" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M164" s="5"/>
     </row>
     <row r="165" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B165" s="2"/>
-      <c r="C165" s="3"/>
-      <c r="D165" s="5"/>
-      <c r="E165" s="5"/>
+      <c r="B165" s="2">
+        <v>161</v>
+      </c>
+      <c r="C165" s="3">
+        <v>43518</v>
+      </c>
+      <c r="D165" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E165" s="5" t="s">
+        <v>877</v>
+      </c>
       <c r="F165" s="5"/>
-      <c r="G165" s="5"/>
+      <c r="G165" s="5" t="s">
+        <v>878</v>
+      </c>
       <c r="H165" s="5"/>
       <c r="I165" s="5"/>
       <c r="J165" s="5"/>
-      <c r="K165" s="5"/>
-      <c r="L165" s="5"/>
+      <c r="K165" s="5">
+        <v>1</v>
+      </c>
+      <c r="L165" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M165" s="5"/>
     </row>
     <row r="166" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B166" s="2"/>
-      <c r="C166" s="3"/>
-      <c r="D166" s="5"/>
-      <c r="E166" s="5"/>
+      <c r="B166" s="2">
+        <v>162</v>
+      </c>
+      <c r="C166" s="3">
+        <v>43518</v>
+      </c>
+      <c r="D166" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E166" s="5" t="s">
+        <v>848</v>
+      </c>
       <c r="F166" s="5"/>
-      <c r="G166" s="5"/>
+      <c r="G166" s="5" t="s">
+        <v>866</v>
+      </c>
       <c r="H166" s="5"/>
       <c r="I166" s="5"/>
       <c r="J166" s="5"/>
-      <c r="K166" s="5"/>
-      <c r="L166" s="5"/>
+      <c r="K166" s="5">
+        <v>1</v>
+      </c>
+      <c r="L166" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M166" s="5"/>
     </row>
     <row r="167" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B167" s="2"/>
-      <c r="C167" s="3"/>
-      <c r="D167" s="5"/>
-      <c r="E167" s="5"/>
+      <c r="B167" s="2">
+        <v>163</v>
+      </c>
+      <c r="C167" s="3">
+        <v>43518</v>
+      </c>
+      <c r="D167" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E167" s="5" t="s">
+        <v>849</v>
+      </c>
       <c r="F167" s="5"/>
-      <c r="G167" s="5"/>
+      <c r="G167" s="5" t="s">
+        <v>867</v>
+      </c>
       <c r="H167" s="5"/>
       <c r="I167" s="5"/>
       <c r="J167" s="5"/>
-      <c r="K167" s="5"/>
-      <c r="L167" s="5"/>
+      <c r="K167" s="5">
+        <v>1</v>
+      </c>
+      <c r="L167" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M167" s="5"/>
     </row>
     <row r="168" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B168" s="2"/>
-      <c r="C168" s="3"/>
-      <c r="D168" s="5"/>
-      <c r="E168" s="5"/>
+      <c r="B168" s="2">
+        <v>164</v>
+      </c>
+      <c r="C168" s="3">
+        <v>43518</v>
+      </c>
+      <c r="D168" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E168" s="5" t="s">
+        <v>850</v>
+      </c>
       <c r="F168" s="5"/>
-      <c r="G168" s="5"/>
+      <c r="G168" s="5" t="s">
+        <v>868</v>
+      </c>
       <c r="H168" s="5"/>
       <c r="I168" s="5"/>
       <c r="J168" s="5"/>
-      <c r="K168" s="5"/>
-      <c r="L168" s="5"/>
+      <c r="K168" s="5">
+        <v>1</v>
+      </c>
+      <c r="L168" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M168" s="5"/>
     </row>
     <row r="169" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B169" s="2"/>
-      <c r="C169" s="3"/>
-      <c r="D169" s="5"/>
-      <c r="E169" s="5"/>
+      <c r="B169" s="2">
+        <v>165</v>
+      </c>
+      <c r="C169" s="3">
+        <v>43518</v>
+      </c>
+      <c r="D169" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E169" s="5" t="s">
+        <v>851</v>
+      </c>
       <c r="F169" s="5"/>
-      <c r="G169" s="5"/>
+      <c r="G169" s="5" t="s">
+        <v>869</v>
+      </c>
       <c r="H169" s="5"/>
       <c r="I169" s="5"/>
       <c r="J169" s="5"/>
-      <c r="K169" s="5"/>
-      <c r="L169" s="5"/>
+      <c r="K169" s="5">
+        <v>1</v>
+      </c>
+      <c r="L169" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M169" s="5"/>
     </row>
     <row r="170" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B170" s="2"/>
-      <c r="C170" s="3"/>
-      <c r="D170" s="5"/>
-      <c r="E170" s="5"/>
+      <c r="B170" s="2">
+        <v>166</v>
+      </c>
+      <c r="C170" s="3">
+        <v>43518</v>
+      </c>
+      <c r="D170" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E170" s="5" t="s">
+        <v>852</v>
+      </c>
       <c r="F170" s="5"/>
-      <c r="G170" s="5"/>
-      <c r="H170" s="5"/>
+      <c r="G170" s="5" t="s">
+        <v>870</v>
+      </c>
+      <c r="H170" s="5" t="s">
+        <v>876</v>
+      </c>
       <c r="I170" s="5"/>
       <c r="J170" s="5"/>
-      <c r="K170" s="5"/>
-      <c r="L170" s="5"/>
+      <c r="K170" s="5">
+        <v>1</v>
+      </c>
+      <c r="L170" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M170" s="5"/>
     </row>
     <row r="171" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B171" s="2"/>
-      <c r="C171" s="3"/>
-      <c r="D171" s="5"/>
-      <c r="E171" s="5"/>
+      <c r="B171" s="2">
+        <v>167</v>
+      </c>
+      <c r="C171" s="3">
+        <v>43518</v>
+      </c>
+      <c r="D171" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E171" s="5" t="s">
+        <v>853</v>
+      </c>
       <c r="F171" s="5"/>
-      <c r="G171" s="5"/>
+      <c r="G171" s="5" t="s">
+        <v>871</v>
+      </c>
       <c r="H171" s="5"/>
       <c r="I171" s="5"/>
       <c r="J171" s="5"/>
-      <c r="K171" s="5"/>
-      <c r="L171" s="5"/>
+      <c r="K171" s="5">
+        <v>1</v>
+      </c>
+      <c r="L171" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M171" s="5"/>
     </row>
     <row r="172" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B172" s="2"/>
-      <c r="C172" s="3"/>
-      <c r="D172" s="5"/>
-      <c r="E172" s="5"/>
+      <c r="B172" s="2">
+        <v>168</v>
+      </c>
+      <c r="C172" s="3">
+        <v>43518</v>
+      </c>
+      <c r="D172" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E172" s="5" t="s">
+        <v>854</v>
+      </c>
       <c r="F172" s="5"/>
-      <c r="G172" s="5"/>
+      <c r="G172" s="5" t="s">
+        <v>872</v>
+      </c>
       <c r="H172" s="5"/>
       <c r="I172" s="5"/>
       <c r="J172" s="5"/>
-      <c r="K172" s="5"/>
-      <c r="L172" s="5"/>
+      <c r="K172" s="5">
+        <v>1</v>
+      </c>
+      <c r="L172" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M172" s="5"/>
     </row>
     <row r="173" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B173" s="2"/>
-      <c r="C173" s="3"/>
-      <c r="D173" s="5"/>
-      <c r="E173" s="5"/>
+      <c r="B173" s="2">
+        <v>169</v>
+      </c>
+      <c r="C173" s="3">
+        <v>43518</v>
+      </c>
+      <c r="D173" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E173" s="5" t="s">
+        <v>855</v>
+      </c>
       <c r="F173" s="5"/>
-      <c r="G173" s="5"/>
+      <c r="G173" s="5" t="s">
+        <v>873</v>
+      </c>
       <c r="H173" s="5"/>
       <c r="I173" s="5"/>
       <c r="J173" s="5"/>
-      <c r="K173" s="5"/>
-      <c r="L173" s="5"/>
+      <c r="K173" s="5">
+        <v>1</v>
+      </c>
+      <c r="L173" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M173" s="5"/>
     </row>
     <row r="174" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B174" s="2"/>
-      <c r="C174" s="3"/>
-      <c r="D174" s="5"/>
-      <c r="E174" s="5"/>
+      <c r="B174" s="2">
+        <v>170</v>
+      </c>
+      <c r="C174" s="3">
+        <v>43518</v>
+      </c>
+      <c r="D174" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E174" s="5" t="s">
+        <v>856</v>
+      </c>
       <c r="F174" s="5"/>
-      <c r="G174" s="5"/>
+      <c r="G174" s="5" t="s">
+        <v>874</v>
+      </c>
       <c r="H174" s="5"/>
       <c r="I174" s="5"/>
       <c r="J174" s="5"/>
-      <c r="K174" s="5"/>
-      <c r="L174" s="5"/>
+      <c r="K174" s="5">
+        <v>1</v>
+      </c>
+      <c r="L174" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M174" s="5"/>
     </row>
     <row r="175" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B175" s="2"/>
-      <c r="C175" s="3"/>
-      <c r="D175" s="5"/>
-      <c r="E175" s="5"/>
+      <c r="B175" s="2">
+        <v>171</v>
+      </c>
+      <c r="C175" s="3">
+        <v>43518</v>
+      </c>
+      <c r="D175" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E175" s="5" t="s">
+        <v>857</v>
+      </c>
       <c r="F175" s="5"/>
-      <c r="G175" s="5"/>
+      <c r="G175" s="5" t="s">
+        <v>875</v>
+      </c>
       <c r="H175" s="5"/>
       <c r="I175" s="5"/>
       <c r="J175" s="5"/>
-      <c r="K175" s="5"/>
-      <c r="L175" s="5"/>
+      <c r="K175" s="5">
+        <v>1</v>
+      </c>
+      <c r="L175" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M175" s="5"/>
     </row>
     <row r="176" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B176" s="2"/>
-      <c r="C176" s="3"/>
-      <c r="D176" s="5"/>
-      <c r="E176" s="5"/>
+      <c r="B176" s="2">
+        <v>172</v>
+      </c>
+      <c r="C176" s="3">
+        <v>43521</v>
+      </c>
+      <c r="D176" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E176" s="5" t="s">
+        <v>884</v>
+      </c>
       <c r="F176" s="5"/>
-      <c r="G176" s="5"/>
+      <c r="G176" s="5" t="s">
+        <v>897</v>
+      </c>
       <c r="H176" s="5"/>
       <c r="I176" s="5"/>
       <c r="J176" s="5"/>
-      <c r="K176" s="5"/>
-      <c r="L176" s="5"/>
+      <c r="K176" s="5">
+        <v>1</v>
+      </c>
+      <c r="L176" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M176" s="5"/>
     </row>
     <row r="177" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B177" s="2"/>
-      <c r="C177" s="3"/>
-      <c r="D177" s="5"/>
-      <c r="E177" s="5"/>
+      <c r="B177" s="2">
+        <v>173</v>
+      </c>
+      <c r="C177" s="3">
+        <v>43521</v>
+      </c>
+      <c r="D177" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E177" s="5" t="s">
+        <v>885</v>
+      </c>
       <c r="F177" s="5"/>
-      <c r="G177" s="5"/>
+      <c r="G177" s="5" t="s">
+        <v>898</v>
+      </c>
       <c r="H177" s="5"/>
       <c r="I177" s="5"/>
       <c r="J177" s="5"/>
-      <c r="K177" s="5"/>
-      <c r="L177" s="5"/>
+      <c r="K177" s="5">
+        <v>1</v>
+      </c>
+      <c r="L177" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M177" s="5"/>
     </row>
     <row r="178" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B178" s="2"/>
-      <c r="C178" s="3"/>
-      <c r="D178" s="5"/>
-      <c r="E178" s="5"/>
+      <c r="B178" s="2">
+        <v>174</v>
+      </c>
+      <c r="C178" s="3">
+        <v>43521</v>
+      </c>
+      <c r="D178" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E178" s="5" t="s">
+        <v>886</v>
+      </c>
       <c r="F178" s="5"/>
-      <c r="G178" s="5"/>
+      <c r="G178" s="5" t="s">
+        <v>899</v>
+      </c>
       <c r="H178" s="5"/>
       <c r="I178" s="5"/>
       <c r="J178" s="5"/>
-      <c r="K178" s="5"/>
-      <c r="L178" s="5"/>
+      <c r="K178" s="5">
+        <v>1</v>
+      </c>
+      <c r="L178" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M178" s="5"/>
     </row>
     <row r="179" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B179" s="2"/>
-      <c r="C179" s="3"/>
-      <c r="D179" s="5"/>
-      <c r="E179" s="5"/>
+      <c r="B179" s="2">
+        <v>175</v>
+      </c>
+      <c r="C179" s="3">
+        <v>43521</v>
+      </c>
+      <c r="D179" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E179" s="5" t="s">
+        <v>887</v>
+      </c>
       <c r="F179" s="5"/>
-      <c r="G179" s="5"/>
+      <c r="G179" s="5" t="s">
+        <v>900</v>
+      </c>
       <c r="H179" s="5"/>
       <c r="I179" s="5"/>
       <c r="J179" s="5"/>
-      <c r="K179" s="5"/>
-      <c r="L179" s="5"/>
+      <c r="K179" s="5">
+        <v>1</v>
+      </c>
+      <c r="L179" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M179" s="5"/>
     </row>
     <row r="180" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B180" s="2"/>
-      <c r="C180" s="3"/>
-      <c r="D180" s="5"/>
-      <c r="E180" s="5"/>
+      <c r="B180" s="2">
+        <v>176</v>
+      </c>
+      <c r="C180" s="3">
+        <v>43521</v>
+      </c>
+      <c r="D180" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E180" s="5" t="s">
+        <v>888</v>
+      </c>
       <c r="F180" s="5"/>
-      <c r="G180" s="5"/>
+      <c r="G180" s="5" t="s">
+        <v>901</v>
+      </c>
       <c r="H180" s="5"/>
       <c r="I180" s="5"/>
       <c r="J180" s="5"/>
-      <c r="K180" s="5"/>
-      <c r="L180" s="5"/>
+      <c r="K180" s="5">
+        <v>1</v>
+      </c>
+      <c r="L180" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M180" s="5"/>
     </row>
     <row r="181" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B181" s="2"/>
-      <c r="C181" s="3"/>
-      <c r="D181" s="5"/>
-      <c r="E181" s="5"/>
+      <c r="B181" s="2">
+        <v>177</v>
+      </c>
+      <c r="C181" s="3">
+        <v>43521</v>
+      </c>
+      <c r="D181" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E181" s="5" t="s">
+        <v>889</v>
+      </c>
       <c r="F181" s="5"/>
-      <c r="G181" s="5"/>
+      <c r="G181" s="5" t="s">
+        <v>902</v>
+      </c>
       <c r="H181" s="5"/>
       <c r="I181" s="5"/>
       <c r="J181" s="5"/>
-      <c r="K181" s="5"/>
-      <c r="L181" s="5"/>
+      <c r="K181" s="5">
+        <v>1</v>
+      </c>
+      <c r="L181" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M181" s="5"/>
     </row>
     <row r="182" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B182" s="2"/>
-      <c r="C182" s="3"/>
-      <c r="D182" s="5"/>
-      <c r="E182" s="5"/>
+      <c r="B182" s="2">
+        <v>178</v>
+      </c>
+      <c r="C182" s="3">
+        <v>43521</v>
+      </c>
+      <c r="D182" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E182" s="5" t="s">
+        <v>890</v>
+      </c>
       <c r="F182" s="5"/>
-      <c r="G182" s="5"/>
+      <c r="G182" s="5" t="s">
+        <v>903</v>
+      </c>
       <c r="H182" s="5"/>
       <c r="I182" s="5"/>
       <c r="J182" s="5"/>
-      <c r="K182" s="5"/>
-      <c r="L182" s="5"/>
+      <c r="K182" s="5">
+        <v>1</v>
+      </c>
+      <c r="L182" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M182" s="5"/>
     </row>
     <row r="183" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B183" s="2"/>
-      <c r="C183" s="3"/>
-      <c r="D183" s="5"/>
-      <c r="E183" s="5"/>
+      <c r="B183" s="2">
+        <v>179</v>
+      </c>
+      <c r="C183" s="3">
+        <v>43521</v>
+      </c>
+      <c r="D183" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E183" s="5" t="s">
+        <v>891</v>
+      </c>
       <c r="F183" s="5"/>
-      <c r="G183" s="5"/>
+      <c r="G183" s="5" t="s">
+        <v>904</v>
+      </c>
       <c r="H183" s="5"/>
       <c r="I183" s="5"/>
       <c r="J183" s="5"/>
-      <c r="K183" s="5"/>
-      <c r="L183" s="5"/>
+      <c r="K183" s="5">
+        <v>1</v>
+      </c>
+      <c r="L183" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M183" s="5"/>
     </row>
     <row r="184" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B184" s="2"/>
-      <c r="C184" s="3"/>
-      <c r="D184" s="5"/>
-      <c r="E184" s="5"/>
+      <c r="B184" s="2">
+        <v>180</v>
+      </c>
+      <c r="C184" s="3">
+        <v>43521</v>
+      </c>
+      <c r="D184" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E184" s="5" t="s">
+        <v>892</v>
+      </c>
       <c r="F184" s="5"/>
-      <c r="G184" s="5"/>
+      <c r="G184" s="5" t="s">
+        <v>905</v>
+      </c>
       <c r="H184" s="5"/>
       <c r="I184" s="5"/>
       <c r="J184" s="5"/>
-      <c r="K184" s="5"/>
-      <c r="L184" s="5"/>
+      <c r="K184" s="5">
+        <v>1</v>
+      </c>
+      <c r="L184" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M184" s="5"/>
     </row>
     <row r="185" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B185" s="2"/>
-      <c r="C185" s="3"/>
-      <c r="D185" s="5"/>
-      <c r="E185" s="5"/>
+      <c r="B185" s="2">
+        <v>181</v>
+      </c>
+      <c r="C185" s="3">
+        <v>43521</v>
+      </c>
+      <c r="D185" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E185" s="5" t="s">
+        <v>893</v>
+      </c>
       <c r="F185" s="5"/>
-      <c r="G185" s="5"/>
+      <c r="G185" s="5" t="s">
+        <v>906</v>
+      </c>
       <c r="H185" s="5"/>
       <c r="I185" s="5"/>
       <c r="J185" s="5"/>
-      <c r="K185" s="5"/>
-      <c r="L185" s="5"/>
+      <c r="K185" s="5">
+        <v>1</v>
+      </c>
+      <c r="L185" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M185" s="5"/>
     </row>
     <row r="186" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B186" s="2"/>
-      <c r="C186" s="3"/>
-      <c r="D186" s="5"/>
-      <c r="E186" s="5"/>
+      <c r="B186" s="2">
+        <v>182</v>
+      </c>
+      <c r="C186" s="3">
+        <v>43521</v>
+      </c>
+      <c r="D186" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E186" s="5" t="s">
+        <v>894</v>
+      </c>
       <c r="F186" s="5"/>
-      <c r="G186" s="5"/>
+      <c r="G186" s="5" t="s">
+        <v>907</v>
+      </c>
       <c r="H186" s="5"/>
       <c r="I186" s="5"/>
       <c r="J186" s="5"/>
-      <c r="K186" s="5"/>
-      <c r="L186" s="5"/>
+      <c r="K186" s="5">
+        <v>1</v>
+      </c>
+      <c r="L186" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M186" s="5"/>
     </row>
     <row r="187" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B187" s="2"/>
-      <c r="C187" s="3"/>
-      <c r="D187" s="5"/>
-      <c r="E187" s="5"/>
+      <c r="B187" s="2">
+        <v>183</v>
+      </c>
+      <c r="C187" s="3">
+        <v>43521</v>
+      </c>
+      <c r="D187" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E187" s="5" t="s">
+        <v>895</v>
+      </c>
       <c r="F187" s="5"/>
-      <c r="G187" s="5"/>
+      <c r="G187" s="5" t="s">
+        <v>908</v>
+      </c>
       <c r="H187" s="5"/>
       <c r="I187" s="5"/>
       <c r="J187" s="5"/>
-      <c r="K187" s="5"/>
-      <c r="L187" s="5"/>
+      <c r="K187" s="5">
+        <v>1</v>
+      </c>
+      <c r="L187" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M187" s="5"/>
     </row>
     <row r="188" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B188" s="2"/>
-      <c r="C188" s="3"/>
-      <c r="D188" s="5"/>
-      <c r="E188" s="5"/>
+      <c r="B188" s="2">
+        <v>184</v>
+      </c>
+      <c r="C188" s="3">
+        <v>43521</v>
+      </c>
+      <c r="D188" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E188" s="5" t="s">
+        <v>896</v>
+      </c>
       <c r="F188" s="5"/>
-      <c r="G188" s="5"/>
+      <c r="G188" s="5" t="s">
+        <v>909</v>
+      </c>
       <c r="H188" s="5"/>
       <c r="I188" s="5"/>
       <c r="J188" s="5"/>
-      <c r="K188" s="5"/>
-      <c r="L188" s="5"/>
+      <c r="K188" s="5">
+        <v>1</v>
+      </c>
+      <c r="L188" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M188" s="5"/>
     </row>
     <row r="189" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
@@ -8692,7 +9397,7 @@
       <c r="L250" s="5"/>
       <c r="M250" s="5"/>
     </row>
-    <row r="251" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="251" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B251" s="2"/>
       <c r="C251" s="3"/>
       <c r="D251" s="5"/>
@@ -8706,7 +9411,7 @@
       <c r="L251" s="5"/>
       <c r="M251" s="5"/>
     </row>
-    <row r="252" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="252" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B252" s="2"/>
       <c r="C252" s="3"/>
       <c r="D252" s="5"/>
@@ -12486,50 +13191,22 @@
       <c r="L521" s="5"/>
       <c r="M521" s="5"/>
     </row>
-    <row r="522" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B522" s="2"/>
-      <c r="C522" s="3"/>
-      <c r="D522" s="5"/>
-      <c r="E522" s="5"/>
-      <c r="F522" s="5"/>
-      <c r="G522" s="5"/>
-      <c r="H522" s="5"/>
-      <c r="I522" s="5"/>
-      <c r="J522" s="5"/>
-      <c r="K522" s="5"/>
-      <c r="L522" s="5"/>
-      <c r="M522" s="5"/>
-    </row>
-    <row r="523" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B523" s="2"/>
-      <c r="C523" s="3"/>
-      <c r="D523" s="5"/>
-      <c r="E523" s="5"/>
-      <c r="F523" s="5"/>
-      <c r="G523" s="5"/>
-      <c r="H523" s="5"/>
-      <c r="I523" s="5"/>
-      <c r="J523" s="5"/>
-      <c r="K523" s="5"/>
-      <c r="L523" s="5"/>
-      <c r="M523" s="5"/>
-    </row>
   </sheetData>
-  <autoFilter ref="B4:M104"/>
+  <autoFilter ref="B4:M175"/>
   <mergeCells count="1">
     <mergeCell ref="B2:L2"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D115 D154:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D115 D189:D1048576">
       <formula1>"Likeshuo,TOEFL,TPO"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D116:D153">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D116:D188">
       <formula1>"Likeshuo,TOEFL,TPO, 500 setns"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L5:L523">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L5:L521">
       <formula1>"Input, Renew, Understood, Reviewed, Forgot"</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C523">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C521">
       <formula1>43508</formula1>
     </dataValidation>
   </dataValidations>
@@ -12545,7 +13222,7 @@
   </sheetPr>
   <dimension ref="B1:M410"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F95" sqref="F95"/>
     </sheetView>

</xml_diff>

<commit_message>
updated english vocabulary for TOEFL
</commit_message>
<xml_diff>
--- a/english_learning/Vocabulary Statistic Chart for TOEFL.xlsx
+++ b/english_learning/Vocabulary Statistic Chart for TOEFL.xlsx
@@ -16,7 +16,7 @@
     <sheet name="TOEFL" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">main!$B$4:$M$175</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">main!$B$4:$M$190</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">TOEFL!$B$4:$M$4</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1866" uniqueCount="910">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2083" uniqueCount="1020">
   <si>
     <t>Expression</t>
   </si>
@@ -2564,9 +2564,6 @@
     <t>intramural</t>
   </si>
   <si>
-    <t>confinement</t>
-  </si>
-  <si>
     <t>partake</t>
   </si>
   <si>
@@ -2618,9 +2615,6 @@
     <t>友情</t>
   </si>
   <si>
-    <t>坐月子</t>
-  </si>
-  <si>
     <t>参加</t>
   </si>
   <si>
@@ -2760,6 +2754,342 @@
   </si>
   <si>
     <t>现金周转</t>
+  </si>
+  <si>
+    <t>keep or restrict someone or something within certain limits</t>
+  </si>
+  <si>
+    <t>obscure one's meaning</t>
+  </si>
+  <si>
+    <t>flowery but vague expressions</t>
+  </si>
+  <si>
+    <t>warmer, less severe interiors</t>
+  </si>
+  <si>
+    <t>libel is printed</t>
+  </si>
+  <si>
+    <t>slander is spoken</t>
+  </si>
+  <si>
+    <t>thigh bone</t>
+  </si>
+  <si>
+    <t>a corrosive action on metals</t>
+  </si>
+  <si>
+    <t>certain blue vegetable dyes</t>
+  </si>
+  <si>
+    <t>rest on</t>
+  </si>
+  <si>
+    <t>花哨但模糊的表达</t>
+  </si>
+  <si>
+    <t>obscure:模糊v</t>
+  </si>
+  <si>
+    <t>温暖且不严肃的内饰</t>
+  </si>
+  <si>
+    <t>诋毁是书面的</t>
+  </si>
+  <si>
+    <t>诽谤是口头的</t>
+  </si>
+  <si>
+    <t>大腿骨</t>
+  </si>
+  <si>
+    <t>对金属有腐蚀作用</t>
+  </si>
+  <si>
+    <t>特定蓝色蔬菜染料</t>
+  </si>
+  <si>
+    <t>corrosive action</t>
+  </si>
+  <si>
+    <t>倚重于, 依赖于</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> give emotional depth to …</t>
+  </si>
+  <si>
+    <t>倾注深度情感于…</t>
+  </si>
+  <si>
+    <t>Richard the Lionheart</t>
+  </si>
+  <si>
+    <t>Crusader King</t>
+  </si>
+  <si>
+    <t>colloquial</t>
+  </si>
+  <si>
+    <t>slang</t>
+  </si>
+  <si>
+    <t>monarchy</t>
+  </si>
+  <si>
+    <t>crusade</t>
+  </si>
+  <si>
+    <t>medieval military expedition</t>
+  </si>
+  <si>
+    <t>vanquish</t>
+  </si>
+  <si>
+    <t>defeat</t>
+  </si>
+  <si>
+    <t>pious</t>
+  </si>
+  <si>
+    <t>devoutly religious</t>
+  </si>
+  <si>
+    <t>iconic</t>
+  </si>
+  <si>
+    <t>statue</t>
+  </si>
+  <si>
+    <t>carved or cast figure of a person or animal</t>
+  </si>
+  <si>
+    <t>pope</t>
+  </si>
+  <si>
+    <t>the Houses of Parliament</t>
+  </si>
+  <si>
+    <t>he was reputed to be a great military leader.</t>
+  </si>
+  <si>
+    <t>take command of his own army</t>
+  </si>
+  <si>
+    <t>score considerable victories against his Muslim counterpart, Saladin.</t>
+  </si>
+  <si>
+    <t>Following his accession, ...</t>
+  </si>
+  <si>
+    <t>by his subjects.</t>
+  </si>
+  <si>
+    <t>You're avin a larf!</t>
+  </si>
+  <si>
+    <t>Nice one Cyril.</t>
+  </si>
+  <si>
+    <t>I'm so chuffed.</t>
+  </si>
+  <si>
+    <t>I'm knackered.</t>
+  </si>
+  <si>
+    <t>Fancy a cuppa?</t>
+  </si>
+  <si>
+    <t>I'm gagging for a pint.</t>
+  </si>
+  <si>
+    <t>How come?</t>
+  </si>
+  <si>
+    <t>Surely, you are not serious?</t>
+  </si>
+  <si>
+    <t>That's great!</t>
+  </si>
+  <si>
+    <t>I'm so happy for you.</t>
+  </si>
+  <si>
+    <t>I'm really tired.</t>
+  </si>
+  <si>
+    <t>Would you like a cup of tea?</t>
+  </si>
+  <si>
+    <t>I would love a drink of beer.</t>
+  </si>
+  <si>
+    <t>Why?</t>
+  </si>
+  <si>
+    <t>How come you're late again?</t>
+  </si>
+  <si>
+    <t>I'm bursting.</t>
+  </si>
+  <si>
+    <t>I'm stuffed.</t>
+  </si>
+  <si>
+    <t>I'm wrecked.</t>
+  </si>
+  <si>
+    <t>I'm pissed off.</t>
+  </si>
+  <si>
+    <t>狮心王理查德</t>
+  </si>
+  <si>
+    <t>十字军国王</t>
+  </si>
+  <si>
+    <t>口语</t>
+  </si>
+  <si>
+    <t>俚语</t>
+  </si>
+  <si>
+    <t>帝制</t>
+  </si>
+  <si>
+    <t>运动</t>
+  </si>
+  <si>
+    <t>中世纪军事探险</t>
+  </si>
+  <si>
+    <t>征服</t>
+  </si>
+  <si>
+    <t>打败</t>
+  </si>
+  <si>
+    <t>虔诚的宗教</t>
+  </si>
+  <si>
+    <t>标志性的</t>
+  </si>
+  <si>
+    <t>雕像</t>
+  </si>
+  <si>
+    <t>雕刻或铸造人或动物的身影</t>
+  </si>
+  <si>
+    <t>教皇</t>
+  </si>
+  <si>
+    <t>国会大厦</t>
+  </si>
+  <si>
+    <t>他被誉为伟大的军事领袖。</t>
+  </si>
+  <si>
+    <t>掌握自己的军队</t>
+  </si>
+  <si>
+    <t>与穆斯林对手萨拉丁取得了相当大的胜利。</t>
+  </si>
+  <si>
+    <t>accession</t>
+  </si>
+  <si>
+    <t>随他登基之后…</t>
+  </si>
+  <si>
+    <t>由他的臣民们</t>
+  </si>
+  <si>
+    <t>I need to go to the toilet very soon.</t>
+  </si>
+  <si>
+    <t>I can't eat anymore.</t>
+  </si>
+  <si>
+    <t>I'm extremely tired.</t>
+  </si>
+  <si>
+    <t>I'm angery about something.</t>
+  </si>
+  <si>
+    <t>虔诚</t>
+  </si>
+  <si>
+    <t>flapper</t>
+  </si>
+  <si>
+    <t>rebellious</t>
+  </si>
+  <si>
+    <t>a woman with bob haircut</t>
+  </si>
+  <si>
+    <t>speakeasy</t>
+  </si>
+  <si>
+    <t>diaphragm</t>
+  </si>
+  <si>
+    <t>home appliances</t>
+  </si>
+  <si>
+    <t>insulin</t>
+  </si>
+  <si>
+    <t>mashed potato</t>
+  </si>
+  <si>
+    <t>悖</t>
+  </si>
+  <si>
+    <t>一个女人与鲍勃发型</t>
+  </si>
+  <si>
+    <t>非法经营</t>
+  </si>
+  <si>
+    <t>家用电器</t>
+  </si>
+  <si>
+    <t>胰岛素</t>
+  </si>
+  <si>
+    <t>青霉素</t>
+  </si>
+  <si>
+    <t>土豆泥</t>
+  </si>
+  <si>
+    <t>避孕隔膜</t>
+  </si>
+  <si>
+    <t>膈膜</t>
+  </si>
+  <si>
+    <t>in the 1920s, a fashionable young woman, especially one showing independent behaviour</t>
+  </si>
+  <si>
+    <t>penicillin</t>
+  </si>
+  <si>
+    <t>scenery</t>
+  </si>
+  <si>
+    <t>sceneries</t>
+  </si>
+  <si>
+    <t>blurry</t>
+  </si>
+  <si>
+    <t>风景</t>
+  </si>
+  <si>
+    <t>模糊</t>
   </si>
 </sst>
 </file>
@@ -3212,11 +3542,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:M521"/>
+  <dimension ref="B1:M520"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A174" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J183" sqref="J183"/>
+      <pane ySplit="4" topLeftCell="A232" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G234" sqref="G234"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
@@ -7562,7 +7892,7 @@
       </c>
       <c r="F154" s="5"/>
       <c r="G154" s="5" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="H154" s="5"/>
       <c r="I154" s="5"/>
@@ -7590,7 +7920,7 @@
       </c>
       <c r="F155" s="5"/>
       <c r="G155" s="5" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="H155" s="5"/>
       <c r="I155" s="5"/>
@@ -7618,7 +7948,7 @@
       </c>
       <c r="F156" s="5"/>
       <c r="G156" s="5" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="H156" s="5"/>
       <c r="I156" s="5"/>
@@ -7646,7 +7976,7 @@
       </c>
       <c r="F157" s="5"/>
       <c r="G157" s="5" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="H157" s="5"/>
       <c r="I157" s="5"/>
@@ -7674,7 +8004,7 @@
       </c>
       <c r="F158" s="5"/>
       <c r="G158" s="5" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="H158" s="5"/>
       <c r="I158" s="5"/>
@@ -7698,11 +8028,11 @@
         <v>213</v>
       </c>
       <c r="E159" s="5" t="s">
-        <v>844</v>
+        <v>834</v>
       </c>
       <c r="F159" s="5"/>
       <c r="G159" s="5" t="s">
-        <v>862</v>
+        <v>908</v>
       </c>
       <c r="H159" s="5"/>
       <c r="I159" s="5"/>
@@ -7726,11 +8056,11 @@
         <v>213</v>
       </c>
       <c r="E160" s="5" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="F160" s="5"/>
       <c r="G160" s="5" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="H160" s="5"/>
       <c r="I160" s="5"/>
@@ -7754,11 +8084,11 @@
         <v>213</v>
       </c>
       <c r="E161" s="5" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="F161" s="5"/>
       <c r="G161" s="5" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
       <c r="H161" s="5"/>
       <c r="I161" s="5"/>
@@ -7782,11 +8112,11 @@
         <v>213</v>
       </c>
       <c r="E162" s="5" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="F162" s="5"/>
       <c r="G162" s="5" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="H162" s="5"/>
       <c r="I162" s="5"/>
@@ -7810,11 +8140,11 @@
         <v>213</v>
       </c>
       <c r="E163" s="5" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="F163" s="5"/>
       <c r="G163" s="5" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
       <c r="H163" s="5"/>
       <c r="I163" s="5"/>
@@ -7838,11 +8168,11 @@
         <v>213</v>
       </c>
       <c r="E164" s="5" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="F164" s="5"/>
       <c r="G164" s="5" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="H164" s="5"/>
       <c r="I164" s="5"/>
@@ -7866,11 +8196,11 @@
         <v>213</v>
       </c>
       <c r="E165" s="5" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="F165" s="5"/>
       <c r="G165" s="5" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="H165" s="5"/>
       <c r="I165" s="5"/>
@@ -7894,11 +8224,11 @@
         <v>213</v>
       </c>
       <c r="E166" s="5" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="F166" s="5"/>
       <c r="G166" s="5" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="H166" s="5"/>
       <c r="I166" s="5"/>
@@ -7922,11 +8252,11 @@
         <v>213</v>
       </c>
       <c r="E167" s="5" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="F167" s="5"/>
       <c r="G167" s="5" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="H167" s="5"/>
       <c r="I167" s="5"/>
@@ -7950,11 +8280,11 @@
         <v>213</v>
       </c>
       <c r="E168" s="5" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="F168" s="5"/>
       <c r="G168" s="5" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="H168" s="5"/>
       <c r="I168" s="5"/>
@@ -7978,11 +8308,11 @@
         <v>213</v>
       </c>
       <c r="E169" s="5" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="F169" s="5"/>
       <c r="G169" s="5" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="H169" s="5"/>
       <c r="I169" s="5"/>
@@ -8006,14 +8336,14 @@
         <v>213</v>
       </c>
       <c r="E170" s="5" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="F170" s="5"/>
       <c r="G170" s="5" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
       <c r="H170" s="5" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="I170" s="5"/>
       <c r="J170" s="5"/>
@@ -8036,11 +8366,11 @@
         <v>213</v>
       </c>
       <c r="E171" s="5" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="F171" s="5"/>
       <c r="G171" s="5" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="H171" s="5"/>
       <c r="I171" s="5"/>
@@ -8064,11 +8394,11 @@
         <v>213</v>
       </c>
       <c r="E172" s="5" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="F172" s="5"/>
       <c r="G172" s="5" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="H172" s="5"/>
       <c r="I172" s="5"/>
@@ -8092,11 +8422,11 @@
         <v>213</v>
       </c>
       <c r="E173" s="5" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="F173" s="5"/>
       <c r="G173" s="5" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="H173" s="5"/>
       <c r="I173" s="5"/>
@@ -8120,11 +8450,11 @@
         <v>213</v>
       </c>
       <c r="E174" s="5" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="F174" s="5"/>
       <c r="G174" s="5" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="H174" s="5"/>
       <c r="I174" s="5"/>
@@ -8148,11 +8478,11 @@
         <v>213</v>
       </c>
       <c r="E175" s="5" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="F175" s="5"/>
       <c r="G175" s="5" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="H175" s="5"/>
       <c r="I175" s="5"/>
@@ -8176,11 +8506,11 @@
         <v>213</v>
       </c>
       <c r="E176" s="5" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="F176" s="5"/>
       <c r="G176" s="5" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="H176" s="5"/>
       <c r="I176" s="5"/>
@@ -8204,11 +8534,11 @@
         <v>213</v>
       </c>
       <c r="E177" s="5" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="F177" s="5"/>
       <c r="G177" s="5" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="H177" s="5"/>
       <c r="I177" s="5"/>
@@ -8232,11 +8562,11 @@
         <v>213</v>
       </c>
       <c r="E178" s="5" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="F178" s="5"/>
       <c r="G178" s="5" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="H178" s="5"/>
       <c r="I178" s="5"/>
@@ -8260,11 +8590,11 @@
         <v>213</v>
       </c>
       <c r="E179" s="5" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="F179" s="5"/>
       <c r="G179" s="5" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="H179" s="5"/>
       <c r="I179" s="5"/>
@@ -8288,11 +8618,11 @@
         <v>213</v>
       </c>
       <c r="E180" s="5" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="F180" s="5"/>
       <c r="G180" s="5" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="H180" s="5"/>
       <c r="I180" s="5"/>
@@ -8316,11 +8646,11 @@
         <v>213</v>
       </c>
       <c r="E181" s="5" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="F181" s="5"/>
       <c r="G181" s="5" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="H181" s="5"/>
       <c r="I181" s="5"/>
@@ -8344,11 +8674,11 @@
         <v>213</v>
       </c>
       <c r="E182" s="5" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="F182" s="5"/>
       <c r="G182" s="5" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="H182" s="5"/>
       <c r="I182" s="5"/>
@@ -8372,11 +8702,11 @@
         <v>213</v>
       </c>
       <c r="E183" s="5" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="F183" s="5"/>
       <c r="G183" s="5" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="H183" s="5"/>
       <c r="I183" s="5"/>
@@ -8400,11 +8730,11 @@
         <v>213</v>
       </c>
       <c r="E184" s="5" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="F184" s="5"/>
       <c r="G184" s="5" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="H184" s="5"/>
       <c r="I184" s="5"/>
@@ -8428,11 +8758,11 @@
         <v>213</v>
       </c>
       <c r="E185" s="5" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="F185" s="5"/>
       <c r="G185" s="5" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="H185" s="5"/>
       <c r="I185" s="5"/>
@@ -8456,11 +8786,11 @@
         <v>213</v>
       </c>
       <c r="E186" s="5" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="F186" s="5"/>
       <c r="G186" s="5" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="H186" s="5"/>
       <c r="I186" s="5"/>
@@ -8484,11 +8814,11 @@
         <v>213</v>
       </c>
       <c r="E187" s="5" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="F187" s="5"/>
       <c r="G187" s="5" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="H187" s="5"/>
       <c r="I187" s="5"/>
@@ -8512,11 +8842,11 @@
         <v>213</v>
       </c>
       <c r="E188" s="5" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="F188" s="5"/>
       <c r="G188" s="5" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="H188" s="5"/>
       <c r="I188" s="5"/>
@@ -8530,745 +8860,1497 @@
       <c r="M188" s="5"/>
     </row>
     <row r="189" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B189" s="2"/>
-      <c r="C189" s="3"/>
-      <c r="D189" s="5"/>
-      <c r="E189" s="5"/>
+      <c r="B189" s="2">
+        <v>185</v>
+      </c>
+      <c r="C189" s="3">
+        <v>43522</v>
+      </c>
+      <c r="D189" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="E189" s="5" t="s">
+        <v>910</v>
+      </c>
       <c r="F189" s="5"/>
-      <c r="G189" s="5"/>
+      <c r="G189" s="5" t="s">
+        <v>918</v>
+      </c>
       <c r="H189" s="5"/>
       <c r="I189" s="5"/>
       <c r="J189" s="5"/>
-      <c r="K189" s="5"/>
-      <c r="L189" s="5"/>
+      <c r="K189" s="5">
+        <v>1</v>
+      </c>
+      <c r="L189" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M189" s="5"/>
     </row>
     <row r="190" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B190" s="2"/>
-      <c r="C190" s="3"/>
-      <c r="D190" s="5"/>
-      <c r="E190" s="5"/>
+      <c r="B190" s="2">
+        <v>186</v>
+      </c>
+      <c r="C190" s="3">
+        <v>43522</v>
+      </c>
+      <c r="D190" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="E190" s="5" t="s">
+        <v>909</v>
+      </c>
       <c r="F190" s="5"/>
-      <c r="G190" s="5"/>
+      <c r="G190" s="5" t="s">
+        <v>919</v>
+      </c>
       <c r="H190" s="5"/>
       <c r="I190" s="5"/>
       <c r="J190" s="5"/>
-      <c r="K190" s="5"/>
-      <c r="L190" s="5"/>
+      <c r="K190" s="5">
+        <v>1</v>
+      </c>
+      <c r="L190" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M190" s="5"/>
     </row>
     <row r="191" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B191" s="2"/>
-      <c r="C191" s="3"/>
-      <c r="D191" s="5"/>
-      <c r="E191" s="5"/>
+      <c r="B191" s="2">
+        <v>187</v>
+      </c>
+      <c r="C191" s="3">
+        <v>43522</v>
+      </c>
+      <c r="D191" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="E191" s="5" t="s">
+        <v>911</v>
+      </c>
       <c r="F191" s="5"/>
-      <c r="G191" s="5"/>
+      <c r="G191" s="5" t="s">
+        <v>920</v>
+      </c>
       <c r="H191" s="5"/>
       <c r="I191" s="5"/>
       <c r="J191" s="5"/>
-      <c r="K191" s="5"/>
-      <c r="L191" s="5"/>
+      <c r="K191" s="5">
+        <v>1</v>
+      </c>
+      <c r="L191" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M191" s="5"/>
     </row>
     <row r="192" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B192" s="2"/>
-      <c r="C192" s="3"/>
-      <c r="D192" s="5"/>
-      <c r="E192" s="5"/>
+      <c r="B192" s="2">
+        <v>188</v>
+      </c>
+      <c r="C192" s="3">
+        <v>43522</v>
+      </c>
+      <c r="D192" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="E192" s="5" t="s">
+        <v>912</v>
+      </c>
       <c r="F192" s="5"/>
-      <c r="G192" s="5"/>
+      <c r="G192" s="5" t="s">
+        <v>921</v>
+      </c>
       <c r="H192" s="5"/>
       <c r="I192" s="5"/>
       <c r="J192" s="5"/>
-      <c r="K192" s="5"/>
-      <c r="L192" s="5"/>
+      <c r="K192" s="5">
+        <v>1</v>
+      </c>
+      <c r="L192" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M192" s="5"/>
     </row>
     <row r="193" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B193" s="2"/>
-      <c r="C193" s="3"/>
-      <c r="D193" s="5"/>
-      <c r="E193" s="5"/>
+      <c r="B193" s="2">
+        <v>189</v>
+      </c>
+      <c r="C193" s="3">
+        <v>43522</v>
+      </c>
+      <c r="D193" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="E193" s="5" t="s">
+        <v>913</v>
+      </c>
       <c r="F193" s="5"/>
-      <c r="G193" s="5"/>
+      <c r="G193" s="5" t="s">
+        <v>922</v>
+      </c>
       <c r="H193" s="5"/>
       <c r="I193" s="5"/>
       <c r="J193" s="5"/>
-      <c r="K193" s="5"/>
-      <c r="L193" s="5"/>
+      <c r="K193" s="5">
+        <v>1</v>
+      </c>
+      <c r="L193" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M193" s="5"/>
     </row>
     <row r="194" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B194" s="2"/>
-      <c r="C194" s="3"/>
-      <c r="D194" s="5"/>
-      <c r="E194" s="5"/>
+      <c r="B194" s="2">
+        <v>190</v>
+      </c>
+      <c r="C194" s="3">
+        <v>43522</v>
+      </c>
+      <c r="D194" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="E194" s="5" t="s">
+        <v>914</v>
+      </c>
       <c r="F194" s="5"/>
-      <c r="G194" s="5"/>
+      <c r="G194" s="5" t="s">
+        <v>923</v>
+      </c>
       <c r="H194" s="5"/>
       <c r="I194" s="5"/>
       <c r="J194" s="5"/>
-      <c r="K194" s="5"/>
-      <c r="L194" s="5"/>
+      <c r="K194" s="5">
+        <v>1</v>
+      </c>
+      <c r="L194" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M194" s="5"/>
     </row>
     <row r="195" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B195" s="2"/>
-      <c r="C195" s="3"/>
-      <c r="D195" s="5"/>
-      <c r="E195" s="5"/>
+      <c r="B195" s="2">
+        <v>191</v>
+      </c>
+      <c r="C195" s="3">
+        <v>43522</v>
+      </c>
+      <c r="D195" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="E195" s="5" t="s">
+        <v>915</v>
+      </c>
       <c r="F195" s="5"/>
-      <c r="G195" s="5"/>
-      <c r="H195" s="5"/>
+      <c r="G195" s="5" t="s">
+        <v>924</v>
+      </c>
+      <c r="H195" s="5" t="s">
+        <v>926</v>
+      </c>
       <c r="I195" s="5"/>
       <c r="J195" s="5"/>
-      <c r="K195" s="5"/>
-      <c r="L195" s="5"/>
+      <c r="K195" s="5">
+        <v>1</v>
+      </c>
+      <c r="L195" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M195" s="5"/>
     </row>
     <row r="196" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B196" s="2"/>
-      <c r="C196" s="3"/>
-      <c r="D196" s="5"/>
-      <c r="E196" s="5"/>
+      <c r="B196" s="2">
+        <v>192</v>
+      </c>
+      <c r="C196" s="3">
+        <v>43522</v>
+      </c>
+      <c r="D196" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="E196" s="5" t="s">
+        <v>916</v>
+      </c>
       <c r="F196" s="5"/>
-      <c r="G196" s="5"/>
+      <c r="G196" s="5" t="s">
+        <v>925</v>
+      </c>
       <c r="H196" s="5"/>
       <c r="I196" s="5"/>
       <c r="J196" s="5"/>
-      <c r="K196" s="5"/>
-      <c r="L196" s="5"/>
+      <c r="K196" s="5">
+        <v>1</v>
+      </c>
+      <c r="L196" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M196" s="5"/>
     </row>
     <row r="197" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B197" s="2"/>
-      <c r="C197" s="3"/>
-      <c r="D197" s="5"/>
-      <c r="E197" s="5"/>
+      <c r="B197" s="2">
+        <v>193</v>
+      </c>
+      <c r="C197" s="3">
+        <v>43522</v>
+      </c>
+      <c r="D197" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="E197" s="5" t="s">
+        <v>917</v>
+      </c>
       <c r="F197" s="5"/>
-      <c r="G197" s="5"/>
+      <c r="G197" s="5" t="s">
+        <v>927</v>
+      </c>
       <c r="H197" s="5"/>
       <c r="I197" s="5"/>
       <c r="J197" s="5"/>
-      <c r="K197" s="5"/>
-      <c r="L197" s="5"/>
+      <c r="K197" s="5">
+        <v>1</v>
+      </c>
+      <c r="L197" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M197" s="5"/>
     </row>
     <row r="198" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B198" s="2"/>
-      <c r="C198" s="3"/>
-      <c r="D198" s="5"/>
-      <c r="E198" s="5"/>
+      <c r="B198" s="2">
+        <v>194</v>
+      </c>
+      <c r="C198" s="3">
+        <v>43522</v>
+      </c>
+      <c r="D198" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="E198" s="5" t="s">
+        <v>928</v>
+      </c>
       <c r="F198" s="5"/>
-      <c r="G198" s="5"/>
+      <c r="G198" s="5" t="s">
+        <v>929</v>
+      </c>
       <c r="H198" s="5"/>
       <c r="I198" s="5"/>
       <c r="J198" s="5"/>
-      <c r="K198" s="5"/>
-      <c r="L198" s="5"/>
+      <c r="K198" s="5">
+        <v>1</v>
+      </c>
+      <c r="L198" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M198" s="5"/>
     </row>
     <row r="199" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B199" s="2"/>
-      <c r="C199" s="3"/>
-      <c r="D199" s="5"/>
-      <c r="E199" s="5"/>
+      <c r="B199" s="2">
+        <v>195</v>
+      </c>
+      <c r="C199" s="3">
+        <v>43522</v>
+      </c>
+      <c r="D199" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E199" s="5" t="s">
+        <v>930</v>
+      </c>
       <c r="F199" s="5"/>
-      <c r="G199" s="5"/>
+      <c r="G199" s="5" t="s">
+        <v>970</v>
+      </c>
       <c r="H199" s="5"/>
       <c r="I199" s="5"/>
       <c r="J199" s="5"/>
-      <c r="K199" s="5"/>
-      <c r="L199" s="5"/>
+      <c r="K199" s="5">
+        <v>1</v>
+      </c>
+      <c r="L199" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M199" s="5"/>
     </row>
     <row r="200" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B200" s="2"/>
-      <c r="C200" s="3"/>
-      <c r="D200" s="5"/>
-      <c r="E200" s="5"/>
+      <c r="B200" s="2">
+        <v>196</v>
+      </c>
+      <c r="C200" s="3">
+        <v>43522</v>
+      </c>
+      <c r="D200" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E200" s="5" t="s">
+        <v>931</v>
+      </c>
       <c r="F200" s="5"/>
-      <c r="G200" s="5"/>
+      <c r="G200" s="5" t="s">
+        <v>971</v>
+      </c>
       <c r="H200" s="5"/>
       <c r="I200" s="5"/>
       <c r="J200" s="5"/>
-      <c r="K200" s="5"/>
-      <c r="L200" s="5"/>
+      <c r="K200" s="5">
+        <v>1</v>
+      </c>
+      <c r="L200" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M200" s="5"/>
     </row>
     <row r="201" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B201" s="2"/>
-      <c r="C201" s="3"/>
-      <c r="D201" s="5"/>
-      <c r="E201" s="5"/>
+      <c r="B201" s="2">
+        <v>197</v>
+      </c>
+      <c r="C201" s="3">
+        <v>43522</v>
+      </c>
+      <c r="D201" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E201" s="5" t="s">
+        <v>932</v>
+      </c>
       <c r="F201" s="5"/>
-      <c r="G201" s="5"/>
+      <c r="G201" s="5" t="s">
+        <v>972</v>
+      </c>
       <c r="H201" s="5"/>
       <c r="I201" s="5"/>
       <c r="J201" s="5"/>
-      <c r="K201" s="5"/>
-      <c r="L201" s="5"/>
+      <c r="K201" s="5">
+        <v>1</v>
+      </c>
+      <c r="L201" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M201" s="5"/>
     </row>
     <row r="202" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B202" s="2"/>
-      <c r="C202" s="3"/>
-      <c r="D202" s="5"/>
-      <c r="E202" s="5"/>
+      <c r="B202" s="2">
+        <v>198</v>
+      </c>
+      <c r="C202" s="3">
+        <v>43522</v>
+      </c>
+      <c r="D202" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E202" s="5" t="s">
+        <v>933</v>
+      </c>
       <c r="F202" s="5"/>
-      <c r="G202" s="5"/>
+      <c r="G202" s="5" t="s">
+        <v>973</v>
+      </c>
       <c r="H202" s="5"/>
       <c r="I202" s="5"/>
       <c r="J202" s="5"/>
-      <c r="K202" s="5"/>
-      <c r="L202" s="5"/>
+      <c r="K202" s="5">
+        <v>1</v>
+      </c>
+      <c r="L202" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M202" s="5"/>
     </row>
     <row r="203" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B203" s="2"/>
-      <c r="C203" s="3"/>
-      <c r="D203" s="5"/>
-      <c r="E203" s="5"/>
+      <c r="B203" s="2">
+        <v>199</v>
+      </c>
+      <c r="C203" s="3">
+        <v>43522</v>
+      </c>
+      <c r="D203" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E203" s="5" t="s">
+        <v>934</v>
+      </c>
       <c r="F203" s="5"/>
-      <c r="G203" s="5"/>
+      <c r="G203" s="5" t="s">
+        <v>974</v>
+      </c>
       <c r="H203" s="5"/>
       <c r="I203" s="5"/>
       <c r="J203" s="5"/>
-      <c r="K203" s="5"/>
-      <c r="L203" s="5"/>
+      <c r="K203" s="5">
+        <v>1</v>
+      </c>
+      <c r="L203" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M203" s="5"/>
     </row>
     <row r="204" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B204" s="2"/>
-      <c r="C204" s="3"/>
-      <c r="D204" s="5"/>
-      <c r="E204" s="5"/>
+      <c r="B204" s="2">
+        <v>200</v>
+      </c>
+      <c r="C204" s="3">
+        <v>43522</v>
+      </c>
+      <c r="D204" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E204" s="5" t="s">
+        <v>935</v>
+      </c>
       <c r="F204" s="5"/>
-      <c r="G204" s="5"/>
+      <c r="G204" s="5" t="s">
+        <v>975</v>
+      </c>
       <c r="H204" s="5"/>
       <c r="I204" s="5"/>
       <c r="J204" s="5"/>
-      <c r="K204" s="5"/>
-      <c r="L204" s="5"/>
+      <c r="K204" s="5">
+        <v>1</v>
+      </c>
+      <c r="L204" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M204" s="5"/>
     </row>
     <row r="205" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B205" s="2"/>
-      <c r="C205" s="3"/>
-      <c r="D205" s="5"/>
-      <c r="E205" s="5"/>
+      <c r="B205" s="2">
+        <v>201</v>
+      </c>
+      <c r="C205" s="3">
+        <v>43522</v>
+      </c>
+      <c r="D205" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E205" s="5" t="s">
+        <v>936</v>
+      </c>
       <c r="F205" s="5"/>
-      <c r="G205" s="5"/>
+      <c r="G205" s="5" t="s">
+        <v>976</v>
+      </c>
       <c r="H205" s="5"/>
       <c r="I205" s="5"/>
       <c r="J205" s="5"/>
-      <c r="K205" s="5"/>
-      <c r="L205" s="5"/>
+      <c r="K205" s="5">
+        <v>1</v>
+      </c>
+      <c r="L205" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M205" s="5"/>
     </row>
     <row r="206" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B206" s="2"/>
-      <c r="C206" s="3"/>
-      <c r="D206" s="5"/>
-      <c r="E206" s="5"/>
+      <c r="B206" s="2">
+        <v>202</v>
+      </c>
+      <c r="C206" s="3">
+        <v>43522</v>
+      </c>
+      <c r="D206" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E206" s="5" t="s">
+        <v>937</v>
+      </c>
       <c r="F206" s="5"/>
-      <c r="G206" s="5"/>
+      <c r="G206" s="5" t="s">
+        <v>977</v>
+      </c>
       <c r="H206" s="5"/>
       <c r="I206" s="5"/>
       <c r="J206" s="5"/>
-      <c r="K206" s="5"/>
-      <c r="L206" s="5"/>
+      <c r="K206" s="5">
+        <v>1</v>
+      </c>
+      <c r="L206" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M206" s="5"/>
     </row>
     <row r="207" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B207" s="2"/>
-      <c r="C207" s="3"/>
-      <c r="D207" s="5"/>
-      <c r="E207" s="5"/>
+      <c r="B207" s="2">
+        <v>203</v>
+      </c>
+      <c r="C207" s="3">
+        <v>43522</v>
+      </c>
+      <c r="D207" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E207" s="5" t="s">
+        <v>938</v>
+      </c>
       <c r="F207" s="5"/>
-      <c r="G207" s="5"/>
+      <c r="G207" s="5" t="s">
+        <v>978</v>
+      </c>
       <c r="H207" s="5"/>
       <c r="I207" s="5"/>
       <c r="J207" s="5"/>
-      <c r="K207" s="5"/>
-      <c r="L207" s="5"/>
+      <c r="K207" s="5">
+        <v>1</v>
+      </c>
+      <c r="L207" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M207" s="5"/>
     </row>
     <row r="208" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B208" s="2"/>
-      <c r="C208" s="3"/>
-      <c r="D208" s="5"/>
-      <c r="E208" s="5"/>
+      <c r="B208" s="2">
+        <v>204</v>
+      </c>
+      <c r="C208" s="3">
+        <v>43522</v>
+      </c>
+      <c r="D208" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E208" s="5" t="s">
+        <v>939</v>
+      </c>
       <c r="F208" s="5"/>
-      <c r="G208" s="5"/>
+      <c r="G208" s="5" t="s">
+        <v>995</v>
+      </c>
       <c r="H208" s="5"/>
       <c r="I208" s="5"/>
       <c r="J208" s="5"/>
-      <c r="K208" s="5"/>
-      <c r="L208" s="5"/>
+      <c r="K208" s="5">
+        <v>1</v>
+      </c>
+      <c r="L208" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M208" s="5"/>
     </row>
     <row r="209" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B209" s="2"/>
-      <c r="C209" s="3"/>
-      <c r="D209" s="5"/>
-      <c r="E209" s="5"/>
+      <c r="B209" s="2">
+        <v>205</v>
+      </c>
+      <c r="C209" s="3">
+        <v>43522</v>
+      </c>
+      <c r="D209" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E209" s="5" t="s">
+        <v>940</v>
+      </c>
       <c r="F209" s="5"/>
-      <c r="G209" s="5"/>
+      <c r="G209" s="5" t="s">
+        <v>979</v>
+      </c>
       <c r="H209" s="5"/>
       <c r="I209" s="5"/>
       <c r="J209" s="5"/>
-      <c r="K209" s="5"/>
-      <c r="L209" s="5"/>
+      <c r="K209" s="5">
+        <v>1</v>
+      </c>
+      <c r="L209" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M209" s="5"/>
     </row>
     <row r="210" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B210" s="2"/>
-      <c r="C210" s="3"/>
-      <c r="D210" s="5"/>
-      <c r="E210" s="5"/>
+      <c r="B210" s="2">
+        <v>206</v>
+      </c>
+      <c r="C210" s="3">
+        <v>43522</v>
+      </c>
+      <c r="D210" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E210" s="5" t="s">
+        <v>941</v>
+      </c>
       <c r="F210" s="5"/>
-      <c r="G210" s="5"/>
+      <c r="G210" s="5" t="s">
+        <v>980</v>
+      </c>
       <c r="H210" s="5"/>
       <c r="I210" s="5"/>
       <c r="J210" s="5"/>
-      <c r="K210" s="5"/>
-      <c r="L210" s="5"/>
+      <c r="K210" s="5">
+        <v>1</v>
+      </c>
+      <c r="L210" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M210" s="5"/>
     </row>
     <row r="211" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B211" s="2"/>
-      <c r="C211" s="3"/>
-      <c r="D211" s="5"/>
-      <c r="E211" s="5"/>
+      <c r="B211" s="2">
+        <v>207</v>
+      </c>
+      <c r="C211" s="3">
+        <v>43522</v>
+      </c>
+      <c r="D211" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E211" s="5" t="s">
+        <v>942</v>
+      </c>
       <c r="F211" s="5"/>
-      <c r="G211" s="5"/>
+      <c r="G211" s="5" t="s">
+        <v>981</v>
+      </c>
       <c r="H211" s="5"/>
       <c r="I211" s="5"/>
       <c r="J211" s="5"/>
-      <c r="K211" s="5"/>
-      <c r="L211" s="5"/>
+      <c r="K211" s="5">
+        <v>1</v>
+      </c>
+      <c r="L211" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M211" s="5"/>
     </row>
     <row r="212" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B212" s="2"/>
-      <c r="C212" s="3"/>
-      <c r="D212" s="5"/>
-      <c r="E212" s="5"/>
+      <c r="B212" s="2">
+        <v>208</v>
+      </c>
+      <c r="C212" s="3">
+        <v>43522</v>
+      </c>
+      <c r="D212" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E212" s="5" t="s">
+        <v>943</v>
+      </c>
       <c r="F212" s="5"/>
-      <c r="G212" s="5"/>
+      <c r="G212" s="5" t="s">
+        <v>982</v>
+      </c>
       <c r="H212" s="5"/>
       <c r="I212" s="5"/>
       <c r="J212" s="5"/>
-      <c r="K212" s="5"/>
-      <c r="L212" s="5"/>
+      <c r="K212" s="5">
+        <v>1</v>
+      </c>
+      <c r="L212" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M212" s="5"/>
     </row>
     <row r="213" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B213" s="2"/>
-      <c r="C213" s="3"/>
-      <c r="D213" s="5"/>
-      <c r="E213" s="5"/>
+      <c r="B213" s="2">
+        <v>209</v>
+      </c>
+      <c r="C213" s="3">
+        <v>43522</v>
+      </c>
+      <c r="D213" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E213" s="5" t="s">
+        <v>944</v>
+      </c>
       <c r="F213" s="5"/>
-      <c r="G213" s="5"/>
+      <c r="G213" s="5" t="s">
+        <v>983</v>
+      </c>
       <c r="H213" s="5"/>
       <c r="I213" s="5"/>
       <c r="J213" s="5"/>
-      <c r="K213" s="5"/>
-      <c r="L213" s="5"/>
+      <c r="K213" s="5">
+        <v>1</v>
+      </c>
+      <c r="L213" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M213" s="5"/>
     </row>
     <row r="214" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B214" s="2"/>
-      <c r="C214" s="3"/>
-      <c r="D214" s="5"/>
-      <c r="E214" s="5"/>
+      <c r="B214" s="2">
+        <v>210</v>
+      </c>
+      <c r="C214" s="3">
+        <v>43522</v>
+      </c>
+      <c r="D214" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E214" s="5" t="s">
+        <v>945</v>
+      </c>
       <c r="F214" s="5"/>
-      <c r="G214" s="5"/>
+      <c r="G214" s="5" t="s">
+        <v>984</v>
+      </c>
       <c r="H214" s="5"/>
       <c r="I214" s="5"/>
       <c r="J214" s="5"/>
-      <c r="K214" s="5"/>
-      <c r="L214" s="5"/>
+      <c r="K214" s="5">
+        <v>1</v>
+      </c>
+      <c r="L214" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M214" s="5"/>
     </row>
     <row r="215" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B215" s="2"/>
-      <c r="C215" s="3"/>
-      <c r="D215" s="5"/>
-      <c r="E215" s="5"/>
+      <c r="B215" s="2">
+        <v>211</v>
+      </c>
+      <c r="C215" s="3">
+        <v>43522</v>
+      </c>
+      <c r="D215" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E215" s="5" t="s">
+        <v>946</v>
+      </c>
       <c r="F215" s="5"/>
-      <c r="G215" s="5"/>
+      <c r="G215" s="5" t="s">
+        <v>985</v>
+      </c>
       <c r="H215" s="5"/>
       <c r="I215" s="5"/>
       <c r="J215" s="5"/>
-      <c r="K215" s="5"/>
-      <c r="L215" s="5"/>
+      <c r="K215" s="5">
+        <v>1</v>
+      </c>
+      <c r="L215" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M215" s="5"/>
     </row>
     <row r="216" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B216" s="2"/>
-      <c r="C216" s="3"/>
-      <c r="D216" s="5"/>
-      <c r="E216" s="5"/>
+      <c r="B216" s="2">
+        <v>212</v>
+      </c>
+      <c r="C216" s="3">
+        <v>43522</v>
+      </c>
+      <c r="D216" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E216" s="5" t="s">
+        <v>947</v>
+      </c>
       <c r="F216" s="5"/>
-      <c r="G216" s="5"/>
+      <c r="G216" s="5" t="s">
+        <v>986</v>
+      </c>
       <c r="H216" s="5"/>
       <c r="I216" s="5"/>
       <c r="J216" s="5"/>
-      <c r="K216" s="5"/>
-      <c r="L216" s="5"/>
+      <c r="K216" s="5">
+        <v>1</v>
+      </c>
+      <c r="L216" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M216" s="5"/>
     </row>
     <row r="217" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B217" s="2"/>
-      <c r="C217" s="3"/>
-      <c r="D217" s="5"/>
-      <c r="E217" s="5"/>
+      <c r="B217" s="2">
+        <v>213</v>
+      </c>
+      <c r="C217" s="3">
+        <v>43522</v>
+      </c>
+      <c r="D217" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E217" s="5" t="s">
+        <v>948</v>
+      </c>
       <c r="F217" s="5"/>
-      <c r="G217" s="5"/>
+      <c r="G217" s="5" t="s">
+        <v>987</v>
+      </c>
       <c r="H217" s="5"/>
       <c r="I217" s="5"/>
       <c r="J217" s="5"/>
-      <c r="K217" s="5"/>
-      <c r="L217" s="5"/>
+      <c r="K217" s="5">
+        <v>1</v>
+      </c>
+      <c r="L217" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M217" s="5"/>
     </row>
     <row r="218" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B218" s="2"/>
-      <c r="C218" s="3"/>
-      <c r="D218" s="5"/>
-      <c r="E218" s="5"/>
+      <c r="B218" s="2">
+        <v>214</v>
+      </c>
+      <c r="C218" s="3">
+        <v>43522</v>
+      </c>
+      <c r="D218" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E218" s="5" t="s">
+        <v>949</v>
+      </c>
       <c r="F218" s="5"/>
-      <c r="G218" s="5"/>
-      <c r="H218" s="5"/>
+      <c r="G218" s="5" t="s">
+        <v>989</v>
+      </c>
+      <c r="H218" s="5" t="s">
+        <v>988</v>
+      </c>
       <c r="I218" s="5"/>
       <c r="J218" s="5"/>
-      <c r="K218" s="5"/>
-      <c r="L218" s="5"/>
+      <c r="K218" s="5">
+        <v>1</v>
+      </c>
+      <c r="L218" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M218" s="5"/>
     </row>
     <row r="219" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B219" s="2"/>
-      <c r="C219" s="3"/>
-      <c r="D219" s="5"/>
-      <c r="E219" s="5"/>
+      <c r="B219" s="2">
+        <v>215</v>
+      </c>
+      <c r="C219" s="3">
+        <v>43522</v>
+      </c>
+      <c r="D219" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E219" s="5" t="s">
+        <v>950</v>
+      </c>
       <c r="F219" s="5"/>
-      <c r="G219" s="5"/>
+      <c r="G219" s="5" t="s">
+        <v>990</v>
+      </c>
       <c r="H219" s="5"/>
       <c r="I219" s="5"/>
       <c r="J219" s="5"/>
-      <c r="K219" s="5"/>
-      <c r="L219" s="5"/>
+      <c r="K219" s="5">
+        <v>1</v>
+      </c>
+      <c r="L219" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M219" s="5"/>
     </row>
     <row r="220" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B220" s="2"/>
-      <c r="C220" s="3"/>
-      <c r="D220" s="5"/>
-      <c r="E220" s="5"/>
+      <c r="B220" s="2">
+        <v>216</v>
+      </c>
+      <c r="C220" s="3">
+        <v>43522</v>
+      </c>
+      <c r="D220" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E220" s="5" t="s">
+        <v>951</v>
+      </c>
       <c r="F220" s="5"/>
-      <c r="G220" s="5"/>
+      <c r="G220" s="5" t="s">
+        <v>958</v>
+      </c>
       <c r="H220" s="5"/>
       <c r="I220" s="5"/>
       <c r="J220" s="5"/>
-      <c r="K220" s="5"/>
-      <c r="L220" s="5"/>
+      <c r="K220" s="5">
+        <v>1</v>
+      </c>
+      <c r="L220" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M220" s="5"/>
     </row>
     <row r="221" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B221" s="2"/>
-      <c r="C221" s="3"/>
-      <c r="D221" s="5"/>
-      <c r="E221" s="5"/>
+      <c r="B221" s="2">
+        <v>217</v>
+      </c>
+      <c r="C221" s="3">
+        <v>43522</v>
+      </c>
+      <c r="D221" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E221" s="5" t="s">
+        <v>952</v>
+      </c>
       <c r="F221" s="5"/>
-      <c r="G221" s="5"/>
+      <c r="G221" s="5" t="s">
+        <v>959</v>
+      </c>
       <c r="H221" s="5"/>
       <c r="I221" s="5"/>
       <c r="J221" s="5"/>
-      <c r="K221" s="5"/>
-      <c r="L221" s="5"/>
+      <c r="K221" s="5">
+        <v>1</v>
+      </c>
+      <c r="L221" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M221" s="5"/>
     </row>
     <row r="222" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B222" s="2"/>
-      <c r="C222" s="3"/>
-      <c r="D222" s="5"/>
-      <c r="E222" s="5"/>
+      <c r="B222" s="2">
+        <v>218</v>
+      </c>
+      <c r="C222" s="3">
+        <v>43522</v>
+      </c>
+      <c r="D222" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E222" s="5" t="s">
+        <v>953</v>
+      </c>
       <c r="F222" s="5"/>
-      <c r="G222" s="5"/>
+      <c r="G222" s="5" t="s">
+        <v>960</v>
+      </c>
       <c r="H222" s="5"/>
       <c r="I222" s="5"/>
       <c r="J222" s="5"/>
-      <c r="K222" s="5"/>
-      <c r="L222" s="5"/>
+      <c r="K222" s="5">
+        <v>1</v>
+      </c>
+      <c r="L222" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M222" s="5"/>
     </row>
     <row r="223" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B223" s="2"/>
-      <c r="C223" s="3"/>
-      <c r="D223" s="5"/>
-      <c r="E223" s="5"/>
+      <c r="B223" s="2">
+        <v>219</v>
+      </c>
+      <c r="C223" s="3">
+        <v>43522</v>
+      </c>
+      <c r="D223" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E223" s="5" t="s">
+        <v>954</v>
+      </c>
       <c r="F223" s="5"/>
-      <c r="G223" s="5"/>
+      <c r="G223" s="5" t="s">
+        <v>961</v>
+      </c>
       <c r="H223" s="5"/>
       <c r="I223" s="5"/>
       <c r="J223" s="5"/>
-      <c r="K223" s="5"/>
-      <c r="L223" s="5"/>
+      <c r="K223" s="5">
+        <v>1</v>
+      </c>
+      <c r="L223" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M223" s="5"/>
     </row>
     <row r="224" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B224" s="2"/>
-      <c r="C224" s="3"/>
-      <c r="D224" s="5"/>
-      <c r="E224" s="5"/>
+      <c r="B224" s="2">
+        <v>220</v>
+      </c>
+      <c r="C224" s="3">
+        <v>43522</v>
+      </c>
+      <c r="D224" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E224" s="5" t="s">
+        <v>955</v>
+      </c>
       <c r="F224" s="5"/>
-      <c r="G224" s="5"/>
+      <c r="G224" s="5" t="s">
+        <v>962</v>
+      </c>
       <c r="H224" s="5"/>
       <c r="I224" s="5"/>
       <c r="J224" s="5"/>
-      <c r="K224" s="5"/>
-      <c r="L224" s="5"/>
+      <c r="K224" s="5">
+        <v>1</v>
+      </c>
+      <c r="L224" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M224" s="5"/>
     </row>
     <row r="225" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B225" s="2"/>
-      <c r="C225" s="3"/>
-      <c r="D225" s="5"/>
-      <c r="E225" s="5"/>
+      <c r="B225" s="2">
+        <v>221</v>
+      </c>
+      <c r="C225" s="3">
+        <v>43522</v>
+      </c>
+      <c r="D225" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E225" s="5" t="s">
+        <v>956</v>
+      </c>
       <c r="F225" s="5"/>
-      <c r="G225" s="5"/>
+      <c r="G225" s="5" t="s">
+        <v>963</v>
+      </c>
       <c r="H225" s="5"/>
       <c r="I225" s="5"/>
       <c r="J225" s="5"/>
-      <c r="K225" s="5"/>
-      <c r="L225" s="5"/>
+      <c r="K225" s="5">
+        <v>1</v>
+      </c>
+      <c r="L225" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M225" s="5"/>
     </row>
     <row r="226" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B226" s="2"/>
-      <c r="C226" s="3"/>
-      <c r="D226" s="5"/>
-      <c r="E226" s="5"/>
+      <c r="B226" s="2">
+        <v>222</v>
+      </c>
+      <c r="C226" s="3">
+        <v>43522</v>
+      </c>
+      <c r="D226" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E226" s="5" t="s">
+        <v>957</v>
+      </c>
       <c r="F226" s="5"/>
-      <c r="G226" s="5"/>
-      <c r="H226" s="5"/>
+      <c r="G226" s="5" t="s">
+        <v>964</v>
+      </c>
+      <c r="H226" s="5" t="s">
+        <v>965</v>
+      </c>
       <c r="I226" s="5"/>
       <c r="J226" s="5"/>
-      <c r="K226" s="5"/>
-      <c r="L226" s="5"/>
+      <c r="K226" s="5">
+        <v>1</v>
+      </c>
+      <c r="L226" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M226" s="5"/>
     </row>
     <row r="227" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B227" s="2"/>
-      <c r="C227" s="3"/>
-      <c r="D227" s="5"/>
-      <c r="E227" s="5"/>
+      <c r="B227" s="2">
+        <v>223</v>
+      </c>
+      <c r="C227" s="3">
+        <v>43522</v>
+      </c>
+      <c r="D227" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E227" s="5" t="s">
+        <v>966</v>
+      </c>
       <c r="F227" s="5"/>
-      <c r="G227" s="5"/>
+      <c r="G227" s="5" t="s">
+        <v>991</v>
+      </c>
       <c r="H227" s="5"/>
       <c r="I227" s="5"/>
       <c r="J227" s="5"/>
-      <c r="K227" s="5"/>
-      <c r="L227" s="5"/>
+      <c r="K227" s="5">
+        <v>1</v>
+      </c>
+      <c r="L227" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M227" s="5"/>
     </row>
     <row r="228" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B228" s="2"/>
-      <c r="C228" s="3"/>
-      <c r="D228" s="5"/>
-      <c r="E228" s="5"/>
+      <c r="B228" s="2">
+        <v>224</v>
+      </c>
+      <c r="C228" s="3">
+        <v>43522</v>
+      </c>
+      <c r="D228" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E228" s="5" t="s">
+        <v>967</v>
+      </c>
       <c r="F228" s="5"/>
-      <c r="G228" s="5"/>
+      <c r="G228" s="5" t="s">
+        <v>992</v>
+      </c>
       <c r="H228" s="5"/>
       <c r="I228" s="5"/>
       <c r="J228" s="5"/>
-      <c r="K228" s="5"/>
-      <c r="L228" s="5"/>
+      <c r="K228" s="5">
+        <v>1</v>
+      </c>
+      <c r="L228" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M228" s="5"/>
     </row>
     <row r="229" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B229" s="2"/>
-      <c r="C229" s="3"/>
-      <c r="D229" s="5"/>
-      <c r="E229" s="5"/>
+      <c r="B229" s="2">
+        <v>225</v>
+      </c>
+      <c r="C229" s="3">
+        <v>43522</v>
+      </c>
+      <c r="D229" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E229" s="5" t="s">
+        <v>968</v>
+      </c>
       <c r="F229" s="5"/>
-      <c r="G229" s="5"/>
+      <c r="G229" s="5" t="s">
+        <v>993</v>
+      </c>
       <c r="H229" s="5"/>
       <c r="I229" s="5"/>
       <c r="J229" s="5"/>
-      <c r="K229" s="5"/>
-      <c r="L229" s="5"/>
+      <c r="K229" s="5">
+        <v>1</v>
+      </c>
+      <c r="L229" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M229" s="5"/>
     </row>
     <row r="230" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B230" s="2"/>
-      <c r="C230" s="3"/>
-      <c r="D230" s="5"/>
-      <c r="E230" s="5"/>
+      <c r="B230" s="2">
+        <v>226</v>
+      </c>
+      <c r="C230" s="3">
+        <v>43522</v>
+      </c>
+      <c r="D230" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E230" s="5" t="s">
+        <v>969</v>
+      </c>
       <c r="F230" s="5"/>
-      <c r="G230" s="5"/>
+      <c r="G230" s="5" t="s">
+        <v>994</v>
+      </c>
       <c r="H230" s="5"/>
       <c r="I230" s="5"/>
       <c r="J230" s="5"/>
-      <c r="K230" s="5"/>
-      <c r="L230" s="5"/>
+      <c r="K230" s="5">
+        <v>1</v>
+      </c>
+      <c r="L230" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M230" s="5"/>
     </row>
     <row r="231" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B231" s="2"/>
-      <c r="C231" s="3"/>
-      <c r="D231" s="5"/>
-      <c r="E231" s="5"/>
+      <c r="B231" s="2">
+        <v>227</v>
+      </c>
+      <c r="C231" s="3">
+        <v>43523</v>
+      </c>
+      <c r="D231" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E231" s="5" t="s">
+        <v>996</v>
+      </c>
       <c r="F231" s="5"/>
-      <c r="G231" s="5"/>
+      <c r="G231" s="5" t="s">
+        <v>1013</v>
+      </c>
       <c r="H231" s="5"/>
       <c r="I231" s="5"/>
       <c r="J231" s="5"/>
-      <c r="K231" s="5"/>
-      <c r="L231" s="5"/>
+      <c r="K231" s="5">
+        <v>1</v>
+      </c>
+      <c r="L231" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M231" s="5"/>
     </row>
     <row r="232" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B232" s="2"/>
-      <c r="C232" s="3"/>
-      <c r="D232" s="5"/>
-      <c r="E232" s="5"/>
+      <c r="B232" s="2">
+        <v>228</v>
+      </c>
+      <c r="C232" s="3">
+        <v>43523</v>
+      </c>
+      <c r="D232" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E232" s="5" t="s">
+        <v>997</v>
+      </c>
       <c r="F232" s="5"/>
-      <c r="G232" s="5"/>
+      <c r="G232" s="5" t="s">
+        <v>1004</v>
+      </c>
       <c r="H232" s="5"/>
       <c r="I232" s="5"/>
       <c r="J232" s="5"/>
-      <c r="K232" s="5"/>
-      <c r="L232" s="5"/>
+      <c r="K232" s="5">
+        <v>1</v>
+      </c>
+      <c r="L232" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M232" s="5"/>
     </row>
     <row r="233" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B233" s="2"/>
-      <c r="C233" s="3"/>
-      <c r="D233" s="5"/>
-      <c r="E233" s="5"/>
+      <c r="B233" s="2">
+        <v>229</v>
+      </c>
+      <c r="C233" s="3">
+        <v>43523</v>
+      </c>
+      <c r="D233" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E233" s="5" t="s">
+        <v>998</v>
+      </c>
       <c r="F233" s="5"/>
-      <c r="G233" s="5"/>
+      <c r="G233" s="5" t="s">
+        <v>1005</v>
+      </c>
       <c r="H233" s="5"/>
       <c r="I233" s="5"/>
       <c r="J233" s="5"/>
-      <c r="K233" s="5"/>
-      <c r="L233" s="5"/>
+      <c r="K233" s="5">
+        <v>1</v>
+      </c>
+      <c r="L233" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M233" s="5"/>
     </row>
     <row r="234" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B234" s="2"/>
-      <c r="C234" s="3"/>
-      <c r="D234" s="5"/>
-      <c r="E234" s="5"/>
+      <c r="B234" s="2">
+        <v>230</v>
+      </c>
+      <c r="C234" s="3">
+        <v>43523</v>
+      </c>
+      <c r="D234" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E234" s="5" t="s">
+        <v>999</v>
+      </c>
       <c r="F234" s="5"/>
-      <c r="G234" s="5"/>
+      <c r="G234" s="5" t="s">
+        <v>1006</v>
+      </c>
       <c r="H234" s="5"/>
       <c r="I234" s="5"/>
       <c r="J234" s="5"/>
-      <c r="K234" s="5"/>
-      <c r="L234" s="5"/>
+      <c r="K234" s="5">
+        <v>1</v>
+      </c>
+      <c r="L234" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M234" s="5"/>
     </row>
     <row r="235" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B235" s="2"/>
-      <c r="C235" s="3"/>
-      <c r="D235" s="5"/>
-      <c r="E235" s="5"/>
+      <c r="B235" s="2">
+        <v>231</v>
+      </c>
+      <c r="C235" s="3">
+        <v>43523</v>
+      </c>
+      <c r="D235" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E235" s="5" t="s">
+        <v>1000</v>
+      </c>
       <c r="F235" s="5"/>
-      <c r="G235" s="5"/>
-      <c r="H235" s="5"/>
+      <c r="G235" s="5" t="s">
+        <v>1011</v>
+      </c>
+      <c r="H235" s="5" t="s">
+        <v>1012</v>
+      </c>
       <c r="I235" s="5"/>
       <c r="J235" s="5"/>
-      <c r="K235" s="5"/>
-      <c r="L235" s="5"/>
+      <c r="K235" s="5">
+        <v>1</v>
+      </c>
+      <c r="L235" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M235" s="5"/>
     </row>
     <row r="236" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B236" s="2"/>
-      <c r="C236" s="3"/>
-      <c r="D236" s="5"/>
-      <c r="E236" s="5"/>
+      <c r="B236" s="2">
+        <v>232</v>
+      </c>
+      <c r="C236" s="3">
+        <v>43523</v>
+      </c>
+      <c r="D236" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E236" s="5" t="s">
+        <v>1001</v>
+      </c>
       <c r="F236" s="5"/>
-      <c r="G236" s="5"/>
+      <c r="G236" s="5" t="s">
+        <v>1007</v>
+      </c>
       <c r="H236" s="5"/>
       <c r="I236" s="5"/>
       <c r="J236" s="5"/>
-      <c r="K236" s="5"/>
-      <c r="L236" s="5"/>
+      <c r="K236" s="5">
+        <v>1</v>
+      </c>
+      <c r="L236" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M236" s="5"/>
     </row>
     <row r="237" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B237" s="2"/>
-      <c r="C237" s="3"/>
-      <c r="D237" s="5"/>
-      <c r="E237" s="5"/>
+      <c r="B237" s="2">
+        <v>233</v>
+      </c>
+      <c r="C237" s="3">
+        <v>43523</v>
+      </c>
+      <c r="D237" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E237" s="5" t="s">
+        <v>1002</v>
+      </c>
       <c r="F237" s="5"/>
-      <c r="G237" s="5"/>
+      <c r="G237" s="5" t="s">
+        <v>1008</v>
+      </c>
       <c r="H237" s="5"/>
       <c r="I237" s="5"/>
       <c r="J237" s="5"/>
-      <c r="K237" s="5"/>
-      <c r="L237" s="5"/>
+      <c r="K237" s="5">
+        <v>1</v>
+      </c>
+      <c r="L237" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M237" s="5"/>
     </row>
     <row r="238" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B238" s="2"/>
-      <c r="C238" s="3"/>
-      <c r="D238" s="5"/>
-      <c r="E238" s="5"/>
+      <c r="B238" s="2">
+        <v>234</v>
+      </c>
+      <c r="C238" s="3">
+        <v>43523</v>
+      </c>
+      <c r="D238" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E238" s="5" t="s">
+        <v>1014</v>
+      </c>
       <c r="F238" s="5"/>
-      <c r="G238" s="5"/>
+      <c r="G238" s="5" t="s">
+        <v>1009</v>
+      </c>
       <c r="H238" s="5"/>
       <c r="I238" s="5"/>
       <c r="J238" s="5"/>
-      <c r="K238" s="5"/>
-      <c r="L238" s="5"/>
+      <c r="K238" s="5">
+        <v>1</v>
+      </c>
+      <c r="L238" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M238" s="5"/>
     </row>
     <row r="239" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B239" s="2"/>
-      <c r="C239" s="3"/>
-      <c r="D239" s="5"/>
-      <c r="E239" s="5"/>
+      <c r="B239" s="2">
+        <v>235</v>
+      </c>
+      <c r="C239" s="3">
+        <v>43523</v>
+      </c>
+      <c r="D239" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E239" s="5" t="s">
+        <v>1003</v>
+      </c>
       <c r="F239" s="5"/>
-      <c r="G239" s="5"/>
+      <c r="G239" s="5" t="s">
+        <v>1010</v>
+      </c>
       <c r="H239" s="5"/>
       <c r="I239" s="5"/>
       <c r="J239" s="5"/>
-      <c r="K239" s="5"/>
-      <c r="L239" s="5"/>
+      <c r="K239" s="5">
+        <v>1</v>
+      </c>
+      <c r="L239" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M239" s="5"/>
     </row>
     <row r="240" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B240" s="2"/>
-      <c r="C240" s="3"/>
-      <c r="D240" s="5"/>
-      <c r="E240" s="5"/>
+      <c r="B240" s="2">
+        <v>236</v>
+      </c>
+      <c r="C240" s="3">
+        <v>43524</v>
+      </c>
+      <c r="D240" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E240" s="5" t="s">
+        <v>1015</v>
+      </c>
       <c r="F240" s="5"/>
-      <c r="G240" s="5"/>
-      <c r="H240" s="5"/>
+      <c r="G240" s="5" t="s">
+        <v>1018</v>
+      </c>
+      <c r="H240" s="5" t="s">
+        <v>1016</v>
+      </c>
       <c r="I240" s="5"/>
       <c r="J240" s="5"/>
-      <c r="K240" s="5"/>
-      <c r="L240" s="5"/>
+      <c r="K240" s="5">
+        <v>1</v>
+      </c>
+      <c r="L240" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M240" s="5"/>
     </row>
     <row r="241" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B241" s="2"/>
-      <c r="C241" s="3"/>
-      <c r="D241" s="5"/>
-      <c r="E241" s="5"/>
+      <c r="B241" s="2">
+        <v>237</v>
+      </c>
+      <c r="C241" s="3">
+        <v>43524</v>
+      </c>
+      <c r="D241" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E241" s="5" t="s">
+        <v>1017</v>
+      </c>
       <c r="F241" s="5"/>
-      <c r="G241" s="5"/>
+      <c r="G241" s="5" t="s">
+        <v>1019</v>
+      </c>
       <c r="H241" s="5"/>
       <c r="I241" s="5"/>
       <c r="J241" s="5"/>
-      <c r="K241" s="5"/>
-      <c r="L241" s="5"/>
+      <c r="K241" s="5">
+        <v>1</v>
+      </c>
+      <c r="L241" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M241" s="5"/>
     </row>
     <row r="242" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
@@ -9383,7 +10465,7 @@
       <c r="L249" s="5"/>
       <c r="M249" s="5"/>
     </row>
-    <row r="250" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="250" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B250" s="2"/>
       <c r="C250" s="3"/>
       <c r="D250" s="5"/>
@@ -13177,36 +14259,22 @@
       <c r="L520" s="5"/>
       <c r="M520" s="5"/>
     </row>
-    <row r="521" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B521" s="2"/>
-      <c r="C521" s="3"/>
-      <c r="D521" s="5"/>
-      <c r="E521" s="5"/>
-      <c r="F521" s="5"/>
-      <c r="G521" s="5"/>
-      <c r="H521" s="5"/>
-      <c r="I521" s="5"/>
-      <c r="J521" s="5"/>
-      <c r="K521" s="5"/>
-      <c r="L521" s="5"/>
-      <c r="M521" s="5"/>
-    </row>
   </sheetData>
-  <autoFilter ref="B4:M175"/>
+  <autoFilter ref="B4:M190"/>
   <mergeCells count="1">
     <mergeCell ref="B2:L2"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D115 D189:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D115 D242:D1048576">
       <formula1>"Likeshuo,TOEFL,TPO"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D116:D188">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D116:D241">
       <formula1>"Likeshuo,TOEFL,TPO, 500 setns"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L5:L521">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L5:L520">
       <formula1>"Input, Renew, Understood, Reviewed, Forgot"</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C521">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C520">
       <formula1>43508</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Vocabulary Statistic Chart for TOEFL update
</commit_message>
<xml_diff>
--- a/english_learning/Vocabulary Statistic Chart for TOEFL.xlsx
+++ b/english_learning/Vocabulary Statistic Chart for TOEFL.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2083" uniqueCount="1020">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2241" uniqueCount="1100">
   <si>
     <t>Expression</t>
   </si>
@@ -3047,9 +3047,6 @@
     <t>悖</t>
   </si>
   <si>
-    <t>一个女人与鲍勃发型</t>
-  </si>
-  <si>
     <t>非法经营</t>
   </si>
   <si>
@@ -3090,6 +3087,249 @@
   </si>
   <si>
     <t>模糊</t>
+  </si>
+  <si>
+    <t>一个鲍勃发型女人</t>
+  </si>
+  <si>
+    <t>antonyms</t>
+  </si>
+  <si>
+    <t>justifying</t>
+  </si>
+  <si>
+    <t>fell asleep</t>
+  </si>
+  <si>
+    <t>反义词</t>
+  </si>
+  <si>
+    <t>合乎道德的</t>
+  </si>
+  <si>
+    <t>睡着了</t>
+  </si>
+  <si>
+    <t>找理由</t>
+  </si>
+  <si>
+    <t>etiquette</t>
+  </si>
+  <si>
+    <t>quilt</t>
+  </si>
+  <si>
+    <t>recipe</t>
+  </si>
+  <si>
+    <t>bridal registry</t>
+  </si>
+  <si>
+    <t>a particular profession or group</t>
+  </si>
+  <si>
+    <t>gratitude</t>
+  </si>
+  <si>
+    <t>allergies</t>
+  </si>
+  <si>
+    <t>bridal shower</t>
+  </si>
+  <si>
+    <t>bride-to-be</t>
+  </si>
+  <si>
+    <t>itch</t>
+  </si>
+  <si>
+    <t>embroidery</t>
+  </si>
+  <si>
+    <t>Knitting sweater</t>
+  </si>
+  <si>
+    <t>Sewing machine</t>
+  </si>
+  <si>
+    <t>痒</t>
+  </si>
+  <si>
+    <t>刺绣</t>
+  </si>
+  <si>
+    <t>织毛衣</t>
+  </si>
+  <si>
+    <t>缝纫机</t>
+  </si>
+  <si>
+    <t>礼仪</t>
+  </si>
+  <si>
+    <t>被子</t>
+  </si>
+  <si>
+    <t>食谱</t>
+  </si>
+  <si>
+    <t>新娘登记</t>
+  </si>
+  <si>
+    <t>特定的职业或团体</t>
+  </si>
+  <si>
+    <t>感谢</t>
+  </si>
+  <si>
+    <t>过敏</t>
+  </si>
+  <si>
+    <t>新娘送礼</t>
+  </si>
+  <si>
+    <t>准新娘</t>
+  </si>
+  <si>
+    <t>recount it as sagas</t>
+  </si>
+  <si>
+    <t>recount:叙述</t>
+  </si>
+  <si>
+    <t>saga:英雄故事</t>
+  </si>
+  <si>
+    <t>NCE4</t>
+  </si>
+  <si>
+    <t>legends handed down</t>
+  </si>
+  <si>
+    <t>flint</t>
+  </si>
+  <si>
+    <t>have rotted away</t>
+  </si>
+  <si>
+    <t>hand on:传承</t>
+  </si>
+  <si>
+    <t>a hard kind of stone</t>
+  </si>
+  <si>
+    <t>rot away</t>
+  </si>
+  <si>
+    <t>rotted</t>
+  </si>
+  <si>
+    <t>offender</t>
+  </si>
+  <si>
+    <t>transgress</t>
+  </si>
+  <si>
+    <t>moral or civil law</t>
+  </si>
+  <si>
+    <t>appeal</t>
+  </si>
+  <si>
+    <t>smooth</t>
+  </si>
+  <si>
+    <t>penalty</t>
+  </si>
+  <si>
+    <t>abide</t>
+  </si>
+  <si>
+    <t>sanction</t>
+  </si>
+  <si>
+    <t>condemnation</t>
+  </si>
+  <si>
+    <t>objective</t>
+  </si>
+  <si>
+    <t>censure</t>
+  </si>
+  <si>
+    <t>repent</t>
+  </si>
+  <si>
+    <t>deter</t>
+  </si>
+  <si>
+    <t>inflict</t>
+  </si>
+  <si>
+    <t>judge</t>
+  </si>
+  <si>
+    <t>court</t>
+  </si>
+  <si>
+    <t>bribe</t>
+  </si>
+  <si>
+    <t>conduct</t>
+  </si>
+  <si>
+    <t>犯罪分子</t>
+  </si>
+  <si>
+    <t>侵越</t>
+  </si>
+  <si>
+    <t>道德或民法</t>
+  </si>
+  <si>
+    <t>上诉</t>
+  </si>
+  <si>
+    <t>平滑</t>
+  </si>
+  <si>
+    <t>罚款</t>
+  </si>
+  <si>
+    <t>遵守</t>
+  </si>
+  <si>
+    <t>制裁</t>
+  </si>
+  <si>
+    <t>非难</t>
+  </si>
+  <si>
+    <t>目的</t>
+  </si>
+  <si>
+    <t>谴责</t>
+  </si>
+  <si>
+    <t>悔改</t>
+  </si>
+  <si>
+    <t>阻止</t>
+  </si>
+  <si>
+    <t>造成</t>
+  </si>
+  <si>
+    <t>法官</t>
+  </si>
+  <si>
+    <t>法庭</t>
+  </si>
+  <si>
+    <t>贿赂</t>
+  </si>
+  <si>
+    <t>进行</t>
   </si>
 </sst>
 </file>
@@ -3545,8 +3785,8 @@
   <dimension ref="B1:M520"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A232" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G234" sqref="G234"/>
+      <pane ySplit="4" topLeftCell="A261" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E274" sqref="E274"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
@@ -10056,7 +10296,7 @@
       </c>
       <c r="F231" s="5"/>
       <c r="G231" s="5" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="H231" s="5"/>
       <c r="I231" s="5"/>
@@ -10112,7 +10352,7 @@
       </c>
       <c r="F233" s="5"/>
       <c r="G233" s="5" t="s">
-        <v>1005</v>
+        <v>1019</v>
       </c>
       <c r="H233" s="5"/>
       <c r="I233" s="5"/>
@@ -10140,7 +10380,7 @@
       </c>
       <c r="F234" s="5"/>
       <c r="G234" s="5" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="H234" s="5"/>
       <c r="I234" s="5"/>
@@ -10168,10 +10408,10 @@
       </c>
       <c r="F235" s="5"/>
       <c r="G235" s="5" t="s">
+        <v>1010</v>
+      </c>
+      <c r="H235" s="5" t="s">
         <v>1011</v>
-      </c>
-      <c r="H235" s="5" t="s">
-        <v>1012</v>
       </c>
       <c r="I235" s="5"/>
       <c r="J235" s="5"/>
@@ -10198,7 +10438,7 @@
       </c>
       <c r="F236" s="5"/>
       <c r="G236" s="5" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="H236" s="5"/>
       <c r="I236" s="5"/>
@@ -10226,7 +10466,7 @@
       </c>
       <c r="F237" s="5"/>
       <c r="G237" s="5" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="H237" s="5"/>
       <c r="I237" s="5"/>
@@ -10250,11 +10490,11 @@
         <v>213</v>
       </c>
       <c r="E238" s="5" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="F238" s="5"/>
       <c r="G238" s="5" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="H238" s="5"/>
       <c r="I238" s="5"/>
@@ -10282,7 +10522,7 @@
       </c>
       <c r="F239" s="5"/>
       <c r="G239" s="5" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="H239" s="5"/>
       <c r="I239" s="5"/>
@@ -10306,14 +10546,14 @@
         <v>213</v>
       </c>
       <c r="E240" s="5" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="F240" s="5"/>
       <c r="G240" s="5" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="H240" s="5" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="I240" s="5"/>
       <c r="J240" s="5"/>
@@ -10336,11 +10576,11 @@
         <v>213</v>
       </c>
       <c r="E241" s="5" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="F241" s="5"/>
       <c r="G241" s="5" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="H241" s="5"/>
       <c r="I241" s="5"/>
@@ -10354,549 +10594,1099 @@
       <c r="M241" s="5"/>
     </row>
     <row r="242" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B242" s="2"/>
-      <c r="C242" s="3"/>
-      <c r="D242" s="5"/>
-      <c r="E242" s="5"/>
+      <c r="B242" s="2">
+        <v>238</v>
+      </c>
+      <c r="C242" s="3">
+        <v>43525</v>
+      </c>
+      <c r="D242" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E242" s="5" t="s">
+        <v>1020</v>
+      </c>
       <c r="F242" s="5"/>
-      <c r="G242" s="5"/>
+      <c r="G242" s="5" t="s">
+        <v>1023</v>
+      </c>
       <c r="H242" s="5"/>
       <c r="I242" s="5"/>
       <c r="J242" s="5"/>
-      <c r="K242" s="5"/>
-      <c r="L242" s="5"/>
+      <c r="K242" s="5">
+        <v>1</v>
+      </c>
+      <c r="L242" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M242" s="5"/>
     </row>
     <row r="243" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B243" s="2"/>
-      <c r="C243" s="3"/>
-      <c r="D243" s="5"/>
-      <c r="E243" s="5"/>
+      <c r="B243" s="2">
+        <v>239</v>
+      </c>
+      <c r="C243" s="3">
+        <v>43525</v>
+      </c>
+      <c r="D243" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E243" s="5" t="s">
+        <v>425</v>
+      </c>
       <c r="F243" s="5"/>
-      <c r="G243" s="5"/>
+      <c r="G243" s="5" t="s">
+        <v>1024</v>
+      </c>
       <c r="H243" s="5"/>
       <c r="I243" s="5"/>
       <c r="J243" s="5"/>
-      <c r="K243" s="5"/>
-      <c r="L243" s="5"/>
+      <c r="K243" s="5">
+        <v>1</v>
+      </c>
+      <c r="L243" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M243" s="5"/>
     </row>
     <row r="244" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B244" s="2"/>
-      <c r="C244" s="3"/>
-      <c r="D244" s="5"/>
-      <c r="E244" s="5"/>
+      <c r="B244" s="2">
+        <v>240</v>
+      </c>
+      <c r="C244" s="3">
+        <v>43525</v>
+      </c>
+      <c r="D244" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E244" s="5" t="s">
+        <v>1021</v>
+      </c>
       <c r="F244" s="5"/>
-      <c r="G244" s="5"/>
+      <c r="G244" s="5" t="s">
+        <v>1026</v>
+      </c>
       <c r="H244" s="5"/>
       <c r="I244" s="5"/>
       <c r="J244" s="5"/>
-      <c r="K244" s="5"/>
-      <c r="L244" s="5"/>
+      <c r="K244" s="5">
+        <v>1</v>
+      </c>
+      <c r="L244" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M244" s="5"/>
     </row>
     <row r="245" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B245" s="2"/>
-      <c r="C245" s="3"/>
-      <c r="D245" s="5"/>
-      <c r="E245" s="5"/>
+      <c r="B245" s="2">
+        <v>241</v>
+      </c>
+      <c r="C245" s="3">
+        <v>43525</v>
+      </c>
+      <c r="D245" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E245" s="5" t="s">
+        <v>1022</v>
+      </c>
       <c r="F245" s="5"/>
-      <c r="G245" s="5"/>
+      <c r="G245" s="5" t="s">
+        <v>1025</v>
+      </c>
       <c r="H245" s="5"/>
       <c r="I245" s="5"/>
       <c r="J245" s="5"/>
-      <c r="K245" s="5"/>
-      <c r="L245" s="5"/>
+      <c r="K245" s="5">
+        <v>1</v>
+      </c>
+      <c r="L245" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M245" s="5"/>
     </row>
     <row r="246" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B246" s="2"/>
-      <c r="C246" s="3"/>
-      <c r="D246" s="5"/>
-      <c r="E246" s="5"/>
+      <c r="B246" s="2">
+        <v>242</v>
+      </c>
+      <c r="C246" s="3">
+        <v>43528</v>
+      </c>
+      <c r="D246" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E246" s="5" t="s">
+        <v>1027</v>
+      </c>
       <c r="F246" s="5"/>
-      <c r="G246" s="5"/>
+      <c r="G246" s="5" t="s">
+        <v>1044</v>
+      </c>
       <c r="H246" s="5"/>
       <c r="I246" s="5"/>
       <c r="J246" s="5"/>
-      <c r="K246" s="5"/>
-      <c r="L246" s="5"/>
+      <c r="K246" s="5">
+        <v>1</v>
+      </c>
+      <c r="L246" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M246" s="5"/>
     </row>
     <row r="247" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B247" s="2"/>
-      <c r="C247" s="3"/>
-      <c r="D247" s="5"/>
-      <c r="E247" s="5"/>
+      <c r="B247" s="2">
+        <v>243</v>
+      </c>
+      <c r="C247" s="3">
+        <v>43528</v>
+      </c>
+      <c r="D247" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E247" s="5" t="s">
+        <v>1028</v>
+      </c>
       <c r="F247" s="5"/>
-      <c r="G247" s="5"/>
+      <c r="G247" s="5" t="s">
+        <v>1045</v>
+      </c>
       <c r="H247" s="5"/>
       <c r="I247" s="5"/>
       <c r="J247" s="5"/>
-      <c r="K247" s="5"/>
-      <c r="L247" s="5"/>
+      <c r="K247" s="5">
+        <v>1</v>
+      </c>
+      <c r="L247" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M247" s="5"/>
     </row>
     <row r="248" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B248" s="2"/>
-      <c r="C248" s="3"/>
-      <c r="D248" s="5"/>
-      <c r="E248" s="5"/>
+      <c r="B248" s="2">
+        <v>244</v>
+      </c>
+      <c r="C248" s="3">
+        <v>43528</v>
+      </c>
+      <c r="D248" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E248" s="5" t="s">
+        <v>1029</v>
+      </c>
       <c r="F248" s="5"/>
-      <c r="G248" s="5"/>
+      <c r="G248" s="5" t="s">
+        <v>1046</v>
+      </c>
       <c r="H248" s="5"/>
       <c r="I248" s="5"/>
       <c r="J248" s="5"/>
-      <c r="K248" s="5"/>
-      <c r="L248" s="5"/>
+      <c r="K248" s="5">
+        <v>1</v>
+      </c>
+      <c r="L248" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M248" s="5"/>
     </row>
     <row r="249" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B249" s="2"/>
-      <c r="C249" s="3"/>
-      <c r="D249" s="5"/>
-      <c r="E249" s="5"/>
+      <c r="B249" s="2">
+        <v>245</v>
+      </c>
+      <c r="C249" s="3">
+        <v>43528</v>
+      </c>
+      <c r="D249" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E249" s="5" t="s">
+        <v>1030</v>
+      </c>
       <c r="F249" s="5"/>
-      <c r="G249" s="5"/>
+      <c r="G249" s="5" t="s">
+        <v>1047</v>
+      </c>
       <c r="H249" s="5"/>
       <c r="I249" s="5"/>
       <c r="J249" s="5"/>
-      <c r="K249" s="5"/>
-      <c r="L249" s="5"/>
+      <c r="K249" s="5">
+        <v>1</v>
+      </c>
+      <c r="L249" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M249" s="5"/>
     </row>
     <row r="250" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B250" s="2"/>
-      <c r="C250" s="3"/>
-      <c r="D250" s="5"/>
-      <c r="E250" s="5"/>
+      <c r="B250" s="2">
+        <v>246</v>
+      </c>
+      <c r="C250" s="3">
+        <v>43528</v>
+      </c>
+      <c r="D250" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E250" s="5" t="s">
+        <v>1031</v>
+      </c>
       <c r="F250" s="5"/>
-      <c r="G250" s="5"/>
+      <c r="G250" s="5" t="s">
+        <v>1048</v>
+      </c>
       <c r="H250" s="5"/>
       <c r="I250" s="5"/>
       <c r="J250" s="5"/>
-      <c r="K250" s="5"/>
-      <c r="L250" s="5"/>
+      <c r="K250" s="5">
+        <v>1</v>
+      </c>
+      <c r="L250" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M250" s="5"/>
     </row>
     <row r="251" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B251" s="2"/>
-      <c r="C251" s="3"/>
-      <c r="D251" s="5"/>
-      <c r="E251" s="5"/>
+      <c r="B251" s="2">
+        <v>247</v>
+      </c>
+      <c r="C251" s="3">
+        <v>43528</v>
+      </c>
+      <c r="D251" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E251" s="5" t="s">
+        <v>1032</v>
+      </c>
       <c r="F251" s="5"/>
-      <c r="G251" s="5"/>
+      <c r="G251" s="5" t="s">
+        <v>1049</v>
+      </c>
       <c r="H251" s="5"/>
       <c r="I251" s="5"/>
       <c r="J251" s="5"/>
-      <c r="K251" s="5"/>
-      <c r="L251" s="5"/>
+      <c r="K251" s="5">
+        <v>1</v>
+      </c>
+      <c r="L251" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M251" s="5"/>
     </row>
     <row r="252" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B252" s="2"/>
-      <c r="C252" s="3"/>
-      <c r="D252" s="5"/>
-      <c r="E252" s="5"/>
+      <c r="B252" s="2">
+        <v>248</v>
+      </c>
+      <c r="C252" s="3">
+        <v>43528</v>
+      </c>
+      <c r="D252" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E252" s="5" t="s">
+        <v>1033</v>
+      </c>
       <c r="F252" s="5"/>
-      <c r="G252" s="5"/>
+      <c r="G252" s="5" t="s">
+        <v>1050</v>
+      </c>
       <c r="H252" s="5"/>
       <c r="I252" s="5"/>
       <c r="J252" s="5"/>
-      <c r="K252" s="5"/>
-      <c r="L252" s="5"/>
+      <c r="K252" s="5">
+        <v>1</v>
+      </c>
+      <c r="L252" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M252" s="5"/>
     </row>
     <row r="253" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B253" s="2"/>
-      <c r="C253" s="3"/>
-      <c r="D253" s="5"/>
-      <c r="E253" s="5"/>
+      <c r="B253" s="2">
+        <v>249</v>
+      </c>
+      <c r="C253" s="3">
+        <v>43528</v>
+      </c>
+      <c r="D253" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E253" s="5" t="s">
+        <v>1034</v>
+      </c>
       <c r="F253" s="5"/>
-      <c r="G253" s="5"/>
+      <c r="G253" s="5" t="s">
+        <v>1051</v>
+      </c>
       <c r="H253" s="5"/>
       <c r="I253" s="5"/>
       <c r="J253" s="5"/>
-      <c r="K253" s="5"/>
-      <c r="L253" s="5"/>
+      <c r="K253" s="5">
+        <v>1</v>
+      </c>
+      <c r="L253" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M253" s="5"/>
     </row>
     <row r="254" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B254" s="2"/>
-      <c r="C254" s="3"/>
-      <c r="D254" s="5"/>
-      <c r="E254" s="5"/>
+      <c r="B254" s="2">
+        <v>250</v>
+      </c>
+      <c r="C254" s="3">
+        <v>43528</v>
+      </c>
+      <c r="D254" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E254" s="5" t="s">
+        <v>1035</v>
+      </c>
       <c r="F254" s="5"/>
-      <c r="G254" s="5"/>
+      <c r="G254" s="5" t="s">
+        <v>1052</v>
+      </c>
       <c r="H254" s="5"/>
       <c r="I254" s="5"/>
       <c r="J254" s="5"/>
-      <c r="K254" s="5"/>
-      <c r="L254" s="5"/>
+      <c r="K254" s="5">
+        <v>1</v>
+      </c>
+      <c r="L254" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M254" s="5"/>
     </row>
     <row r="255" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B255" s="2"/>
-      <c r="C255" s="3"/>
-      <c r="D255" s="5"/>
-      <c r="E255" s="5"/>
+      <c r="B255" s="2">
+        <v>251</v>
+      </c>
+      <c r="C255" s="3">
+        <v>43528</v>
+      </c>
+      <c r="D255" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E255" s="5" t="s">
+        <v>1036</v>
+      </c>
       <c r="F255" s="5"/>
-      <c r="G255" s="5"/>
+      <c r="G255" s="5" t="s">
+        <v>1040</v>
+      </c>
       <c r="H255" s="5"/>
       <c r="I255" s="5"/>
       <c r="J255" s="5"/>
-      <c r="K255" s="5"/>
-      <c r="L255" s="5"/>
+      <c r="K255" s="5">
+        <v>1</v>
+      </c>
+      <c r="L255" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M255" s="5"/>
     </row>
     <row r="256" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B256" s="2"/>
-      <c r="C256" s="3"/>
-      <c r="D256" s="5"/>
-      <c r="E256" s="5"/>
+      <c r="B256" s="2">
+        <v>252</v>
+      </c>
+      <c r="C256" s="3">
+        <v>43528</v>
+      </c>
+      <c r="D256" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E256" s="5" t="s">
+        <v>1037</v>
+      </c>
       <c r="F256" s="5"/>
-      <c r="G256" s="5"/>
+      <c r="G256" s="5" t="s">
+        <v>1041</v>
+      </c>
       <c r="H256" s="5"/>
       <c r="I256" s="5"/>
       <c r="J256" s="5"/>
-      <c r="K256" s="5"/>
-      <c r="L256" s="5"/>
+      <c r="K256" s="5">
+        <v>1</v>
+      </c>
+      <c r="L256" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M256" s="5"/>
     </row>
     <row r="257" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B257" s="2"/>
-      <c r="C257" s="3"/>
-      <c r="D257" s="5"/>
-      <c r="E257" s="5"/>
+      <c r="B257" s="2">
+        <v>253</v>
+      </c>
+      <c r="C257" s="3">
+        <v>43528</v>
+      </c>
+      <c r="D257" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E257" s="5" t="s">
+        <v>1038</v>
+      </c>
       <c r="F257" s="5"/>
-      <c r="G257" s="5"/>
+      <c r="G257" s="5" t="s">
+        <v>1042</v>
+      </c>
       <c r="H257" s="5"/>
       <c r="I257" s="5"/>
       <c r="J257" s="5"/>
-      <c r="K257" s="5"/>
-      <c r="L257" s="5"/>
+      <c r="K257" s="5">
+        <v>1</v>
+      </c>
+      <c r="L257" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M257" s="5"/>
     </row>
     <row r="258" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B258" s="2"/>
-      <c r="C258" s="3"/>
-      <c r="D258" s="5"/>
-      <c r="E258" s="5"/>
+      <c r="B258" s="2">
+        <v>254</v>
+      </c>
+      <c r="C258" s="3">
+        <v>43528</v>
+      </c>
+      <c r="D258" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E258" s="5" t="s">
+        <v>1039</v>
+      </c>
       <c r="F258" s="5"/>
-      <c r="G258" s="5"/>
+      <c r="G258" s="5" t="s">
+        <v>1043</v>
+      </c>
       <c r="H258" s="5"/>
       <c r="I258" s="5"/>
       <c r="J258" s="5"/>
-      <c r="K258" s="5"/>
-      <c r="L258" s="5"/>
+      <c r="K258" s="5">
+        <v>1</v>
+      </c>
+      <c r="L258" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M258" s="5"/>
     </row>
     <row r="259" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B259" s="2"/>
-      <c r="C259" s="3"/>
-      <c r="D259" s="5"/>
-      <c r="E259" s="5"/>
+      <c r="B259" s="2">
+        <v>255</v>
+      </c>
+      <c r="C259" s="3">
+        <v>43529</v>
+      </c>
+      <c r="D259" s="5" t="s">
+        <v>1056</v>
+      </c>
+      <c r="E259" s="5" t="s">
+        <v>1053</v>
+      </c>
       <c r="F259" s="5"/>
-      <c r="G259" s="5"/>
-      <c r="H259" s="5"/>
+      <c r="G259" s="5" t="s">
+        <v>1054</v>
+      </c>
+      <c r="H259" s="5" t="s">
+        <v>1055</v>
+      </c>
       <c r="I259" s="5"/>
       <c r="J259" s="5"/>
-      <c r="K259" s="5"/>
-      <c r="L259" s="5"/>
+      <c r="K259" s="5">
+        <v>1</v>
+      </c>
+      <c r="L259" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M259" s="5"/>
     </row>
     <row r="260" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B260" s="2"/>
-      <c r="C260" s="3"/>
-      <c r="D260" s="5"/>
-      <c r="E260" s="5"/>
+      <c r="B260" s="2">
+        <v>256</v>
+      </c>
+      <c r="C260" s="3">
+        <v>43529</v>
+      </c>
+      <c r="D260" s="5" t="s">
+        <v>1056</v>
+      </c>
+      <c r="E260" s="5" t="s">
+        <v>1057</v>
+      </c>
       <c r="F260" s="5"/>
-      <c r="G260" s="5"/>
+      <c r="G260" s="5" t="s">
+        <v>1060</v>
+      </c>
       <c r="H260" s="5"/>
       <c r="I260" s="5"/>
       <c r="J260" s="5"/>
-      <c r="K260" s="5"/>
-      <c r="L260" s="5"/>
+      <c r="K260" s="5">
+        <v>1</v>
+      </c>
+      <c r="L260" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M260" s="5"/>
     </row>
     <row r="261" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B261" s="2"/>
-      <c r="C261" s="3"/>
-      <c r="D261" s="5"/>
-      <c r="E261" s="5"/>
+      <c r="B261" s="2">
+        <v>257</v>
+      </c>
+      <c r="C261" s="3">
+        <v>43529</v>
+      </c>
+      <c r="D261" s="5" t="s">
+        <v>1056</v>
+      </c>
+      <c r="E261" s="5" t="s">
+        <v>1058</v>
+      </c>
       <c r="F261" s="5"/>
-      <c r="G261" s="5"/>
+      <c r="G261" s="5" t="s">
+        <v>1061</v>
+      </c>
       <c r="H261" s="5"/>
       <c r="I261" s="5"/>
       <c r="J261" s="5"/>
-      <c r="K261" s="5"/>
-      <c r="L261" s="5"/>
+      <c r="K261" s="5">
+        <v>1</v>
+      </c>
+      <c r="L261" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M261" s="5"/>
     </row>
     <row r="262" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B262" s="2"/>
-      <c r="C262" s="3"/>
-      <c r="D262" s="5"/>
-      <c r="E262" s="5"/>
+      <c r="B262" s="2">
+        <v>258</v>
+      </c>
+      <c r="C262" s="3">
+        <v>43529</v>
+      </c>
+      <c r="D262" s="5" t="s">
+        <v>1056</v>
+      </c>
+      <c r="E262" s="5" t="s">
+        <v>1059</v>
+      </c>
       <c r="F262" s="5"/>
-      <c r="G262" s="5"/>
-      <c r="H262" s="5"/>
+      <c r="G262" s="5" t="s">
+        <v>1062</v>
+      </c>
+      <c r="H262" s="5" t="s">
+        <v>1063</v>
+      </c>
       <c r="I262" s="5"/>
       <c r="J262" s="5"/>
-      <c r="K262" s="5"/>
-      <c r="L262" s="5"/>
+      <c r="K262" s="5">
+        <v>1</v>
+      </c>
+      <c r="L262" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M262" s="5"/>
     </row>
     <row r="263" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B263" s="2"/>
-      <c r="C263" s="3"/>
-      <c r="D263" s="5"/>
-      <c r="E263" s="5"/>
+      <c r="B263" s="2">
+        <v>259</v>
+      </c>
+      <c r="C263" s="3">
+        <v>43529</v>
+      </c>
+      <c r="D263" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E263" s="5" t="s">
+        <v>1064</v>
+      </c>
       <c r="F263" s="5"/>
-      <c r="G263" s="5"/>
+      <c r="G263" s="5" t="s">
+        <v>1082</v>
+      </c>
       <c r="H263" s="5"/>
       <c r="I263" s="5"/>
       <c r="J263" s="5"/>
-      <c r="K263" s="5"/>
-      <c r="L263" s="5"/>
+      <c r="K263" s="5">
+        <v>1</v>
+      </c>
+      <c r="L263" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M263" s="5"/>
     </row>
     <row r="264" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B264" s="2"/>
-      <c r="C264" s="3"/>
-      <c r="D264" s="5"/>
-      <c r="E264" s="5"/>
+      <c r="B264" s="2">
+        <v>260</v>
+      </c>
+      <c r="C264" s="3">
+        <v>43529</v>
+      </c>
+      <c r="D264" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E264" s="5" t="s">
+        <v>1065</v>
+      </c>
       <c r="F264" s="5"/>
-      <c r="G264" s="5"/>
+      <c r="G264" s="5" t="s">
+        <v>1083</v>
+      </c>
       <c r="H264" s="5"/>
       <c r="I264" s="5"/>
       <c r="J264" s="5"/>
-      <c r="K264" s="5"/>
-      <c r="L264" s="5"/>
+      <c r="K264" s="5">
+        <v>1</v>
+      </c>
+      <c r="L264" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M264" s="5"/>
     </row>
     <row r="265" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B265" s="2"/>
-      <c r="C265" s="3"/>
-      <c r="D265" s="5"/>
-      <c r="E265" s="5"/>
+      <c r="B265" s="2">
+        <v>261</v>
+      </c>
+      <c r="C265" s="3">
+        <v>43529</v>
+      </c>
+      <c r="D265" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E265" s="5" t="s">
+        <v>1066</v>
+      </c>
       <c r="F265" s="5"/>
-      <c r="G265" s="5"/>
+      <c r="G265" s="5" t="s">
+        <v>1084</v>
+      </c>
       <c r="H265" s="5"/>
       <c r="I265" s="5"/>
       <c r="J265" s="5"/>
-      <c r="K265" s="5"/>
-      <c r="L265" s="5"/>
+      <c r="K265" s="5">
+        <v>1</v>
+      </c>
+      <c r="L265" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M265" s="5"/>
     </row>
     <row r="266" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B266" s="2"/>
-      <c r="C266" s="3"/>
-      <c r="D266" s="5"/>
-      <c r="E266" s="5"/>
+      <c r="B266" s="2">
+        <v>262</v>
+      </c>
+      <c r="C266" s="3">
+        <v>43529</v>
+      </c>
+      <c r="D266" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E266" s="5" t="s">
+        <v>1067</v>
+      </c>
       <c r="F266" s="5"/>
-      <c r="G266" s="5"/>
+      <c r="G266" s="5" t="s">
+        <v>1085</v>
+      </c>
       <c r="H266" s="5"/>
       <c r="I266" s="5"/>
       <c r="J266" s="5"/>
-      <c r="K266" s="5"/>
-      <c r="L266" s="5"/>
+      <c r="K266" s="5">
+        <v>1</v>
+      </c>
+      <c r="L266" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M266" s="5"/>
     </row>
     <row r="267" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B267" s="2"/>
-      <c r="C267" s="3"/>
-      <c r="D267" s="5"/>
-      <c r="E267" s="5"/>
+      <c r="B267" s="2">
+        <v>263</v>
+      </c>
+      <c r="C267" s="3">
+        <v>43529</v>
+      </c>
+      <c r="D267" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E267" s="5" t="s">
+        <v>1068</v>
+      </c>
       <c r="F267" s="5"/>
-      <c r="G267" s="5"/>
+      <c r="G267" s="5" t="s">
+        <v>1086</v>
+      </c>
       <c r="H267" s="5"/>
       <c r="I267" s="5"/>
       <c r="J267" s="5"/>
-      <c r="K267" s="5"/>
-      <c r="L267" s="5"/>
+      <c r="K267" s="5">
+        <v>1</v>
+      </c>
+      <c r="L267" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M267" s="5"/>
     </row>
     <row r="268" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B268" s="2"/>
-      <c r="C268" s="3"/>
-      <c r="D268" s="5"/>
-      <c r="E268" s="5"/>
+      <c r="B268" s="2">
+        <v>264</v>
+      </c>
+      <c r="C268" s="3">
+        <v>43529</v>
+      </c>
+      <c r="D268" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E268" s="5" t="s">
+        <v>1069</v>
+      </c>
       <c r="F268" s="5"/>
-      <c r="G268" s="5"/>
+      <c r="G268" s="5" t="s">
+        <v>1087</v>
+      </c>
       <c r="H268" s="5"/>
       <c r="I268" s="5"/>
       <c r="J268" s="5"/>
-      <c r="K268" s="5"/>
-      <c r="L268" s="5"/>
+      <c r="K268" s="5">
+        <v>1</v>
+      </c>
+      <c r="L268" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M268" s="5"/>
     </row>
     <row r="269" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B269" s="2"/>
-      <c r="C269" s="3"/>
-      <c r="D269" s="5"/>
-      <c r="E269" s="5"/>
+      <c r="B269" s="2">
+        <v>265</v>
+      </c>
+      <c r="C269" s="3">
+        <v>43529</v>
+      </c>
+      <c r="D269" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E269" s="5" t="s">
+        <v>1070</v>
+      </c>
       <c r="F269" s="5"/>
-      <c r="G269" s="5"/>
+      <c r="G269" s="5" t="s">
+        <v>1088</v>
+      </c>
       <c r="H269" s="5"/>
       <c r="I269" s="5"/>
       <c r="J269" s="5"/>
-      <c r="K269" s="5"/>
-      <c r="L269" s="5"/>
+      <c r="K269" s="5">
+        <v>1</v>
+      </c>
+      <c r="L269" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M269" s="5"/>
     </row>
     <row r="270" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B270" s="2"/>
-      <c r="C270" s="3"/>
-      <c r="D270" s="5"/>
-      <c r="E270" s="5"/>
+      <c r="B270" s="2">
+        <v>266</v>
+      </c>
+      <c r="C270" s="3">
+        <v>43529</v>
+      </c>
+      <c r="D270" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E270" s="5" t="s">
+        <v>1071</v>
+      </c>
       <c r="F270" s="5"/>
-      <c r="G270" s="5"/>
+      <c r="G270" s="5" t="s">
+        <v>1089</v>
+      </c>
       <c r="H270" s="5"/>
       <c r="I270" s="5"/>
       <c r="J270" s="5"/>
-      <c r="K270" s="5"/>
-      <c r="L270" s="5"/>
+      <c r="K270" s="5">
+        <v>1</v>
+      </c>
+      <c r="L270" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M270" s="5"/>
     </row>
     <row r="271" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B271" s="2"/>
-      <c r="C271" s="3"/>
-      <c r="D271" s="5"/>
-      <c r="E271" s="5"/>
+      <c r="B271" s="2">
+        <v>267</v>
+      </c>
+      <c r="C271" s="3">
+        <v>43529</v>
+      </c>
+      <c r="D271" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E271" s="5" t="s">
+        <v>1072</v>
+      </c>
       <c r="F271" s="5"/>
-      <c r="G271" s="5"/>
+      <c r="G271" s="5" t="s">
+        <v>1090</v>
+      </c>
       <c r="H271" s="5"/>
       <c r="I271" s="5"/>
       <c r="J271" s="5"/>
-      <c r="K271" s="5"/>
-      <c r="L271" s="5"/>
+      <c r="K271" s="5">
+        <v>1</v>
+      </c>
+      <c r="L271" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M271" s="5"/>
     </row>
     <row r="272" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B272" s="2"/>
-      <c r="C272" s="3"/>
-      <c r="D272" s="5"/>
-      <c r="E272" s="5"/>
+      <c r="B272" s="2">
+        <v>268</v>
+      </c>
+      <c r="C272" s="3">
+        <v>43529</v>
+      </c>
+      <c r="D272" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E272" s="5" t="s">
+        <v>1073</v>
+      </c>
       <c r="F272" s="5"/>
-      <c r="G272" s="5"/>
+      <c r="G272" s="5" t="s">
+        <v>1091</v>
+      </c>
       <c r="H272" s="5"/>
       <c r="I272" s="5"/>
       <c r="J272" s="5"/>
-      <c r="K272" s="5"/>
-      <c r="L272" s="5"/>
+      <c r="K272" s="5">
+        <v>1</v>
+      </c>
+      <c r="L272" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M272" s="5"/>
     </row>
     <row r="273" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B273" s="2"/>
-      <c r="C273" s="3"/>
-      <c r="D273" s="5"/>
-      <c r="E273" s="5"/>
+      <c r="B273" s="2">
+        <v>269</v>
+      </c>
+      <c r="C273" s="3">
+        <v>43529</v>
+      </c>
+      <c r="D273" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E273" s="5" t="s">
+        <v>1074</v>
+      </c>
       <c r="F273" s="5"/>
-      <c r="G273" s="5"/>
+      <c r="G273" s="5" t="s">
+        <v>1092</v>
+      </c>
       <c r="H273" s="5"/>
       <c r="I273" s="5"/>
       <c r="J273" s="5"/>
-      <c r="K273" s="5"/>
-      <c r="L273" s="5"/>
+      <c r="K273" s="5">
+        <v>1</v>
+      </c>
+      <c r="L273" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M273" s="5"/>
     </row>
     <row r="274" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B274" s="2"/>
-      <c r="C274" s="3"/>
-      <c r="D274" s="5"/>
-      <c r="E274" s="5"/>
+      <c r="B274" s="2">
+        <v>270</v>
+      </c>
+      <c r="C274" s="3">
+        <v>43529</v>
+      </c>
+      <c r="D274" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E274" s="5" t="s">
+        <v>1075</v>
+      </c>
       <c r="F274" s="5"/>
-      <c r="G274" s="5"/>
+      <c r="G274" s="5" t="s">
+        <v>1093</v>
+      </c>
       <c r="H274" s="5"/>
       <c r="I274" s="5"/>
       <c r="J274" s="5"/>
-      <c r="K274" s="5"/>
-      <c r="L274" s="5"/>
+      <c r="K274" s="5">
+        <v>1</v>
+      </c>
+      <c r="L274" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M274" s="5"/>
     </row>
     <row r="275" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B275" s="2"/>
-      <c r="C275" s="3"/>
-      <c r="D275" s="5"/>
-      <c r="E275" s="5"/>
+      <c r="B275" s="2">
+        <v>271</v>
+      </c>
+      <c r="C275" s="3">
+        <v>43529</v>
+      </c>
+      <c r="D275" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E275" s="5" t="s">
+        <v>1076</v>
+      </c>
       <c r="F275" s="5"/>
-      <c r="G275" s="5"/>
+      <c r="G275" s="5" t="s">
+        <v>1094</v>
+      </c>
       <c r="H275" s="5"/>
       <c r="I275" s="5"/>
       <c r="J275" s="5"/>
-      <c r="K275" s="5"/>
-      <c r="L275" s="5"/>
+      <c r="K275" s="5">
+        <v>1</v>
+      </c>
+      <c r="L275" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M275" s="5"/>
     </row>
     <row r="276" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B276" s="2"/>
-      <c r="C276" s="3"/>
-      <c r="D276" s="5"/>
-      <c r="E276" s="5"/>
+      <c r="B276" s="2">
+        <v>272</v>
+      </c>
+      <c r="C276" s="3">
+        <v>43529</v>
+      </c>
+      <c r="D276" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E276" s="5" t="s">
+        <v>1077</v>
+      </c>
       <c r="F276" s="5"/>
-      <c r="G276" s="5"/>
+      <c r="G276" s="5" t="s">
+        <v>1095</v>
+      </c>
       <c r="H276" s="5"/>
       <c r="I276" s="5"/>
       <c r="J276" s="5"/>
-      <c r="K276" s="5"/>
-      <c r="L276" s="5"/>
+      <c r="K276" s="5">
+        <v>1</v>
+      </c>
+      <c r="L276" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M276" s="5"/>
     </row>
     <row r="277" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B277" s="2"/>
-      <c r="C277" s="3"/>
-      <c r="D277" s="5"/>
-      <c r="E277" s="5"/>
+      <c r="B277" s="2">
+        <v>273</v>
+      </c>
+      <c r="C277" s="3">
+        <v>43529</v>
+      </c>
+      <c r="D277" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E277" s="5" t="s">
+        <v>1078</v>
+      </c>
       <c r="F277" s="5"/>
-      <c r="G277" s="5"/>
+      <c r="G277" s="5" t="s">
+        <v>1096</v>
+      </c>
       <c r="H277" s="5"/>
       <c r="I277" s="5"/>
       <c r="J277" s="5"/>
-      <c r="K277" s="5"/>
-      <c r="L277" s="5"/>
+      <c r="K277" s="5">
+        <v>1</v>
+      </c>
+      <c r="L277" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M277" s="5"/>
     </row>
     <row r="278" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B278" s="2"/>
-      <c r="C278" s="3"/>
-      <c r="D278" s="5"/>
-      <c r="E278" s="5"/>
+      <c r="B278" s="2">
+        <v>274</v>
+      </c>
+      <c r="C278" s="3">
+        <v>43529</v>
+      </c>
+      <c r="D278" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E278" s="5" t="s">
+        <v>1079</v>
+      </c>
       <c r="F278" s="5"/>
-      <c r="G278" s="5"/>
+      <c r="G278" s="5" t="s">
+        <v>1097</v>
+      </c>
       <c r="H278" s="5"/>
       <c r="I278" s="5"/>
       <c r="J278" s="5"/>
-      <c r="K278" s="5"/>
-      <c r="L278" s="5"/>
+      <c r="K278" s="5">
+        <v>1</v>
+      </c>
+      <c r="L278" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M278" s="5"/>
     </row>
     <row r="279" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B279" s="2"/>
-      <c r="C279" s="3"/>
-      <c r="D279" s="5"/>
-      <c r="E279" s="5"/>
+      <c r="B279" s="2">
+        <v>275</v>
+      </c>
+      <c r="C279" s="3">
+        <v>43529</v>
+      </c>
+      <c r="D279" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E279" s="5" t="s">
+        <v>1080</v>
+      </c>
       <c r="F279" s="5"/>
-      <c r="G279" s="5"/>
+      <c r="G279" s="5" t="s">
+        <v>1098</v>
+      </c>
       <c r="H279" s="5"/>
       <c r="I279" s="5"/>
       <c r="J279" s="5"/>
-      <c r="K279" s="5"/>
-      <c r="L279" s="5"/>
+      <c r="K279" s="5">
+        <v>1</v>
+      </c>
+      <c r="L279" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M279" s="5"/>
     </row>
     <row r="280" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B280" s="2"/>
-      <c r="C280" s="3"/>
-      <c r="D280" s="5"/>
-      <c r="E280" s="5"/>
+      <c r="B280" s="2">
+        <v>276</v>
+      </c>
+      <c r="C280" s="3">
+        <v>43529</v>
+      </c>
+      <c r="D280" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E280" s="5" t="s">
+        <v>1081</v>
+      </c>
       <c r="F280" s="5"/>
-      <c r="G280" s="5"/>
+      <c r="G280" s="5" t="s">
+        <v>1099</v>
+      </c>
       <c r="H280" s="5"/>
       <c r="I280" s="5"/>
       <c r="J280" s="5"/>
-      <c r="K280" s="5"/>
-      <c r="L280" s="5"/>
+      <c r="K280" s="5">
+        <v>1</v>
+      </c>
+      <c r="L280" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M280" s="5"/>
     </row>
     <row r="281" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
@@ -14264,11 +15054,11 @@
   <mergeCells count="1">
     <mergeCell ref="B2:L2"/>
   </mergeCells>
-  <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D115 D242:D1048576">
+  <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D115 D281:D1048576">
       <formula1>"Likeshuo,TOEFL,TPO"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D116:D241">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D116:D257">
       <formula1>"Likeshuo,TOEFL,TPO, 500 setns"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L5:L520">
@@ -14276,6 +15066,9 @@
     </dataValidation>
     <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C520">
       <formula1>43508</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D258:D280">
+      <formula1>"Likeshuo,TOEFL,TPO, 500 setns, NCE4"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
english_learning Vocabulary Statistic Chart updated
</commit_message>
<xml_diff>
--- a/english_learning/Vocabulary Statistic Chart for TOEFL.xlsx
+++ b/english_learning/Vocabulary Statistic Chart for TOEFL.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2241" uniqueCount="1100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2329" uniqueCount="1143">
   <si>
     <t>Expression</t>
   </si>
@@ -3330,6 +3330,135 @@
   </si>
   <si>
     <t>进行</t>
+  </si>
+  <si>
+    <t>fraud</t>
+  </si>
+  <si>
+    <t>coercion</t>
+  </si>
+  <si>
+    <t>deceive</t>
+  </si>
+  <si>
+    <t>burglar</t>
+  </si>
+  <si>
+    <t>burglary</t>
+  </si>
+  <si>
+    <t>intent</t>
+  </si>
+  <si>
+    <t>plainclothes police officer</t>
+  </si>
+  <si>
+    <t>charge</t>
+  </si>
+  <si>
+    <t>impetuous</t>
+  </si>
+  <si>
+    <t>offense</t>
+  </si>
+  <si>
+    <t>stab</t>
+  </si>
+  <si>
+    <t>stabbed</t>
+  </si>
+  <si>
+    <t>strict</t>
+  </si>
+  <si>
+    <t>rigidly</t>
+  </si>
+  <si>
+    <t>deviation</t>
+  </si>
+  <si>
+    <t>follow the tracks of</t>
+  </si>
+  <si>
+    <t>fine</t>
+  </si>
+  <si>
+    <t>something you have to pay</t>
+  </si>
+  <si>
+    <t>smuggler</t>
+  </si>
+  <si>
+    <t>lucrative</t>
+  </si>
+  <si>
+    <t>covert</t>
+  </si>
+  <si>
+    <t>hidden</t>
+  </si>
+  <si>
+    <t>骗局</t>
+  </si>
+  <si>
+    <t>强迫</t>
+  </si>
+  <si>
+    <t>欺骗</t>
+  </si>
+  <si>
+    <t>窃贼</t>
+  </si>
+  <si>
+    <t>窃案</t>
+  </si>
+  <si>
+    <t>意图</t>
+  </si>
+  <si>
+    <t>便衣警察</t>
+  </si>
+  <si>
+    <t>收费</t>
+  </si>
+  <si>
+    <t>浮躁</t>
+  </si>
+  <si>
+    <t>罪行</t>
+  </si>
+  <si>
+    <t>刺</t>
+  </si>
+  <si>
+    <t>被刺</t>
+  </si>
+  <si>
+    <t>严格</t>
+  </si>
+  <si>
+    <t>偏差</t>
+  </si>
+  <si>
+    <t>按照轨道</t>
+  </si>
+  <si>
+    <t>精细</t>
+  </si>
+  <si>
+    <t>你需要支付的东西</t>
+  </si>
+  <si>
+    <t>走私者</t>
+  </si>
+  <si>
+    <t>有利可图</t>
+  </si>
+  <si>
+    <t>隐蔽</t>
+  </si>
+  <si>
+    <t>隐</t>
   </si>
 </sst>
 </file>
@@ -3785,8 +3914,8 @@
   <dimension ref="B1:M520"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A261" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E274" sqref="E274"/>
+      <pane ySplit="4" topLeftCell="A291" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F294" sqref="F294"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
@@ -11690,311 +11819,619 @@
       <c r="M280" s="5"/>
     </row>
     <row r="281" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B281" s="2"/>
-      <c r="C281" s="3"/>
-      <c r="D281" s="5"/>
-      <c r="E281" s="5"/>
+      <c r="B281" s="2">
+        <v>277</v>
+      </c>
+      <c r="C281" s="3">
+        <v>43531</v>
+      </c>
+      <c r="D281" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E281" s="5" t="s">
+        <v>1100</v>
+      </c>
       <c r="F281" s="5"/>
-      <c r="G281" s="5"/>
+      <c r="G281" s="5" t="s">
+        <v>1122</v>
+      </c>
       <c r="H281" s="5"/>
       <c r="I281" s="5"/>
       <c r="J281" s="5"/>
-      <c r="K281" s="5"/>
-      <c r="L281" s="5"/>
+      <c r="K281" s="5">
+        <v>1</v>
+      </c>
+      <c r="L281" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M281" s="5"/>
     </row>
     <row r="282" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B282" s="2"/>
-      <c r="C282" s="3"/>
-      <c r="D282" s="5"/>
-      <c r="E282" s="5"/>
+      <c r="B282" s="2">
+        <v>278</v>
+      </c>
+      <c r="C282" s="3">
+        <v>43531</v>
+      </c>
+      <c r="D282" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E282" s="5" t="s">
+        <v>1101</v>
+      </c>
       <c r="F282" s="5"/>
-      <c r="G282" s="5"/>
+      <c r="G282" s="5" t="s">
+        <v>1123</v>
+      </c>
       <c r="H282" s="5"/>
       <c r="I282" s="5"/>
       <c r="J282" s="5"/>
-      <c r="K282" s="5"/>
-      <c r="L282" s="5"/>
+      <c r="K282" s="5">
+        <v>1</v>
+      </c>
+      <c r="L282" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M282" s="5"/>
     </row>
     <row r="283" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B283" s="2"/>
-      <c r="C283" s="3"/>
-      <c r="D283" s="5"/>
-      <c r="E283" s="5"/>
+      <c r="B283" s="2">
+        <v>279</v>
+      </c>
+      <c r="C283" s="3">
+        <v>43531</v>
+      </c>
+      <c r="D283" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E283" s="5" t="s">
+        <v>1102</v>
+      </c>
       <c r="F283" s="5"/>
-      <c r="G283" s="5"/>
+      <c r="G283" s="5" t="s">
+        <v>1124</v>
+      </c>
       <c r="H283" s="5"/>
       <c r="I283" s="5"/>
       <c r="J283" s="5"/>
-      <c r="K283" s="5"/>
-      <c r="L283" s="5"/>
+      <c r="K283" s="5">
+        <v>1</v>
+      </c>
+      <c r="L283" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M283" s="5"/>
     </row>
     <row r="284" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B284" s="2"/>
-      <c r="C284" s="3"/>
-      <c r="D284" s="5"/>
-      <c r="E284" s="5"/>
+      <c r="B284" s="2">
+        <v>280</v>
+      </c>
+      <c r="C284" s="3">
+        <v>43531</v>
+      </c>
+      <c r="D284" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E284" s="5" t="s">
+        <v>1103</v>
+      </c>
       <c r="F284" s="5"/>
-      <c r="G284" s="5"/>
+      <c r="G284" s="5" t="s">
+        <v>1125</v>
+      </c>
       <c r="H284" s="5"/>
       <c r="I284" s="5"/>
       <c r="J284" s="5"/>
-      <c r="K284" s="5"/>
-      <c r="L284" s="5"/>
+      <c r="K284" s="5">
+        <v>1</v>
+      </c>
+      <c r="L284" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M284" s="5"/>
     </row>
     <row r="285" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B285" s="2"/>
-      <c r="C285" s="3"/>
-      <c r="D285" s="5"/>
-      <c r="E285" s="5"/>
+      <c r="B285" s="2">
+        <v>281</v>
+      </c>
+      <c r="C285" s="3">
+        <v>43531</v>
+      </c>
+      <c r="D285" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E285" s="5" t="s">
+        <v>1104</v>
+      </c>
       <c r="F285" s="5"/>
-      <c r="G285" s="5"/>
+      <c r="G285" s="5" t="s">
+        <v>1126</v>
+      </c>
       <c r="H285" s="5"/>
       <c r="I285" s="5"/>
       <c r="J285" s="5"/>
-      <c r="K285" s="5"/>
-      <c r="L285" s="5"/>
+      <c r="K285" s="5">
+        <v>1</v>
+      </c>
+      <c r="L285" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M285" s="5"/>
     </row>
     <row r="286" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B286" s="2"/>
-      <c r="C286" s="3"/>
-      <c r="D286" s="5"/>
-      <c r="E286" s="5"/>
+      <c r="B286" s="2">
+        <v>282</v>
+      </c>
+      <c r="C286" s="3">
+        <v>43531</v>
+      </c>
+      <c r="D286" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E286" s="5" t="s">
+        <v>1105</v>
+      </c>
       <c r="F286" s="5"/>
-      <c r="G286" s="5"/>
+      <c r="G286" s="5" t="s">
+        <v>1127</v>
+      </c>
       <c r="H286" s="5"/>
       <c r="I286" s="5"/>
       <c r="J286" s="5"/>
-      <c r="K286" s="5"/>
-      <c r="L286" s="5"/>
+      <c r="K286" s="5">
+        <v>1</v>
+      </c>
+      <c r="L286" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M286" s="5"/>
     </row>
     <row r="287" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B287" s="2"/>
-      <c r="C287" s="3"/>
-      <c r="D287" s="5"/>
-      <c r="E287" s="5"/>
+      <c r="B287" s="2">
+        <v>283</v>
+      </c>
+      <c r="C287" s="3">
+        <v>43531</v>
+      </c>
+      <c r="D287" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E287" s="5" t="s">
+        <v>1106</v>
+      </c>
       <c r="F287" s="5"/>
-      <c r="G287" s="5"/>
+      <c r="G287" s="5" t="s">
+        <v>1128</v>
+      </c>
       <c r="H287" s="5"/>
       <c r="I287" s="5"/>
       <c r="J287" s="5"/>
-      <c r="K287" s="5"/>
-      <c r="L287" s="5"/>
+      <c r="K287" s="5">
+        <v>1</v>
+      </c>
+      <c r="L287" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M287" s="5"/>
     </row>
     <row r="288" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B288" s="2"/>
-      <c r="C288" s="3"/>
-      <c r="D288" s="5"/>
-      <c r="E288" s="5"/>
+      <c r="B288" s="2">
+        <v>284</v>
+      </c>
+      <c r="C288" s="3">
+        <v>43531</v>
+      </c>
+      <c r="D288" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E288" s="5" t="s">
+        <v>1107</v>
+      </c>
       <c r="F288" s="5"/>
-      <c r="G288" s="5"/>
+      <c r="G288" s="5" t="s">
+        <v>1129</v>
+      </c>
       <c r="H288" s="5"/>
       <c r="I288" s="5"/>
       <c r="J288" s="5"/>
-      <c r="K288" s="5"/>
-      <c r="L288" s="5"/>
+      <c r="K288" s="5">
+        <v>1</v>
+      </c>
+      <c r="L288" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M288" s="5"/>
     </row>
     <row r="289" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B289" s="2"/>
-      <c r="C289" s="3"/>
-      <c r="D289" s="5"/>
-      <c r="E289" s="5"/>
+      <c r="B289" s="2">
+        <v>285</v>
+      </c>
+      <c r="C289" s="3">
+        <v>43531</v>
+      </c>
+      <c r="D289" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E289" s="5" t="s">
+        <v>1108</v>
+      </c>
       <c r="F289" s="5"/>
-      <c r="G289" s="5"/>
+      <c r="G289" s="5" t="s">
+        <v>1130</v>
+      </c>
       <c r="H289" s="5"/>
       <c r="I289" s="5"/>
       <c r="J289" s="5"/>
-      <c r="K289" s="5"/>
-      <c r="L289" s="5"/>
+      <c r="K289" s="5">
+        <v>1</v>
+      </c>
+      <c r="L289" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M289" s="5"/>
     </row>
     <row r="290" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B290" s="2"/>
-      <c r="C290" s="3"/>
-      <c r="D290" s="5"/>
-      <c r="E290" s="5"/>
+      <c r="B290" s="2">
+        <v>286</v>
+      </c>
+      <c r="C290" s="3">
+        <v>43531</v>
+      </c>
+      <c r="D290" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E290" s="5" t="s">
+        <v>1109</v>
+      </c>
       <c r="F290" s="5"/>
-      <c r="G290" s="5"/>
+      <c r="G290" s="5" t="s">
+        <v>1131</v>
+      </c>
       <c r="H290" s="5"/>
       <c r="I290" s="5"/>
       <c r="J290" s="5"/>
-      <c r="K290" s="5"/>
-      <c r="L290" s="5"/>
+      <c r="K290" s="5">
+        <v>1</v>
+      </c>
+      <c r="L290" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M290" s="5"/>
     </row>
     <row r="291" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B291" s="2"/>
-      <c r="C291" s="3"/>
-      <c r="D291" s="5"/>
-      <c r="E291" s="5"/>
+      <c r="B291" s="2">
+        <v>287</v>
+      </c>
+      <c r="C291" s="3">
+        <v>43531</v>
+      </c>
+      <c r="D291" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E291" s="5" t="s">
+        <v>1110</v>
+      </c>
       <c r="F291" s="5"/>
-      <c r="G291" s="5"/>
+      <c r="G291" s="5" t="s">
+        <v>1132</v>
+      </c>
       <c r="H291" s="5"/>
       <c r="I291" s="5"/>
       <c r="J291" s="5"/>
-      <c r="K291" s="5"/>
-      <c r="L291" s="5"/>
+      <c r="K291" s="5">
+        <v>1</v>
+      </c>
+      <c r="L291" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M291" s="5"/>
     </row>
     <row r="292" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B292" s="2"/>
-      <c r="C292" s="3"/>
-      <c r="D292" s="5"/>
-      <c r="E292" s="5"/>
+      <c r="B292" s="2">
+        <v>288</v>
+      </c>
+      <c r="C292" s="3">
+        <v>43531</v>
+      </c>
+      <c r="D292" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E292" s="5" t="s">
+        <v>1111</v>
+      </c>
       <c r="F292" s="5"/>
-      <c r="G292" s="5"/>
+      <c r="G292" s="5" t="s">
+        <v>1133</v>
+      </c>
       <c r="H292" s="5"/>
       <c r="I292" s="5"/>
       <c r="J292" s="5"/>
-      <c r="K292" s="5"/>
-      <c r="L292" s="5"/>
+      <c r="K292" s="5">
+        <v>1</v>
+      </c>
+      <c r="L292" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M292" s="5"/>
     </row>
     <row r="293" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B293" s="2"/>
-      <c r="C293" s="3"/>
-      <c r="D293" s="5"/>
-      <c r="E293" s="5"/>
+      <c r="B293" s="2">
+        <v>289</v>
+      </c>
+      <c r="C293" s="3">
+        <v>43531</v>
+      </c>
+      <c r="D293" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E293" s="5" t="s">
+        <v>1112</v>
+      </c>
       <c r="F293" s="5"/>
-      <c r="G293" s="5"/>
+      <c r="G293" s="5" t="s">
+        <v>1134</v>
+      </c>
       <c r="H293" s="5"/>
       <c r="I293" s="5"/>
       <c r="J293" s="5"/>
-      <c r="K293" s="5"/>
-      <c r="L293" s="5"/>
+      <c r="K293" s="5">
+        <v>1</v>
+      </c>
+      <c r="L293" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M293" s="5"/>
     </row>
     <row r="294" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B294" s="2"/>
-      <c r="C294" s="3"/>
-      <c r="D294" s="5"/>
-      <c r="E294" s="5"/>
+      <c r="B294" s="2">
+        <v>290</v>
+      </c>
+      <c r="C294" s="3">
+        <v>43531</v>
+      </c>
+      <c r="D294" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E294" s="5" t="s">
+        <v>1113</v>
+      </c>
       <c r="F294" s="5"/>
-      <c r="G294" s="5"/>
+      <c r="G294" s="5" t="s">
+        <v>1134</v>
+      </c>
       <c r="H294" s="5"/>
       <c r="I294" s="5"/>
       <c r="J294" s="5"/>
-      <c r="K294" s="5"/>
-      <c r="L294" s="5"/>
+      <c r="K294" s="5">
+        <v>1</v>
+      </c>
+      <c r="L294" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M294" s="5"/>
     </row>
     <row r="295" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B295" s="2"/>
-      <c r="C295" s="3"/>
-      <c r="D295" s="5"/>
-      <c r="E295" s="5"/>
+      <c r="B295" s="2">
+        <v>291</v>
+      </c>
+      <c r="C295" s="3">
+        <v>43531</v>
+      </c>
+      <c r="D295" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E295" s="5" t="s">
+        <v>1114</v>
+      </c>
       <c r="F295" s="5"/>
-      <c r="G295" s="5"/>
+      <c r="G295" s="5" t="s">
+        <v>1135</v>
+      </c>
       <c r="H295" s="5"/>
       <c r="I295" s="5"/>
       <c r="J295" s="5"/>
-      <c r="K295" s="5"/>
-      <c r="L295" s="5"/>
+      <c r="K295" s="5">
+        <v>1</v>
+      </c>
+      <c r="L295" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M295" s="5"/>
     </row>
     <row r="296" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B296" s="2"/>
-      <c r="C296" s="3"/>
-      <c r="D296" s="5"/>
-      <c r="E296" s="5"/>
+      <c r="B296" s="2">
+        <v>292</v>
+      </c>
+      <c r="C296" s="3">
+        <v>43531</v>
+      </c>
+      <c r="D296" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E296" s="5" t="s">
+        <v>1115</v>
+      </c>
       <c r="F296" s="5"/>
-      <c r="G296" s="5"/>
+      <c r="G296" s="5" t="s">
+        <v>1136</v>
+      </c>
       <c r="H296" s="5"/>
       <c r="I296" s="5"/>
       <c r="J296" s="5"/>
-      <c r="K296" s="5"/>
-      <c r="L296" s="5"/>
+      <c r="K296" s="5">
+        <v>1</v>
+      </c>
+      <c r="L296" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M296" s="5"/>
     </row>
     <row r="297" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B297" s="2"/>
-      <c r="C297" s="3"/>
-      <c r="D297" s="5"/>
-      <c r="E297" s="5"/>
+      <c r="B297" s="2">
+        <v>293</v>
+      </c>
+      <c r="C297" s="3">
+        <v>43531</v>
+      </c>
+      <c r="D297" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E297" s="5" t="s">
+        <v>1116</v>
+      </c>
       <c r="F297" s="5"/>
-      <c r="G297" s="5"/>
+      <c r="G297" s="5" t="s">
+        <v>1137</v>
+      </c>
       <c r="H297" s="5"/>
       <c r="I297" s="5"/>
       <c r="J297" s="5"/>
-      <c r="K297" s="5"/>
-      <c r="L297" s="5"/>
+      <c r="K297" s="5">
+        <v>1</v>
+      </c>
+      <c r="L297" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M297" s="5"/>
     </row>
     <row r="298" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B298" s="2"/>
-      <c r="C298" s="3"/>
-      <c r="D298" s="5"/>
-      <c r="E298" s="5"/>
+      <c r="B298" s="2">
+        <v>294</v>
+      </c>
+      <c r="C298" s="3">
+        <v>43531</v>
+      </c>
+      <c r="D298" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E298" s="5" t="s">
+        <v>1117</v>
+      </c>
       <c r="F298" s="5"/>
-      <c r="G298" s="5"/>
+      <c r="G298" s="5" t="s">
+        <v>1138</v>
+      </c>
       <c r="H298" s="5"/>
       <c r="I298" s="5"/>
       <c r="J298" s="5"/>
-      <c r="K298" s="5"/>
-      <c r="L298" s="5"/>
+      <c r="K298" s="5">
+        <v>1</v>
+      </c>
+      <c r="L298" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M298" s="5"/>
     </row>
     <row r="299" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B299" s="2"/>
-      <c r="C299" s="3"/>
-      <c r="D299" s="5"/>
-      <c r="E299" s="5"/>
+      <c r="B299" s="2">
+        <v>295</v>
+      </c>
+      <c r="C299" s="3">
+        <v>43531</v>
+      </c>
+      <c r="D299" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E299" s="5" t="s">
+        <v>1118</v>
+      </c>
       <c r="F299" s="5"/>
-      <c r="G299" s="5"/>
+      <c r="G299" s="5" t="s">
+        <v>1139</v>
+      </c>
       <c r="H299" s="5"/>
       <c r="I299" s="5"/>
       <c r="J299" s="5"/>
-      <c r="K299" s="5"/>
-      <c r="L299" s="5"/>
+      <c r="K299" s="5">
+        <v>1</v>
+      </c>
+      <c r="L299" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M299" s="5"/>
     </row>
     <row r="300" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B300" s="2"/>
-      <c r="C300" s="3"/>
-      <c r="D300" s="5"/>
-      <c r="E300" s="5"/>
+      <c r="B300" s="2">
+        <v>296</v>
+      </c>
+      <c r="C300" s="3">
+        <v>43531</v>
+      </c>
+      <c r="D300" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E300" s="5" t="s">
+        <v>1119</v>
+      </c>
       <c r="F300" s="5"/>
-      <c r="G300" s="5"/>
+      <c r="G300" s="5" t="s">
+        <v>1140</v>
+      </c>
       <c r="H300" s="5"/>
       <c r="I300" s="5"/>
       <c r="J300" s="5"/>
-      <c r="K300" s="5"/>
-      <c r="L300" s="5"/>
+      <c r="K300" s="5">
+        <v>1</v>
+      </c>
+      <c r="L300" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M300" s="5"/>
     </row>
     <row r="301" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B301" s="2"/>
-      <c r="C301" s="3"/>
-      <c r="D301" s="5"/>
-      <c r="E301" s="5"/>
+      <c r="B301" s="2">
+        <v>297</v>
+      </c>
+      <c r="C301" s="3">
+        <v>43531</v>
+      </c>
+      <c r="D301" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E301" s="5" t="s">
+        <v>1120</v>
+      </c>
       <c r="F301" s="5"/>
-      <c r="G301" s="5"/>
+      <c r="G301" s="5" t="s">
+        <v>1141</v>
+      </c>
       <c r="H301" s="5"/>
       <c r="I301" s="5"/>
       <c r="J301" s="5"/>
-      <c r="K301" s="5"/>
-      <c r="L301" s="5"/>
+      <c r="K301" s="5">
+        <v>1</v>
+      </c>
+      <c r="L301" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M301" s="5"/>
     </row>
     <row r="302" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B302" s="2"/>
-      <c r="C302" s="3"/>
-      <c r="D302" s="5"/>
-      <c r="E302" s="5"/>
+      <c r="B302" s="2">
+        <v>298</v>
+      </c>
+      <c r="C302" s="3">
+        <v>43531</v>
+      </c>
+      <c r="D302" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E302" s="5" t="s">
+        <v>1121</v>
+      </c>
       <c r="F302" s="5"/>
-      <c r="G302" s="5"/>
+      <c r="G302" s="5" t="s">
+        <v>1142</v>
+      </c>
       <c r="H302" s="5"/>
       <c r="I302" s="5"/>
       <c r="J302" s="5"/>
-      <c r="K302" s="5"/>
-      <c r="L302" s="5"/>
+      <c r="K302" s="5">
+        <v>1</v>
+      </c>
+      <c r="L302" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M302" s="5"/>
     </row>
     <row r="303" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
@@ -15055,7 +15492,7 @@
     <mergeCell ref="B2:L2"/>
   </mergeCells>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D115 D281:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D115 D303:D1048576">
       <formula1>"Likeshuo,TOEFL,TPO"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D116:D257">
@@ -15067,7 +15504,7 @@
     <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C520">
       <formula1>43508</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D258:D280">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D258:D302">
       <formula1>"Likeshuo,TOEFL,TPO, 500 setns, NCE4"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
update english_learning Vocabulary Statistic Chart
</commit_message>
<xml_diff>
--- a/english_learning/Vocabulary Statistic Chart for TOEFL.xlsx
+++ b/english_learning/Vocabulary Statistic Chart for TOEFL.xlsx
@@ -16,7 +16,7 @@
     <sheet name="TOEFL" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">main!$B$4:$M$190</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">main!$B$4:$M$424</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">TOEFL!$B$4:$M$4</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2496" uniqueCount="1228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2828" uniqueCount="1391">
   <si>
     <t>Expression</t>
   </si>
@@ -3714,6 +3714,495 @@
   </si>
   <si>
     <t>continue in a course of action even in the face of difficulty or with little or no prospect of success.</t>
+  </si>
+  <si>
+    <t>prompt</t>
+  </si>
+  <si>
+    <t>thwart campus shootings</t>
+  </si>
+  <si>
+    <t>deterrent</t>
+  </si>
+  <si>
+    <t>in the wake of</t>
+  </si>
+  <si>
+    <t>offensive</t>
+  </si>
+  <si>
+    <t>surveillance camera</t>
+  </si>
+  <si>
+    <t>take an offensive stance against</t>
+  </si>
+  <si>
+    <t>allegation</t>
+  </si>
+  <si>
+    <t>mounting allegations</t>
+  </si>
+  <si>
+    <t>absurd</t>
+  </si>
+  <si>
+    <t>another offensive step towards incriminating videos games</t>
+  </si>
+  <si>
+    <t>incriminating</t>
+  </si>
+  <si>
+    <t>shifting blame</t>
+  </si>
+  <si>
+    <t>lenient gun laws</t>
+  </si>
+  <si>
+    <t>no offense</t>
+  </si>
+  <si>
+    <t>kitchen knife</t>
+  </si>
+  <si>
+    <t>wake after a boat:船的尾迹</t>
+  </si>
+  <si>
+    <t>事后</t>
+  </si>
+  <si>
+    <t>at length</t>
+  </si>
+  <si>
+    <t>at last</t>
+  </si>
+  <si>
+    <t>for a long time</t>
+  </si>
+  <si>
+    <t>提示</t>
+  </si>
+  <si>
+    <t>阻挠校园枪击事件</t>
+  </si>
+  <si>
+    <t>威慑</t>
+  </si>
+  <si>
+    <t>监控摄像头</t>
+  </si>
+  <si>
+    <t>采取进攻姿态反对</t>
+  </si>
+  <si>
+    <t>断言</t>
+  </si>
+  <si>
+    <t>越来越多的指控</t>
+  </si>
+  <si>
+    <t>荒诞</t>
+  </si>
+  <si>
+    <t>朝着控制视频游戏的另一个进攻步骤</t>
+  </si>
+  <si>
+    <t>罪证</t>
+  </si>
+  <si>
+    <t>转移责备</t>
+  </si>
+  <si>
+    <t>宽大的枪法</t>
+  </si>
+  <si>
+    <t>没有冒犯的意思</t>
+  </si>
+  <si>
+    <t>菜刀</t>
+  </si>
+  <si>
+    <t>adj 进攻</t>
+  </si>
+  <si>
+    <t>devour all our crops</t>
+  </si>
+  <si>
+    <t>kill our flocks and herds</t>
+  </si>
+  <si>
+    <t>we owe a lot to the birds and beasts</t>
+  </si>
+  <si>
+    <t>A herd is a group of animals with four legs: a herd of buffalo, dairy cows, antelope, zebras.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A flock is a group of winged animals: a flock of doves, Canada geese, mallards. </t>
+  </si>
+  <si>
+    <t>A swarm involves insects: a swarm of bees, love bugs, mosquitoes.</t>
+  </si>
+  <si>
+    <t>devour</t>
+  </si>
+  <si>
+    <t>owe … to sth</t>
+  </si>
+  <si>
+    <t>spiders never do the least harm to us or our belongings</t>
+  </si>
+  <si>
+    <t>do the least harm to</t>
+  </si>
+  <si>
+    <t>on our behalf</t>
+  </si>
+  <si>
+    <t>a census of</t>
+  </si>
+  <si>
+    <t>a football pitch</t>
+  </si>
+  <si>
+    <t>我们的利益</t>
+  </si>
+  <si>
+    <t>It is impossible to make more the the wildest guess at …</t>
+  </si>
+  <si>
+    <t>not content with</t>
+  </si>
+  <si>
+    <t>不可能做出更多最疯狂的猜测......</t>
+  </si>
+  <si>
+    <t>不满足于</t>
+  </si>
+  <si>
+    <t>(人)口普查</t>
+  </si>
+  <si>
+    <t>without doubt</t>
+  </si>
+  <si>
+    <t>be exposed to</t>
+  </si>
+  <si>
+    <t>ashamed</t>
+  </si>
+  <si>
+    <t>enforce</t>
+  </si>
+  <si>
+    <t>interfere</t>
+  </si>
+  <si>
+    <t>chimp</t>
+  </si>
+  <si>
+    <t>毫无疑问</t>
+  </si>
+  <si>
+    <t>接触到</t>
+  </si>
+  <si>
+    <t>羞愧</t>
+  </si>
+  <si>
+    <t>执行</t>
+  </si>
+  <si>
+    <t>干扰</t>
+  </si>
+  <si>
+    <t>黑猩猩</t>
+  </si>
+  <si>
+    <t>adequate</t>
+  </si>
+  <si>
+    <t>equilibrium</t>
+  </si>
+  <si>
+    <t>accusation</t>
+  </si>
+  <si>
+    <t>desperate</t>
+  </si>
+  <si>
+    <t>freelance</t>
+  </si>
+  <si>
+    <t>prevailing</t>
+  </si>
+  <si>
+    <t>alienation</t>
+  </si>
+  <si>
+    <t>stem from</t>
+  </si>
+  <si>
+    <t>an incessant stream of favorable policies</t>
+  </si>
+  <si>
+    <t>scrapping burdensome taxes</t>
+  </si>
+  <si>
+    <t>more rewarding than</t>
+  </si>
+  <si>
+    <t>twofold</t>
+  </si>
+  <si>
+    <t>vacancy</t>
+  </si>
+  <si>
+    <t>segments of China's export industry craw up the value chain</t>
+  </si>
+  <si>
+    <t>Master of Literature</t>
+  </si>
+  <si>
+    <t>a hot economy</t>
+  </si>
+  <si>
+    <t>Christian</t>
+  </si>
+  <si>
+    <t>Christianity</t>
+  </si>
+  <si>
+    <t>by the government</t>
+  </si>
+  <si>
+    <t>充足</t>
+  </si>
+  <si>
+    <t>平衡</t>
+  </si>
+  <si>
+    <t>指控</t>
+  </si>
+  <si>
+    <t>殊死</t>
+  </si>
+  <si>
+    <t>自由职业者</t>
+  </si>
+  <si>
+    <t>异化</t>
+  </si>
+  <si>
+    <t>源于</t>
+  </si>
+  <si>
+    <t>不断的有利政策</t>
+  </si>
+  <si>
+    <t>废弃繁重的税收</t>
+  </si>
+  <si>
+    <t>比...更有价值</t>
+  </si>
+  <si>
+    <t>双重</t>
+  </si>
+  <si>
+    <t>空缺</t>
+  </si>
+  <si>
+    <t>中国出口业的细分市场正在崛起</t>
+  </si>
+  <si>
+    <t>文学硕士</t>
+  </si>
+  <si>
+    <t>一个热门的经济</t>
+  </si>
+  <si>
+    <t>基督教</t>
+  </si>
+  <si>
+    <t>由政府</t>
+  </si>
+  <si>
+    <t>荒谬</t>
+  </si>
+  <si>
+    <t>高周转</t>
+  </si>
+  <si>
+    <t>ridiculous</t>
+  </si>
+  <si>
+    <t>high turnover</t>
+  </si>
+  <si>
+    <t>hybrid car</t>
+  </si>
+  <si>
+    <t>Toyota Prius</t>
+  </si>
+  <si>
+    <t>subsidy</t>
+  </si>
+  <si>
+    <t>mechanic</t>
+  </si>
+  <si>
+    <t>Silicon Valley</t>
+  </si>
+  <si>
+    <t>混合动力汽车</t>
+  </si>
+  <si>
+    <t>丰田普锐斯</t>
+  </si>
+  <si>
+    <t>补贴</t>
+  </si>
+  <si>
+    <t>机械</t>
+  </si>
+  <si>
+    <t>硅谷</t>
+  </si>
+  <si>
+    <t>MSG</t>
+  </si>
+  <si>
+    <t>monosodium glutamate</t>
+  </si>
+  <si>
+    <t>condiments</t>
+  </si>
+  <si>
+    <t>pickle</t>
+  </si>
+  <si>
+    <t>genre</t>
+  </si>
+  <si>
+    <t>vineger</t>
+  </si>
+  <si>
+    <t>contaminted</t>
+  </si>
+  <si>
+    <t>adverse</t>
+  </si>
+  <si>
+    <t>persist</t>
+  </si>
+  <si>
+    <t>faint</t>
+  </si>
+  <si>
+    <t>parsley</t>
+  </si>
+  <si>
+    <t>fancy</t>
+  </si>
+  <si>
+    <t>racked</t>
+  </si>
+  <si>
+    <t>racked my brain</t>
+  </si>
+  <si>
+    <t>excessive intake</t>
+  </si>
+  <si>
+    <t>anecdotal</t>
+  </si>
+  <si>
+    <t>anecdotal report</t>
+  </si>
+  <si>
+    <t>heart palpitation</t>
+  </si>
+  <si>
+    <t>nausea</t>
+  </si>
+  <si>
+    <t>cumin powder</t>
+  </si>
+  <si>
+    <t>Amino acid</t>
+  </si>
+  <si>
+    <t>numb</t>
+  </si>
+  <si>
+    <t>Nitrate</t>
+  </si>
+  <si>
+    <t>Nitrite</t>
+  </si>
+  <si>
+    <t>味精</t>
+  </si>
+  <si>
+    <t>谷氨酸钠</t>
+  </si>
+  <si>
+    <t>调味品</t>
+  </si>
+  <si>
+    <t>泡菜</t>
+  </si>
+  <si>
+    <t>类型</t>
+  </si>
+  <si>
+    <t>不利的</t>
+  </si>
+  <si>
+    <t>坚持</t>
+  </si>
+  <si>
+    <t>晕</t>
+  </si>
+  <si>
+    <t>香菜</t>
+  </si>
+  <si>
+    <t>幻想</t>
+  </si>
+  <si>
+    <t>折磨</t>
+  </si>
+  <si>
+    <t>绞尽脑汁</t>
+  </si>
+  <si>
+    <t>摄入量过多</t>
+  </si>
+  <si>
+    <t>传闻</t>
+  </si>
+  <si>
+    <t>轶事报道</t>
+  </si>
+  <si>
+    <t>心悸</t>
+  </si>
+  <si>
+    <t>恶心</t>
+  </si>
+  <si>
+    <t>孜然粉</t>
+  </si>
+  <si>
+    <t>氨基酸</t>
+  </si>
+  <si>
+    <t>麻木</t>
+  </si>
+  <si>
+    <t>硝酸盐</t>
+  </si>
+  <si>
+    <t>亚硝酸盐</t>
   </si>
 </sst>
 </file>
@@ -3767,7 +4256,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3782,7 +4271,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6699"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3851,7 +4346,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3868,14 +4363,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3889,6 +4393,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF6699"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -4166,11 +4675,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:M520"/>
+  <dimension ref="B1:M518"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A332" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H337" sqref="H337"/>
+      <pane ySplit="4" topLeftCell="A398" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F403" sqref="F403"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
@@ -4186,20 +4695,20 @@
   <sheetData>
     <row r="1" spans="2:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:13" ht="32.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="6" t="s">
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="9" t="s">
         <v>12</v>
       </c>
     </row>
@@ -4254,7 +4763,7 @@
       <c r="E5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="7" t="s">
         <v>13</v>
       </c>
       <c r="G5" s="5" t="s">
@@ -4794,7 +5303,7 @@
       <c r="E23" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="F23" s="7" t="s">
+      <c r="F23" s="6" t="s">
         <v>44</v>
       </c>
       <c r="G23" s="5" t="s">
@@ -4824,7 +5333,7 @@
       <c r="E24" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="F24" s="7" t="s">
+      <c r="F24" s="6" t="s">
         <v>45</v>
       </c>
       <c r="G24" s="5" t="s">
@@ -4854,7 +5363,7 @@
       <c r="E25" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="F25" s="7" t="s">
+      <c r="F25" s="6" t="s">
         <v>46</v>
       </c>
       <c r="G25" s="5" t="s">
@@ -4944,7 +5453,7 @@
       <c r="E28" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F28" s="7" t="s">
+      <c r="F28" s="6" t="s">
         <v>49</v>
       </c>
       <c r="G28" s="5" t="s">
@@ -5094,7 +5603,7 @@
       <c r="E33" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="F33" s="7" t="s">
+      <c r="F33" s="6" t="s">
         <v>54</v>
       </c>
       <c r="G33" s="5" t="s">
@@ -5214,7 +5723,7 @@
       <c r="E37" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="F37" s="7" t="s">
+      <c r="F37" s="6" t="s">
         <v>58</v>
       </c>
       <c r="G37" s="5" t="s">
@@ -5244,7 +5753,7 @@
       <c r="E38" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F38" s="7" t="s">
+      <c r="F38" s="6" t="s">
         <v>59</v>
       </c>
       <c r="G38" s="5" t="s">
@@ -5274,7 +5783,7 @@
       <c r="E39" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="F39" s="8" t="s">
+      <c r="F39" s="7" t="s">
         <v>60</v>
       </c>
       <c r="G39" s="5" t="s">
@@ -13824,1151 +14333,2307 @@
       <c r="M342" s="5"/>
     </row>
     <row r="343" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B343" s="2"/>
-      <c r="C343" s="3"/>
-      <c r="D343" s="5"/>
-      <c r="E343" s="5"/>
+      <c r="B343" s="2">
+        <v>339</v>
+      </c>
+      <c r="C343" s="3">
+        <v>43535</v>
+      </c>
+      <c r="D343" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E343" s="5" t="s">
+        <v>1228</v>
+      </c>
       <c r="F343" s="5"/>
-      <c r="G343" s="5"/>
+      <c r="G343" s="5" t="s">
+        <v>1249</v>
+      </c>
       <c r="H343" s="5"/>
       <c r="I343" s="5"/>
       <c r="J343" s="5"/>
-      <c r="K343" s="5"/>
-      <c r="L343" s="5"/>
+      <c r="K343" s="5">
+        <v>1</v>
+      </c>
+      <c r="L343" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M343" s="5"/>
     </row>
     <row r="344" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B344" s="2"/>
-      <c r="C344" s="3"/>
-      <c r="D344" s="5"/>
-      <c r="E344" s="5"/>
+      <c r="B344" s="2">
+        <v>340</v>
+      </c>
+      <c r="C344" s="3">
+        <v>43535</v>
+      </c>
+      <c r="D344" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E344" s="5" t="s">
+        <v>1246</v>
+      </c>
       <c r="F344" s="5"/>
-      <c r="G344" s="5"/>
-      <c r="H344" s="5"/>
+      <c r="G344" s="5" t="s">
+        <v>1247</v>
+      </c>
+      <c r="H344" s="5" t="s">
+        <v>1248</v>
+      </c>
       <c r="I344" s="5"/>
       <c r="J344" s="5"/>
-      <c r="K344" s="5"/>
-      <c r="L344" s="5"/>
+      <c r="K344" s="5">
+        <v>1</v>
+      </c>
+      <c r="L344" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M344" s="5"/>
     </row>
     <row r="345" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B345" s="2"/>
-      <c r="C345" s="3"/>
-      <c r="D345" s="5"/>
-      <c r="E345" s="5"/>
+      <c r="B345" s="2">
+        <v>341</v>
+      </c>
+      <c r="C345" s="3">
+        <v>43535</v>
+      </c>
+      <c r="D345" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E345" s="5" t="s">
+        <v>1229</v>
+      </c>
       <c r="F345" s="5"/>
-      <c r="G345" s="5"/>
+      <c r="G345" s="5" t="s">
+        <v>1250</v>
+      </c>
       <c r="H345" s="5"/>
       <c r="I345" s="5"/>
       <c r="J345" s="5"/>
-      <c r="K345" s="5"/>
-      <c r="L345" s="5"/>
+      <c r="K345" s="5">
+        <v>1</v>
+      </c>
+      <c r="L345" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M345" s="5"/>
     </row>
     <row r="346" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B346" s="2"/>
-      <c r="C346" s="3"/>
-      <c r="D346" s="5"/>
-      <c r="E346" s="5"/>
+      <c r="B346" s="2">
+        <v>342</v>
+      </c>
+      <c r="C346" s="3">
+        <v>43535</v>
+      </c>
+      <c r="D346" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E346" s="5" t="s">
+        <v>1230</v>
+      </c>
       <c r="F346" s="5"/>
-      <c r="G346" s="5"/>
+      <c r="G346" s="5" t="s">
+        <v>1251</v>
+      </c>
       <c r="H346" s="5"/>
       <c r="I346" s="5"/>
       <c r="J346" s="5"/>
-      <c r="K346" s="5"/>
-      <c r="L346" s="5"/>
+      <c r="K346" s="5">
+        <v>1</v>
+      </c>
+      <c r="L346" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M346" s="5"/>
     </row>
     <row r="347" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B347" s="2"/>
-      <c r="C347" s="3"/>
-      <c r="D347" s="5"/>
-      <c r="E347" s="5"/>
+      <c r="B347" s="2">
+        <v>343</v>
+      </c>
+      <c r="C347" s="3">
+        <v>43535</v>
+      </c>
+      <c r="D347" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E347" s="5" t="s">
+        <v>1231</v>
+      </c>
       <c r="F347" s="5"/>
-      <c r="G347" s="5"/>
-      <c r="H347" s="5"/>
+      <c r="G347" s="5" t="s">
+        <v>1245</v>
+      </c>
+      <c r="H347" s="5" t="s">
+        <v>1244</v>
+      </c>
       <c r="I347" s="5"/>
       <c r="J347" s="5"/>
-      <c r="K347" s="5"/>
-      <c r="L347" s="5"/>
+      <c r="K347" s="5">
+        <v>1</v>
+      </c>
+      <c r="L347" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M347" s="5"/>
     </row>
     <row r="348" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B348" s="2"/>
-      <c r="C348" s="3"/>
-      <c r="D348" s="5"/>
-      <c r="E348" s="5"/>
+      <c r="B348" s="2">
+        <v>344</v>
+      </c>
+      <c r="C348" s="3">
+        <v>43535</v>
+      </c>
+      <c r="D348" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E348" s="5" t="s">
+        <v>1232</v>
+      </c>
       <c r="F348" s="5"/>
-      <c r="G348" s="5"/>
+      <c r="G348" s="5" t="s">
+        <v>1263</v>
+      </c>
       <c r="H348" s="5"/>
       <c r="I348" s="5"/>
       <c r="J348" s="5"/>
-      <c r="K348" s="5"/>
-      <c r="L348" s="5"/>
+      <c r="K348" s="5">
+        <v>1</v>
+      </c>
+      <c r="L348" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M348" s="5"/>
     </row>
     <row r="349" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B349" s="2"/>
-      <c r="C349" s="3"/>
-      <c r="D349" s="5"/>
-      <c r="E349" s="5"/>
+      <c r="B349" s="2">
+        <v>345</v>
+      </c>
+      <c r="C349" s="3">
+        <v>43535</v>
+      </c>
+      <c r="D349" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E349" s="5" t="s">
+        <v>1233</v>
+      </c>
       <c r="F349" s="5"/>
-      <c r="G349" s="5"/>
+      <c r="G349" s="5" t="s">
+        <v>1252</v>
+      </c>
       <c r="H349" s="5"/>
       <c r="I349" s="5"/>
       <c r="J349" s="5"/>
-      <c r="K349" s="5"/>
-      <c r="L349" s="5"/>
+      <c r="K349" s="5">
+        <v>1</v>
+      </c>
+      <c r="L349" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M349" s="5"/>
     </row>
     <row r="350" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B350" s="2"/>
-      <c r="C350" s="3"/>
-      <c r="D350" s="5"/>
-      <c r="E350" s="5"/>
+      <c r="B350" s="2">
+        <v>346</v>
+      </c>
+      <c r="C350" s="3">
+        <v>43535</v>
+      </c>
+      <c r="D350" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E350" s="5" t="s">
+        <v>1234</v>
+      </c>
       <c r="F350" s="5"/>
-      <c r="G350" s="5"/>
+      <c r="G350" s="5" t="s">
+        <v>1253</v>
+      </c>
       <c r="H350" s="5"/>
       <c r="I350" s="5"/>
       <c r="J350" s="5"/>
-      <c r="K350" s="5"/>
-      <c r="L350" s="5"/>
+      <c r="K350" s="5">
+        <v>1</v>
+      </c>
+      <c r="L350" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M350" s="5"/>
     </row>
     <row r="351" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B351" s="2"/>
-      <c r="C351" s="3"/>
-      <c r="D351" s="5"/>
-      <c r="E351" s="5"/>
+      <c r="B351" s="2">
+        <v>347</v>
+      </c>
+      <c r="C351" s="3">
+        <v>43535</v>
+      </c>
+      <c r="D351" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E351" s="5" t="s">
+        <v>1235</v>
+      </c>
       <c r="F351" s="5"/>
-      <c r="G351" s="5"/>
+      <c r="G351" s="5" t="s">
+        <v>1254</v>
+      </c>
       <c r="H351" s="5"/>
       <c r="I351" s="5"/>
       <c r="J351" s="5"/>
-      <c r="K351" s="5"/>
-      <c r="L351" s="5"/>
+      <c r="K351" s="5">
+        <v>1</v>
+      </c>
+      <c r="L351" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M351" s="5"/>
     </row>
     <row r="352" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B352" s="2"/>
-      <c r="C352" s="3"/>
-      <c r="D352" s="5"/>
-      <c r="E352" s="5"/>
+      <c r="B352" s="2">
+        <v>348</v>
+      </c>
+      <c r="C352" s="3">
+        <v>43535</v>
+      </c>
+      <c r="D352" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E352" s="5" t="s">
+        <v>1236</v>
+      </c>
       <c r="F352" s="5"/>
-      <c r="G352" s="5"/>
+      <c r="G352" s="5" t="s">
+        <v>1255</v>
+      </c>
       <c r="H352" s="5"/>
       <c r="I352" s="5"/>
       <c r="J352" s="5"/>
-      <c r="K352" s="5"/>
-      <c r="L352" s="5"/>
+      <c r="K352" s="5">
+        <v>1</v>
+      </c>
+      <c r="L352" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M352" s="5"/>
     </row>
     <row r="353" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B353" s="2"/>
-      <c r="C353" s="3"/>
-      <c r="D353" s="5"/>
-      <c r="E353" s="5"/>
+      <c r="B353" s="2">
+        <v>349</v>
+      </c>
+      <c r="C353" s="3">
+        <v>43535</v>
+      </c>
+      <c r="D353" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E353" s="5" t="s">
+        <v>1237</v>
+      </c>
       <c r="F353" s="5"/>
-      <c r="G353" s="5"/>
+      <c r="G353" s="5" t="s">
+        <v>1256</v>
+      </c>
       <c r="H353" s="5"/>
       <c r="I353" s="5"/>
       <c r="J353" s="5"/>
-      <c r="K353" s="5"/>
-      <c r="L353" s="5"/>
+      <c r="K353" s="5">
+        <v>1</v>
+      </c>
+      <c r="L353" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M353" s="5"/>
     </row>
     <row r="354" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B354" s="2"/>
-      <c r="C354" s="3"/>
-      <c r="D354" s="5"/>
-      <c r="E354" s="5"/>
+      <c r="B354" s="2">
+        <v>350</v>
+      </c>
+      <c r="C354" s="3">
+        <v>43535</v>
+      </c>
+      <c r="D354" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E354" s="5" t="s">
+        <v>1238</v>
+      </c>
       <c r="F354" s="5"/>
-      <c r="G354" s="5"/>
+      <c r="G354" s="5" t="s">
+        <v>1257</v>
+      </c>
       <c r="H354" s="5"/>
       <c r="I354" s="5"/>
       <c r="J354" s="5"/>
-      <c r="K354" s="5"/>
-      <c r="L354" s="5"/>
+      <c r="K354" s="5">
+        <v>1</v>
+      </c>
+      <c r="L354" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M354" s="5"/>
     </row>
     <row r="355" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B355" s="2"/>
-      <c r="C355" s="3"/>
-      <c r="D355" s="5"/>
-      <c r="E355" s="5"/>
+      <c r="B355" s="2">
+        <v>351</v>
+      </c>
+      <c r="C355" s="3">
+        <v>43535</v>
+      </c>
+      <c r="D355" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E355" s="5" t="s">
+        <v>1239</v>
+      </c>
       <c r="F355" s="5"/>
-      <c r="G355" s="5"/>
+      <c r="G355" s="5" t="s">
+        <v>1258</v>
+      </c>
       <c r="H355" s="5"/>
       <c r="I355" s="5"/>
       <c r="J355" s="5"/>
-      <c r="K355" s="5"/>
-      <c r="L355" s="5"/>
+      <c r="K355" s="5">
+        <v>1</v>
+      </c>
+      <c r="L355" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M355" s="5"/>
     </row>
     <row r="356" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B356" s="2"/>
-      <c r="C356" s="3"/>
-      <c r="D356" s="5"/>
-      <c r="E356" s="5"/>
+      <c r="B356" s="2">
+        <v>352</v>
+      </c>
+      <c r="C356" s="3">
+        <v>43535</v>
+      </c>
+      <c r="D356" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E356" s="5" t="s">
+        <v>1240</v>
+      </c>
       <c r="F356" s="5"/>
-      <c r="G356" s="5"/>
+      <c r="G356" s="5" t="s">
+        <v>1259</v>
+      </c>
       <c r="H356" s="5"/>
       <c r="I356" s="5"/>
       <c r="J356" s="5"/>
-      <c r="K356" s="5"/>
-      <c r="L356" s="5"/>
+      <c r="K356" s="5">
+        <v>1</v>
+      </c>
+      <c r="L356" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M356" s="5"/>
     </row>
     <row r="357" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B357" s="2"/>
-      <c r="C357" s="3"/>
-      <c r="D357" s="5"/>
-      <c r="E357" s="5"/>
+      <c r="B357" s="2">
+        <v>353</v>
+      </c>
+      <c r="C357" s="3">
+        <v>43535</v>
+      </c>
+      <c r="D357" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E357" s="5" t="s">
+        <v>1241</v>
+      </c>
       <c r="F357" s="5"/>
-      <c r="G357" s="5"/>
+      <c r="G357" s="5" t="s">
+        <v>1260</v>
+      </c>
       <c r="H357" s="5"/>
       <c r="I357" s="5"/>
       <c r="J357" s="5"/>
-      <c r="K357" s="5"/>
-      <c r="L357" s="5"/>
+      <c r="K357" s="5">
+        <v>1</v>
+      </c>
+      <c r="L357" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M357" s="5"/>
     </row>
     <row r="358" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B358" s="2"/>
-      <c r="C358" s="3"/>
-      <c r="D358" s="5"/>
-      <c r="E358" s="5"/>
+      <c r="B358" s="2">
+        <v>354</v>
+      </c>
+      <c r="C358" s="3">
+        <v>43535</v>
+      </c>
+      <c r="D358" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E358" s="5" t="s">
+        <v>1242</v>
+      </c>
       <c r="F358" s="5"/>
-      <c r="G358" s="5"/>
+      <c r="G358" s="5" t="s">
+        <v>1261</v>
+      </c>
       <c r="H358" s="5"/>
       <c r="I358" s="5"/>
       <c r="J358" s="5"/>
-      <c r="K358" s="5"/>
-      <c r="L358" s="5"/>
+      <c r="K358" s="5">
+        <v>1</v>
+      </c>
+      <c r="L358" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M358" s="5"/>
     </row>
     <row r="359" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B359" s="2"/>
-      <c r="C359" s="3"/>
-      <c r="D359" s="5"/>
-      <c r="E359" s="5"/>
+      <c r="B359" s="2">
+        <v>355</v>
+      </c>
+      <c r="C359" s="3">
+        <v>43535</v>
+      </c>
+      <c r="D359" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E359" s="5" t="s">
+        <v>1243</v>
+      </c>
       <c r="F359" s="5"/>
-      <c r="G359" s="5"/>
+      <c r="G359" s="5" t="s">
+        <v>1262</v>
+      </c>
       <c r="H359" s="5"/>
       <c r="I359" s="5"/>
       <c r="J359" s="5"/>
-      <c r="K359" s="5"/>
-      <c r="L359" s="5"/>
+      <c r="K359" s="5">
+        <v>1</v>
+      </c>
+      <c r="L359" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M359" s="5"/>
     </row>
     <row r="360" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B360" s="2"/>
-      <c r="C360" s="3"/>
-      <c r="D360" s="5"/>
-      <c r="E360" s="5"/>
+      <c r="B360" s="2">
+        <v>356</v>
+      </c>
+      <c r="C360" s="3">
+        <v>43536</v>
+      </c>
+      <c r="D360" s="5" t="s">
+        <v>1056</v>
+      </c>
+      <c r="E360" s="5" t="s">
+        <v>1264</v>
+      </c>
       <c r="F360" s="5"/>
-      <c r="G360" s="5"/>
+      <c r="G360" s="5" t="s">
+        <v>1270</v>
+      </c>
       <c r="H360" s="5"/>
       <c r="I360" s="5"/>
       <c r="J360" s="5"/>
-      <c r="K360" s="5"/>
-      <c r="L360" s="5"/>
+      <c r="K360" s="5">
+        <v>1</v>
+      </c>
+      <c r="L360" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M360" s="5"/>
     </row>
     <row r="361" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B361" s="2"/>
-      <c r="C361" s="3"/>
-      <c r="D361" s="5"/>
-      <c r="E361" s="5"/>
+      <c r="B361" s="2">
+        <v>357</v>
+      </c>
+      <c r="C361" s="3">
+        <v>43536</v>
+      </c>
+      <c r="D361" s="5" t="s">
+        <v>1056</v>
+      </c>
+      <c r="E361" s="5" t="s">
+        <v>1265</v>
+      </c>
       <c r="F361" s="5"/>
-      <c r="G361" s="5"/>
-      <c r="H361" s="5"/>
-      <c r="I361" s="5"/>
+      <c r="G361" s="5" t="s">
+        <v>1268</v>
+      </c>
+      <c r="H361" s="5" t="s">
+        <v>1267</v>
+      </c>
+      <c r="I361" s="5" t="s">
+        <v>1269</v>
+      </c>
       <c r="J361" s="5"/>
-      <c r="K361" s="5"/>
-      <c r="L361" s="5"/>
+      <c r="K361" s="5">
+        <v>1</v>
+      </c>
+      <c r="L361" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M361" s="5"/>
     </row>
     <row r="362" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B362" s="2"/>
-      <c r="C362" s="3"/>
-      <c r="D362" s="5"/>
-      <c r="E362" s="5"/>
+      <c r="B362" s="2">
+        <v>358</v>
+      </c>
+      <c r="C362" s="3">
+        <v>43536</v>
+      </c>
+      <c r="D362" s="5" t="s">
+        <v>1056</v>
+      </c>
+      <c r="E362" s="5" t="s">
+        <v>1266</v>
+      </c>
       <c r="F362" s="5"/>
-      <c r="G362" s="5"/>
+      <c r="G362" s="5" t="s">
+        <v>1271</v>
+      </c>
       <c r="H362" s="5"/>
       <c r="I362" s="5"/>
       <c r="J362" s="5"/>
-      <c r="K362" s="5"/>
-      <c r="L362" s="5"/>
+      <c r="K362" s="5">
+        <v>1</v>
+      </c>
+      <c r="L362" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M362" s="5"/>
     </row>
     <row r="363" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B363" s="2"/>
-      <c r="C363" s="3"/>
-      <c r="D363" s="5"/>
-      <c r="E363" s="5"/>
+      <c r="B363" s="2">
+        <v>359</v>
+      </c>
+      <c r="C363" s="3">
+        <v>43536</v>
+      </c>
+      <c r="D363" s="5" t="s">
+        <v>1056</v>
+      </c>
+      <c r="E363" s="5" t="s">
+        <v>1272</v>
+      </c>
       <c r="F363" s="5"/>
-      <c r="G363" s="5"/>
+      <c r="G363" s="5" t="s">
+        <v>1273</v>
+      </c>
       <c r="H363" s="5"/>
       <c r="I363" s="5"/>
       <c r="J363" s="5"/>
-      <c r="K363" s="5"/>
-      <c r="L363" s="5"/>
+      <c r="K363" s="5">
+        <v>1</v>
+      </c>
+      <c r="L363" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M363" s="5"/>
     </row>
     <row r="364" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B364" s="2"/>
-      <c r="C364" s="3"/>
-      <c r="D364" s="5"/>
-      <c r="E364" s="5"/>
+      <c r="B364" s="2">
+        <v>360</v>
+      </c>
+      <c r="C364" s="3">
+        <v>43536</v>
+      </c>
+      <c r="D364" s="5" t="s">
+        <v>1056</v>
+      </c>
+      <c r="E364" s="5" t="s">
+        <v>1274</v>
+      </c>
       <c r="F364" s="5"/>
-      <c r="G364" s="5"/>
+      <c r="G364" s="5" t="s">
+        <v>1277</v>
+      </c>
       <c r="H364" s="5"/>
       <c r="I364" s="5"/>
       <c r="J364" s="5"/>
-      <c r="K364" s="5"/>
-      <c r="L364" s="5"/>
+      <c r="K364" s="5">
+        <v>1</v>
+      </c>
+      <c r="L364" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M364" s="5"/>
     </row>
     <row r="365" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B365" s="2"/>
-      <c r="C365" s="3"/>
-      <c r="D365" s="5"/>
-      <c r="E365" s="5"/>
+      <c r="B365" s="2">
+        <v>361</v>
+      </c>
+      <c r="C365" s="3">
+        <v>43536</v>
+      </c>
+      <c r="D365" s="5" t="s">
+        <v>1056</v>
+      </c>
+      <c r="E365" s="5" t="s">
+        <v>1275</v>
+      </c>
       <c r="F365" s="5"/>
-      <c r="G365" s="5"/>
+      <c r="G365" s="5" t="s">
+        <v>1282</v>
+      </c>
       <c r="H365" s="5"/>
       <c r="I365" s="5"/>
       <c r="J365" s="5"/>
-      <c r="K365" s="5"/>
-      <c r="L365" s="5"/>
+      <c r="K365" s="5">
+        <v>1</v>
+      </c>
+      <c r="L365" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M365" s="5"/>
     </row>
     <row r="366" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B366" s="2"/>
-      <c r="C366" s="3"/>
-      <c r="D366" s="5"/>
-      <c r="E366" s="5"/>
+      <c r="B366" s="2">
+        <v>362</v>
+      </c>
+      <c r="C366" s="3">
+        <v>43536</v>
+      </c>
+      <c r="D366" s="5" t="s">
+        <v>1056</v>
+      </c>
+      <c r="E366" s="5" t="s">
+        <v>1276</v>
+      </c>
       <c r="F366" s="5"/>
-      <c r="G366" s="5"/>
+      <c r="G366" s="5" t="s">
+        <v>111</v>
+      </c>
       <c r="H366" s="5"/>
       <c r="I366" s="5"/>
       <c r="J366" s="5"/>
-      <c r="K366" s="5"/>
-      <c r="L366" s="5"/>
+      <c r="K366" s="5">
+        <v>1</v>
+      </c>
+      <c r="L366" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M366" s="5"/>
     </row>
     <row r="367" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B367" s="2"/>
-      <c r="C367" s="3"/>
-      <c r="D367" s="5"/>
-      <c r="E367" s="5"/>
+      <c r="B367" s="2">
+        <v>363</v>
+      </c>
+      <c r="C367" s="3">
+        <v>43536</v>
+      </c>
+      <c r="D367" s="5" t="s">
+        <v>1056</v>
+      </c>
+      <c r="E367" s="5" t="s">
+        <v>1278</v>
+      </c>
       <c r="F367" s="5"/>
-      <c r="G367" s="5"/>
+      <c r="G367" s="5" t="s">
+        <v>1280</v>
+      </c>
       <c r="H367" s="5"/>
       <c r="I367" s="5"/>
       <c r="J367" s="5"/>
-      <c r="K367" s="5"/>
-      <c r="L367" s="5"/>
+      <c r="K367" s="5">
+        <v>1</v>
+      </c>
+      <c r="L367" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M367" s="5"/>
     </row>
     <row r="368" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B368" s="2"/>
-      <c r="C368" s="3"/>
-      <c r="D368" s="5"/>
-      <c r="E368" s="5"/>
+      <c r="B368" s="2">
+        <v>364</v>
+      </c>
+      <c r="C368" s="3">
+        <v>43536</v>
+      </c>
+      <c r="D368" s="5" t="s">
+        <v>1056</v>
+      </c>
+      <c r="E368" s="5" t="s">
+        <v>1279</v>
+      </c>
       <c r="F368" s="5"/>
-      <c r="G368" s="5"/>
+      <c r="G368" s="5" t="s">
+        <v>1281</v>
+      </c>
       <c r="H368" s="5"/>
       <c r="I368" s="5"/>
       <c r="J368" s="5"/>
-      <c r="K368" s="5"/>
-      <c r="L368" s="5"/>
+      <c r="K368" s="5">
+        <v>1</v>
+      </c>
+      <c r="L368" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M368" s="5"/>
     </row>
     <row r="369" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B369" s="2"/>
-      <c r="C369" s="3"/>
-      <c r="D369" s="5"/>
-      <c r="E369" s="5"/>
+      <c r="B369" s="2">
+        <v>365</v>
+      </c>
+      <c r="C369" s="3">
+        <v>43538</v>
+      </c>
+      <c r="D369" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E369" s="5" t="s">
+        <v>1283</v>
+      </c>
       <c r="F369" s="5"/>
-      <c r="G369" s="5"/>
+      <c r="G369" s="5" t="s">
+        <v>1289</v>
+      </c>
       <c r="H369" s="5"/>
       <c r="I369" s="5"/>
       <c r="J369" s="5"/>
-      <c r="K369" s="5"/>
-      <c r="L369" s="5"/>
+      <c r="K369" s="5">
+        <v>1</v>
+      </c>
+      <c r="L369" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M369" s="5"/>
     </row>
     <row r="370" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B370" s="2"/>
-      <c r="C370" s="3"/>
-      <c r="D370" s="5"/>
-      <c r="E370" s="5"/>
+      <c r="B370" s="2">
+        <v>366</v>
+      </c>
+      <c r="C370" s="3">
+        <v>43538</v>
+      </c>
+      <c r="D370" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E370" s="5" t="s">
+        <v>1284</v>
+      </c>
       <c r="F370" s="5"/>
-      <c r="G370" s="5"/>
+      <c r="G370" s="5" t="s">
+        <v>1290</v>
+      </c>
       <c r="H370" s="5"/>
       <c r="I370" s="5"/>
       <c r="J370" s="5"/>
-      <c r="K370" s="5"/>
-      <c r="L370" s="5"/>
+      <c r="K370" s="5">
+        <v>1</v>
+      </c>
+      <c r="L370" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M370" s="5"/>
     </row>
     <row r="371" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B371" s="2"/>
-      <c r="C371" s="3"/>
-      <c r="D371" s="5"/>
-      <c r="E371" s="5"/>
+      <c r="B371" s="2">
+        <v>367</v>
+      </c>
+      <c r="C371" s="3">
+        <v>43538</v>
+      </c>
+      <c r="D371" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E371" s="5" t="s">
+        <v>1285</v>
+      </c>
       <c r="F371" s="5"/>
-      <c r="G371" s="5"/>
+      <c r="G371" s="5" t="s">
+        <v>1291</v>
+      </c>
       <c r="H371" s="5"/>
       <c r="I371" s="5"/>
       <c r="J371" s="5"/>
-      <c r="K371" s="5"/>
-      <c r="L371" s="5"/>
+      <c r="K371" s="5">
+        <v>1</v>
+      </c>
+      <c r="L371" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M371" s="5"/>
     </row>
     <row r="372" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B372" s="2"/>
-      <c r="C372" s="3"/>
-      <c r="D372" s="5"/>
-      <c r="E372" s="5"/>
+      <c r="B372" s="2">
+        <v>368</v>
+      </c>
+      <c r="C372" s="3">
+        <v>43538</v>
+      </c>
+      <c r="D372" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E372" s="5" t="s">
+        <v>1286</v>
+      </c>
       <c r="F372" s="5"/>
-      <c r="G372" s="5"/>
+      <c r="G372" s="5" t="s">
+        <v>1292</v>
+      </c>
       <c r="H372" s="5"/>
       <c r="I372" s="5"/>
       <c r="J372" s="5"/>
-      <c r="K372" s="5"/>
-      <c r="L372" s="5"/>
+      <c r="K372" s="5">
+        <v>1</v>
+      </c>
+      <c r="L372" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M372" s="5"/>
     </row>
     <row r="373" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B373" s="2"/>
-      <c r="C373" s="3"/>
-      <c r="D373" s="5"/>
-      <c r="E373" s="5"/>
+      <c r="B373" s="2">
+        <v>369</v>
+      </c>
+      <c r="C373" s="3">
+        <v>43538</v>
+      </c>
+      <c r="D373" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E373" s="5" t="s">
+        <v>1287</v>
+      </c>
       <c r="F373" s="5"/>
-      <c r="G373" s="5"/>
+      <c r="G373" s="5" t="s">
+        <v>1293</v>
+      </c>
       <c r="H373" s="5"/>
       <c r="I373" s="5"/>
       <c r="J373" s="5"/>
-      <c r="K373" s="5"/>
-      <c r="L373" s="5"/>
+      <c r="K373" s="5">
+        <v>1</v>
+      </c>
+      <c r="L373" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M373" s="5"/>
     </row>
     <row r="374" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B374" s="2"/>
-      <c r="C374" s="3"/>
-      <c r="D374" s="5"/>
-      <c r="E374" s="5"/>
+      <c r="B374" s="2">
+        <v>370</v>
+      </c>
+      <c r="C374" s="3">
+        <v>43538</v>
+      </c>
+      <c r="D374" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E374" s="5" t="s">
+        <v>1288</v>
+      </c>
       <c r="F374" s="5"/>
-      <c r="G374" s="5"/>
+      <c r="G374" s="5" t="s">
+        <v>1294</v>
+      </c>
       <c r="H374" s="5"/>
       <c r="I374" s="5"/>
       <c r="J374" s="5"/>
-      <c r="K374" s="5"/>
-      <c r="L374" s="5"/>
+      <c r="K374" s="5">
+        <v>1</v>
+      </c>
+      <c r="L374" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M374" s="5"/>
     </row>
     <row r="375" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B375" s="2"/>
-      <c r="C375" s="3"/>
-      <c r="D375" s="5"/>
-      <c r="E375" s="5"/>
+      <c r="B375" s="2">
+        <v>371</v>
+      </c>
+      <c r="C375" s="3">
+        <v>43539</v>
+      </c>
+      <c r="D375" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E375" s="5" t="s">
+        <v>1295</v>
+      </c>
       <c r="F375" s="5"/>
-      <c r="G375" s="5"/>
+      <c r="G375" s="5" t="s">
+        <v>1314</v>
+      </c>
       <c r="H375" s="5"/>
       <c r="I375" s="5"/>
       <c r="J375" s="5"/>
-      <c r="K375" s="5"/>
-      <c r="L375" s="5"/>
+      <c r="K375" s="5">
+        <v>1</v>
+      </c>
+      <c r="L375" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M375" s="5"/>
     </row>
     <row r="376" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B376" s="2"/>
-      <c r="C376" s="3"/>
-      <c r="D376" s="5"/>
-      <c r="E376" s="5"/>
+      <c r="B376" s="2">
+        <v>372</v>
+      </c>
+      <c r="C376" s="3">
+        <v>43539</v>
+      </c>
+      <c r="D376" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E376" s="5" t="s">
+        <v>1296</v>
+      </c>
       <c r="F376" s="5"/>
-      <c r="G376" s="5"/>
+      <c r="G376" s="5" t="s">
+        <v>1315</v>
+      </c>
       <c r="H376" s="5"/>
       <c r="I376" s="5"/>
       <c r="J376" s="5"/>
-      <c r="K376" s="5"/>
-      <c r="L376" s="5"/>
+      <c r="K376" s="5">
+        <v>1</v>
+      </c>
+      <c r="L376" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M376" s="5"/>
     </row>
     <row r="377" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B377" s="2"/>
-      <c r="C377" s="3"/>
-      <c r="D377" s="5"/>
-      <c r="E377" s="5"/>
+      <c r="B377" s="2">
+        <v>373</v>
+      </c>
+      <c r="C377" s="3">
+        <v>43539</v>
+      </c>
+      <c r="D377" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E377" s="5" t="s">
+        <v>1297</v>
+      </c>
       <c r="F377" s="5"/>
-      <c r="G377" s="5"/>
+      <c r="G377" s="5" t="s">
+        <v>1316</v>
+      </c>
       <c r="H377" s="5"/>
       <c r="I377" s="5"/>
       <c r="J377" s="5"/>
-      <c r="K377" s="5"/>
-      <c r="L377" s="5"/>
+      <c r="K377" s="5">
+        <v>1</v>
+      </c>
+      <c r="L377" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M377" s="5"/>
     </row>
     <row r="378" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B378" s="2"/>
-      <c r="C378" s="3"/>
-      <c r="D378" s="5"/>
-      <c r="E378" s="5"/>
+      <c r="B378" s="2">
+        <v>374</v>
+      </c>
+      <c r="C378" s="3">
+        <v>43539</v>
+      </c>
+      <c r="D378" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E378" s="5" t="s">
+        <v>1298</v>
+      </c>
       <c r="F378" s="5"/>
-      <c r="G378" s="5"/>
+      <c r="G378" s="5" t="s">
+        <v>1317</v>
+      </c>
       <c r="H378" s="5"/>
       <c r="I378" s="5"/>
       <c r="J378" s="5"/>
-      <c r="K378" s="5"/>
-      <c r="L378" s="5"/>
+      <c r="K378" s="5">
+        <v>1</v>
+      </c>
+      <c r="L378" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M378" s="5"/>
     </row>
     <row r="379" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B379" s="2"/>
-      <c r="C379" s="3"/>
-      <c r="D379" s="5"/>
-      <c r="E379" s="5"/>
+      <c r="B379" s="2">
+        <v>375</v>
+      </c>
+      <c r="C379" s="3">
+        <v>43539</v>
+      </c>
+      <c r="D379" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E379" s="5" t="s">
+        <v>1299</v>
+      </c>
       <c r="F379" s="5"/>
-      <c r="G379" s="5"/>
+      <c r="G379" s="5" t="s">
+        <v>1318</v>
+      </c>
       <c r="H379" s="5"/>
       <c r="I379" s="5"/>
       <c r="J379" s="5"/>
-      <c r="K379" s="5"/>
-      <c r="L379" s="5"/>
+      <c r="K379" s="5">
+        <v>1</v>
+      </c>
+      <c r="L379" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M379" s="5"/>
     </row>
     <row r="380" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B380" s="2"/>
-      <c r="C380" s="3"/>
-      <c r="D380" s="5"/>
-      <c r="E380" s="5"/>
+      <c r="B380" s="2">
+        <v>376</v>
+      </c>
+      <c r="C380" s="3">
+        <v>43539</v>
+      </c>
+      <c r="D380" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E380" s="5" t="s">
+        <v>1300</v>
+      </c>
       <c r="F380" s="5"/>
-      <c r="G380" s="5"/>
+      <c r="G380" s="5" t="s">
+        <v>587</v>
+      </c>
       <c r="H380" s="5"/>
       <c r="I380" s="5"/>
       <c r="J380" s="5"/>
-      <c r="K380" s="5"/>
-      <c r="L380" s="5"/>
+      <c r="K380" s="5">
+        <v>1</v>
+      </c>
+      <c r="L380" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M380" s="5"/>
     </row>
     <row r="381" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B381" s="2"/>
-      <c r="C381" s="3"/>
-      <c r="D381" s="5"/>
-      <c r="E381" s="5"/>
+      <c r="B381" s="2">
+        <v>377</v>
+      </c>
+      <c r="C381" s="3">
+        <v>43539</v>
+      </c>
+      <c r="D381" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E381" s="5" t="s">
+        <v>1301</v>
+      </c>
       <c r="F381" s="5"/>
-      <c r="G381" s="5"/>
+      <c r="G381" s="5" t="s">
+        <v>1319</v>
+      </c>
       <c r="H381" s="5"/>
       <c r="I381" s="5"/>
       <c r="J381" s="5"/>
-      <c r="K381" s="5"/>
-      <c r="L381" s="5"/>
+      <c r="K381" s="5">
+        <v>1</v>
+      </c>
+      <c r="L381" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M381" s="5"/>
     </row>
     <row r="382" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B382" s="2"/>
-      <c r="C382" s="3"/>
-      <c r="D382" s="5"/>
-      <c r="E382" s="5"/>
+      <c r="B382" s="2">
+        <v>378</v>
+      </c>
+      <c r="C382" s="3">
+        <v>43539</v>
+      </c>
+      <c r="D382" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E382" s="5" t="s">
+        <v>1302</v>
+      </c>
       <c r="F382" s="5"/>
-      <c r="G382" s="5"/>
+      <c r="G382" s="5" t="s">
+        <v>1320</v>
+      </c>
       <c r="H382" s="5"/>
       <c r="I382" s="5"/>
       <c r="J382" s="5"/>
-      <c r="K382" s="5"/>
-      <c r="L382" s="5"/>
+      <c r="K382" s="5">
+        <v>1</v>
+      </c>
+      <c r="L382" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M382" s="5"/>
     </row>
     <row r="383" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B383" s="2"/>
-      <c r="C383" s="3"/>
-      <c r="D383" s="5"/>
-      <c r="E383" s="5"/>
+      <c r="B383" s="2">
+        <v>379</v>
+      </c>
+      <c r="C383" s="3">
+        <v>43539</v>
+      </c>
+      <c r="D383" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E383" s="5" t="s">
+        <v>1303</v>
+      </c>
       <c r="F383" s="5"/>
-      <c r="G383" s="5"/>
+      <c r="G383" s="5" t="s">
+        <v>1321</v>
+      </c>
       <c r="H383" s="5"/>
       <c r="I383" s="5"/>
       <c r="J383" s="5"/>
-      <c r="K383" s="5"/>
-      <c r="L383" s="5"/>
+      <c r="K383" s="5">
+        <v>1</v>
+      </c>
+      <c r="L383" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M383" s="5"/>
     </row>
     <row r="384" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B384" s="2"/>
-      <c r="C384" s="3"/>
-      <c r="D384" s="5"/>
-      <c r="E384" s="5"/>
+      <c r="B384" s="2">
+        <v>380</v>
+      </c>
+      <c r="C384" s="3">
+        <v>43539</v>
+      </c>
+      <c r="D384" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E384" s="5" t="s">
+        <v>1304</v>
+      </c>
       <c r="F384" s="5"/>
-      <c r="G384" s="5"/>
+      <c r="G384" s="5" t="s">
+        <v>1322</v>
+      </c>
       <c r="H384" s="5"/>
       <c r="I384" s="5"/>
       <c r="J384" s="5"/>
-      <c r="K384" s="5"/>
-      <c r="L384" s="5"/>
+      <c r="K384" s="5">
+        <v>1</v>
+      </c>
+      <c r="L384" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M384" s="5"/>
     </row>
     <row r="385" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B385" s="2"/>
-      <c r="C385" s="3"/>
-      <c r="D385" s="5"/>
-      <c r="E385" s="5"/>
+      <c r="B385" s="2">
+        <v>381</v>
+      </c>
+      <c r="C385" s="3">
+        <v>43539</v>
+      </c>
+      <c r="D385" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E385" s="5" t="s">
+        <v>1305</v>
+      </c>
       <c r="F385" s="5"/>
-      <c r="G385" s="5"/>
+      <c r="G385" s="5" t="s">
+        <v>1323</v>
+      </c>
       <c r="H385" s="5"/>
       <c r="I385" s="5"/>
       <c r="J385" s="5"/>
-      <c r="K385" s="5"/>
-      <c r="L385" s="5"/>
+      <c r="K385" s="5">
+        <v>1</v>
+      </c>
+      <c r="L385" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M385" s="5"/>
     </row>
     <row r="386" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B386" s="2"/>
-      <c r="C386" s="3"/>
-      <c r="D386" s="5"/>
-      <c r="E386" s="5"/>
+      <c r="B386" s="2">
+        <v>382</v>
+      </c>
+      <c r="C386" s="3">
+        <v>43539</v>
+      </c>
+      <c r="D386" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E386" s="5" t="s">
+        <v>1306</v>
+      </c>
       <c r="F386" s="5"/>
-      <c r="G386" s="5"/>
+      <c r="G386" s="5" t="s">
+        <v>1324</v>
+      </c>
       <c r="H386" s="5"/>
       <c r="I386" s="5"/>
       <c r="J386" s="5"/>
-      <c r="K386" s="5"/>
-      <c r="L386" s="5"/>
+      <c r="K386" s="5">
+        <v>1</v>
+      </c>
+      <c r="L386" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M386" s="5"/>
     </row>
     <row r="387" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B387" s="2"/>
-      <c r="C387" s="3"/>
-      <c r="D387" s="5"/>
-      <c r="E387" s="5"/>
+      <c r="B387" s="2">
+        <v>383</v>
+      </c>
+      <c r="C387" s="3">
+        <v>43539</v>
+      </c>
+      <c r="D387" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E387" s="5" t="s">
+        <v>1307</v>
+      </c>
       <c r="F387" s="5"/>
-      <c r="G387" s="5"/>
+      <c r="G387" s="5" t="s">
+        <v>1325</v>
+      </c>
       <c r="H387" s="5"/>
       <c r="I387" s="5"/>
       <c r="J387" s="5"/>
-      <c r="K387" s="5"/>
-      <c r="L387" s="5"/>
+      <c r="K387" s="5">
+        <v>1</v>
+      </c>
+      <c r="L387" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M387" s="5"/>
     </row>
     <row r="388" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B388" s="2"/>
-      <c r="C388" s="3"/>
-      <c r="D388" s="5"/>
-      <c r="E388" s="5"/>
+      <c r="B388" s="2">
+        <v>384</v>
+      </c>
+      <c r="C388" s="3">
+        <v>43539</v>
+      </c>
+      <c r="D388" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E388" s="5" t="s">
+        <v>1308</v>
+      </c>
       <c r="F388" s="5"/>
-      <c r="G388" s="5"/>
+      <c r="G388" s="5" t="s">
+        <v>1326</v>
+      </c>
       <c r="H388" s="5"/>
       <c r="I388" s="5"/>
       <c r="J388" s="5"/>
-      <c r="K388" s="5"/>
-      <c r="L388" s="5"/>
+      <c r="K388" s="5">
+        <v>1</v>
+      </c>
+      <c r="L388" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M388" s="5"/>
     </row>
     <row r="389" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B389" s="2"/>
-      <c r="C389" s="3"/>
-      <c r="D389" s="5"/>
-      <c r="E389" s="5"/>
+      <c r="B389" s="2">
+        <v>385</v>
+      </c>
+      <c r="C389" s="3">
+        <v>43539</v>
+      </c>
+      <c r="D389" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E389" s="5" t="s">
+        <v>1309</v>
+      </c>
       <c r="F389" s="5"/>
-      <c r="G389" s="5"/>
+      <c r="G389" s="5" t="s">
+        <v>1327</v>
+      </c>
       <c r="H389" s="5"/>
       <c r="I389" s="5"/>
       <c r="J389" s="5"/>
-      <c r="K389" s="5"/>
-      <c r="L389" s="5"/>
+      <c r="K389" s="5">
+        <v>1</v>
+      </c>
+      <c r="L389" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M389" s="5"/>
     </row>
     <row r="390" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B390" s="2"/>
-      <c r="C390" s="3"/>
-      <c r="D390" s="5"/>
-      <c r="E390" s="5"/>
+      <c r="B390" s="2">
+        <v>386</v>
+      </c>
+      <c r="C390" s="3">
+        <v>43539</v>
+      </c>
+      <c r="D390" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E390" s="5" t="s">
+        <v>1310</v>
+      </c>
       <c r="F390" s="5"/>
-      <c r="G390" s="5"/>
+      <c r="G390" s="5" t="s">
+        <v>1328</v>
+      </c>
       <c r="H390" s="5"/>
       <c r="I390" s="5"/>
       <c r="J390" s="5"/>
-      <c r="K390" s="5"/>
-      <c r="L390" s="5"/>
+      <c r="K390" s="5">
+        <v>1</v>
+      </c>
+      <c r="L390" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M390" s="5"/>
     </row>
     <row r="391" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B391" s="2"/>
-      <c r="C391" s="3"/>
-      <c r="D391" s="5"/>
-      <c r="E391" s="5"/>
+      <c r="B391" s="2">
+        <v>387</v>
+      </c>
+      <c r="C391" s="3">
+        <v>43539</v>
+      </c>
+      <c r="D391" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E391" s="5" t="s">
+        <v>1311</v>
+      </c>
       <c r="F391" s="5"/>
-      <c r="G391" s="5"/>
+      <c r="G391" s="5" t="s">
+        <v>1329</v>
+      </c>
       <c r="H391" s="5"/>
       <c r="I391" s="5"/>
       <c r="J391" s="5"/>
-      <c r="K391" s="5"/>
-      <c r="L391" s="5"/>
+      <c r="K391" s="5">
+        <v>1</v>
+      </c>
+      <c r="L391" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M391" s="5"/>
     </row>
     <row r="392" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B392" s="2"/>
-      <c r="C392" s="3"/>
-      <c r="D392" s="5"/>
-      <c r="E392" s="5"/>
+      <c r="B392" s="2">
+        <v>388</v>
+      </c>
+      <c r="C392" s="3">
+        <v>43539</v>
+      </c>
+      <c r="D392" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E392" s="5" t="s">
+        <v>1312</v>
+      </c>
       <c r="F392" s="5"/>
-      <c r="G392" s="5"/>
+      <c r="G392" s="5" t="s">
+        <v>1329</v>
+      </c>
       <c r="H392" s="5"/>
       <c r="I392" s="5"/>
       <c r="J392" s="5"/>
-      <c r="K392" s="5"/>
-      <c r="L392" s="5"/>
+      <c r="K392" s="5">
+        <v>1</v>
+      </c>
+      <c r="L392" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M392" s="5"/>
     </row>
     <row r="393" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B393" s="2"/>
-      <c r="C393" s="3"/>
-      <c r="D393" s="5"/>
-      <c r="E393" s="5"/>
+      <c r="B393" s="2">
+        <v>389</v>
+      </c>
+      <c r="C393" s="3">
+        <v>43539</v>
+      </c>
+      <c r="D393" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E393" s="5" t="s">
+        <v>1313</v>
+      </c>
       <c r="F393" s="5"/>
-      <c r="G393" s="5"/>
+      <c r="G393" s="5" t="s">
+        <v>1330</v>
+      </c>
       <c r="H393" s="5"/>
       <c r="I393" s="5"/>
       <c r="J393" s="5"/>
-      <c r="K393" s="5"/>
-      <c r="L393" s="5"/>
+      <c r="K393" s="5">
+        <v>1</v>
+      </c>
+      <c r="L393" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M393" s="5"/>
     </row>
     <row r="394" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B394" s="2"/>
-      <c r="C394" s="3"/>
-      <c r="D394" s="5"/>
-      <c r="E394" s="5"/>
+      <c r="B394" s="2">
+        <v>390</v>
+      </c>
+      <c r="C394" s="3">
+        <v>43539</v>
+      </c>
+      <c r="D394" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E394" s="5" t="s">
+        <v>1333</v>
+      </c>
       <c r="F394" s="5"/>
-      <c r="G394" s="5"/>
+      <c r="G394" s="5" t="s">
+        <v>1331</v>
+      </c>
       <c r="H394" s="5"/>
       <c r="I394" s="5"/>
       <c r="J394" s="5"/>
-      <c r="K394" s="5"/>
-      <c r="L394" s="5"/>
+      <c r="K394" s="5">
+        <v>1</v>
+      </c>
+      <c r="L394" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M394" s="5"/>
     </row>
     <row r="395" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B395" s="2"/>
-      <c r="C395" s="3"/>
-      <c r="D395" s="5"/>
-      <c r="E395" s="5"/>
+      <c r="B395" s="2">
+        <v>391</v>
+      </c>
+      <c r="C395" s="3">
+        <v>43539</v>
+      </c>
+      <c r="D395" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E395" s="5" t="s">
+        <v>1334</v>
+      </c>
       <c r="F395" s="5"/>
-      <c r="G395" s="5"/>
+      <c r="G395" s="5" t="s">
+        <v>1332</v>
+      </c>
       <c r="H395" s="5"/>
       <c r="I395" s="5"/>
       <c r="J395" s="5"/>
-      <c r="K395" s="5"/>
-      <c r="L395" s="5"/>
+      <c r="K395" s="5">
+        <v>1</v>
+      </c>
+      <c r="L395" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M395" s="5"/>
     </row>
     <row r="396" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B396" s="2"/>
-      <c r="C396" s="3"/>
-      <c r="D396" s="5"/>
-      <c r="E396" s="5"/>
+      <c r="B396" s="2">
+        <v>392</v>
+      </c>
+      <c r="C396" s="3">
+        <v>43540</v>
+      </c>
+      <c r="D396" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E396" s="5" t="s">
+        <v>1335</v>
+      </c>
       <c r="F396" s="5"/>
-      <c r="G396" s="5"/>
+      <c r="G396" s="5" t="s">
+        <v>1340</v>
+      </c>
       <c r="H396" s="5"/>
       <c r="I396" s="5"/>
       <c r="J396" s="5"/>
-      <c r="K396" s="5"/>
-      <c r="L396" s="5"/>
+      <c r="K396" s="5">
+        <v>1</v>
+      </c>
+      <c r="L396" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M396" s="5"/>
     </row>
     <row r="397" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B397" s="2"/>
-      <c r="C397" s="3"/>
-      <c r="D397" s="5"/>
-      <c r="E397" s="5"/>
+      <c r="B397" s="2">
+        <v>393</v>
+      </c>
+      <c r="C397" s="3">
+        <v>43540</v>
+      </c>
+      <c r="D397" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E397" s="5" t="s">
+        <v>1336</v>
+      </c>
       <c r="F397" s="5"/>
-      <c r="G397" s="5"/>
+      <c r="G397" s="5" t="s">
+        <v>1341</v>
+      </c>
       <c r="H397" s="5"/>
       <c r="I397" s="5"/>
       <c r="J397" s="5"/>
-      <c r="K397" s="5"/>
-      <c r="L397" s="5"/>
+      <c r="K397" s="5">
+        <v>1</v>
+      </c>
+      <c r="L397" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M397" s="5"/>
     </row>
     <row r="398" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B398" s="2"/>
-      <c r="C398" s="3"/>
-      <c r="D398" s="5"/>
-      <c r="E398" s="5"/>
+      <c r="B398" s="2">
+        <v>394</v>
+      </c>
+      <c r="C398" s="3">
+        <v>43540</v>
+      </c>
+      <c r="D398" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E398" s="5" t="s">
+        <v>1337</v>
+      </c>
       <c r="F398" s="5"/>
-      <c r="G398" s="5"/>
+      <c r="G398" s="5" t="s">
+        <v>1342</v>
+      </c>
       <c r="H398" s="5"/>
       <c r="I398" s="5"/>
       <c r="J398" s="5"/>
-      <c r="K398" s="5"/>
-      <c r="L398" s="5"/>
+      <c r="K398" s="5">
+        <v>1</v>
+      </c>
+      <c r="L398" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M398" s="5"/>
     </row>
     <row r="399" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B399" s="2"/>
-      <c r="C399" s="3"/>
-      <c r="D399" s="5"/>
-      <c r="E399" s="5"/>
+      <c r="B399" s="2">
+        <v>395</v>
+      </c>
+      <c r="C399" s="3">
+        <v>43540</v>
+      </c>
+      <c r="D399" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E399" s="5" t="s">
+        <v>1338</v>
+      </c>
       <c r="F399" s="5"/>
-      <c r="G399" s="5"/>
+      <c r="G399" s="5" t="s">
+        <v>1343</v>
+      </c>
       <c r="H399" s="5"/>
       <c r="I399" s="5"/>
       <c r="J399" s="5"/>
-      <c r="K399" s="5"/>
-      <c r="L399" s="5"/>
+      <c r="K399" s="5">
+        <v>1</v>
+      </c>
+      <c r="L399" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M399" s="5"/>
     </row>
     <row r="400" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B400" s="2"/>
-      <c r="C400" s="3"/>
-      <c r="D400" s="5"/>
-      <c r="E400" s="5"/>
+      <c r="B400" s="2">
+        <v>396</v>
+      </c>
+      <c r="C400" s="3">
+        <v>43540</v>
+      </c>
+      <c r="D400" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E400" s="5" t="s">
+        <v>1339</v>
+      </c>
       <c r="F400" s="5"/>
-      <c r="G400" s="5"/>
+      <c r="G400" s="5" t="s">
+        <v>1344</v>
+      </c>
       <c r="H400" s="5"/>
       <c r="I400" s="5"/>
       <c r="J400" s="5"/>
-      <c r="K400" s="5"/>
-      <c r="L400" s="5"/>
+      <c r="K400" s="5">
+        <v>1</v>
+      </c>
+      <c r="L400" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M400" s="5"/>
     </row>
     <row r="401" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B401" s="2"/>
-      <c r="C401" s="3"/>
-      <c r="D401" s="5"/>
-      <c r="E401" s="5"/>
+      <c r="B401" s="2">
+        <v>397</v>
+      </c>
+      <c r="C401" s="3">
+        <v>43540</v>
+      </c>
+      <c r="D401" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E401" s="5" t="s">
+        <v>1345</v>
+      </c>
       <c r="F401" s="5"/>
-      <c r="G401" s="5"/>
+      <c r="G401" s="5" t="s">
+        <v>1369</v>
+      </c>
       <c r="H401" s="5"/>
       <c r="I401" s="5"/>
       <c r="J401" s="5"/>
-      <c r="K401" s="5"/>
-      <c r="L401" s="5"/>
+      <c r="K401" s="5">
+        <v>1</v>
+      </c>
+      <c r="L401" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M401" s="5"/>
     </row>
     <row r="402" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B402" s="2"/>
-      <c r="C402" s="3"/>
-      <c r="D402" s="5"/>
-      <c r="E402" s="5"/>
+      <c r="B402" s="2">
+        <v>398</v>
+      </c>
+      <c r="C402" s="3">
+        <v>43540</v>
+      </c>
+      <c r="D402" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E402" s="5" t="s">
+        <v>1346</v>
+      </c>
       <c r="F402" s="5"/>
-      <c r="G402" s="5"/>
+      <c r="G402" s="5" t="s">
+        <v>1370</v>
+      </c>
       <c r="H402" s="5"/>
       <c r="I402" s="5"/>
       <c r="J402" s="5"/>
-      <c r="K402" s="5"/>
-      <c r="L402" s="5"/>
+      <c r="K402" s="5">
+        <v>1</v>
+      </c>
+      <c r="L402" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M402" s="5"/>
     </row>
     <row r="403" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B403" s="2"/>
-      <c r="C403" s="3"/>
-      <c r="D403" s="5"/>
-      <c r="E403" s="5"/>
+      <c r="B403" s="2">
+        <v>399</v>
+      </c>
+      <c r="C403" s="3">
+        <v>43540</v>
+      </c>
+      <c r="D403" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E403" s="5" t="s">
+        <v>1347</v>
+      </c>
       <c r="F403" s="5"/>
-      <c r="G403" s="5"/>
+      <c r="G403" s="5" t="s">
+        <v>1371</v>
+      </c>
       <c r="H403" s="5"/>
       <c r="I403" s="5"/>
       <c r="J403" s="5"/>
-      <c r="K403" s="5"/>
-      <c r="L403" s="5"/>
+      <c r="K403" s="5">
+        <v>1</v>
+      </c>
+      <c r="L403" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M403" s="5"/>
     </row>
     <row r="404" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B404" s="2"/>
-      <c r="C404" s="3"/>
-      <c r="D404" s="5"/>
-      <c r="E404" s="5"/>
+      <c r="B404" s="2">
+        <v>400</v>
+      </c>
+      <c r="C404" s="3">
+        <v>43540</v>
+      </c>
+      <c r="D404" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E404" s="5" t="s">
+        <v>1348</v>
+      </c>
       <c r="F404" s="5"/>
-      <c r="G404" s="5"/>
+      <c r="G404" s="5" t="s">
+        <v>1372</v>
+      </c>
       <c r="H404" s="5"/>
       <c r="I404" s="5"/>
       <c r="J404" s="5"/>
-      <c r="K404" s="5"/>
-      <c r="L404" s="5"/>
+      <c r="K404" s="5">
+        <v>1</v>
+      </c>
+      <c r="L404" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M404" s="5"/>
     </row>
     <row r="405" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B405" s="2"/>
-      <c r="C405" s="3"/>
-      <c r="D405" s="5"/>
-      <c r="E405" s="5"/>
+      <c r="B405" s="2">
+        <v>401</v>
+      </c>
+      <c r="C405" s="3">
+        <v>43540</v>
+      </c>
+      <c r="D405" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E405" s="5" t="s">
+        <v>1349</v>
+      </c>
       <c r="F405" s="5"/>
-      <c r="G405" s="5"/>
+      <c r="G405" s="5" t="s">
+        <v>1373</v>
+      </c>
       <c r="H405" s="5"/>
       <c r="I405" s="5"/>
       <c r="J405" s="5"/>
-      <c r="K405" s="5"/>
-      <c r="L405" s="5"/>
+      <c r="K405" s="5">
+        <v>1</v>
+      </c>
+      <c r="L405" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M405" s="5"/>
     </row>
     <row r="406" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B406" s="2"/>
-      <c r="C406" s="3"/>
-      <c r="D406" s="5"/>
-      <c r="E406" s="5"/>
+      <c r="B406" s="2">
+        <v>402</v>
+      </c>
+      <c r="C406" s="3">
+        <v>43540</v>
+      </c>
+      <c r="D406" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E406" s="5" t="s">
+        <v>1350</v>
+      </c>
       <c r="F406" s="5"/>
-      <c r="G406" s="5"/>
+      <c r="G406" s="5" t="s">
+        <v>1350</v>
+      </c>
       <c r="H406" s="5"/>
       <c r="I406" s="5"/>
       <c r="J406" s="5"/>
-      <c r="K406" s="5"/>
-      <c r="L406" s="5"/>
+      <c r="K406" s="5">
+        <v>1</v>
+      </c>
+      <c r="L406" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M406" s="5"/>
     </row>
     <row r="407" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B407" s="2"/>
-      <c r="C407" s="3"/>
-      <c r="D407" s="5"/>
-      <c r="E407" s="5"/>
+      <c r="B407" s="2">
+        <v>403</v>
+      </c>
+      <c r="C407" s="3">
+        <v>43540</v>
+      </c>
+      <c r="D407" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E407" s="5" t="s">
+        <v>1351</v>
+      </c>
       <c r="F407" s="5"/>
-      <c r="G407" s="5"/>
+      <c r="G407" s="5" t="s">
+        <v>1351</v>
+      </c>
       <c r="H407" s="5"/>
       <c r="I407" s="5"/>
       <c r="J407" s="5"/>
-      <c r="K407" s="5"/>
-      <c r="L407" s="5"/>
+      <c r="K407" s="5">
+        <v>1</v>
+      </c>
+      <c r="L407" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M407" s="5"/>
     </row>
     <row r="408" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B408" s="2"/>
-      <c r="C408" s="3"/>
-      <c r="D408" s="5"/>
-      <c r="E408" s="5"/>
+      <c r="B408" s="2">
+        <v>404</v>
+      </c>
+      <c r="C408" s="3">
+        <v>43540</v>
+      </c>
+      <c r="D408" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E408" s="5" t="s">
+        <v>1352</v>
+      </c>
       <c r="F408" s="5"/>
-      <c r="G408" s="5"/>
+      <c r="G408" s="5" t="s">
+        <v>1374</v>
+      </c>
       <c r="H408" s="5"/>
       <c r="I408" s="5"/>
       <c r="J408" s="5"/>
-      <c r="K408" s="5"/>
-      <c r="L408" s="5"/>
+      <c r="K408" s="5">
+        <v>1</v>
+      </c>
+      <c r="L408" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M408" s="5"/>
     </row>
     <row r="409" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B409" s="2"/>
-      <c r="C409" s="3"/>
-      <c r="D409" s="5"/>
-      <c r="E409" s="5"/>
+      <c r="B409" s="2">
+        <v>405</v>
+      </c>
+      <c r="C409" s="3">
+        <v>43540</v>
+      </c>
+      <c r="D409" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E409" s="5" t="s">
+        <v>1353</v>
+      </c>
       <c r="F409" s="5"/>
-      <c r="G409" s="5"/>
+      <c r="G409" s="5" t="s">
+        <v>1375</v>
+      </c>
       <c r="H409" s="5"/>
       <c r="I409" s="5"/>
       <c r="J409" s="5"/>
-      <c r="K409" s="5"/>
-      <c r="L409" s="5"/>
+      <c r="K409" s="5">
+        <v>1</v>
+      </c>
+      <c r="L409" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M409" s="5"/>
     </row>
     <row r="410" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B410" s="2"/>
-      <c r="C410" s="3"/>
-      <c r="D410" s="5"/>
-      <c r="E410" s="5"/>
+      <c r="B410" s="2">
+        <v>406</v>
+      </c>
+      <c r="C410" s="3">
+        <v>43540</v>
+      </c>
+      <c r="D410" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E410" s="5" t="s">
+        <v>1354</v>
+      </c>
       <c r="F410" s="5"/>
-      <c r="G410" s="5"/>
+      <c r="G410" s="5" t="s">
+        <v>1376</v>
+      </c>
       <c r="H410" s="5"/>
       <c r="I410" s="5"/>
       <c r="J410" s="5"/>
-      <c r="K410" s="5"/>
-      <c r="L410" s="5"/>
+      <c r="K410" s="5">
+        <v>1</v>
+      </c>
+      <c r="L410" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M410" s="5"/>
     </row>
     <row r="411" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B411" s="2"/>
-      <c r="C411" s="3"/>
-      <c r="D411" s="5"/>
-      <c r="E411" s="5"/>
+      <c r="B411" s="2">
+        <v>407</v>
+      </c>
+      <c r="C411" s="3">
+        <v>43540</v>
+      </c>
+      <c r="D411" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E411" s="5" t="s">
+        <v>1355</v>
+      </c>
       <c r="F411" s="5"/>
-      <c r="G411" s="5"/>
+      <c r="G411" s="5" t="s">
+        <v>1377</v>
+      </c>
       <c r="H411" s="5"/>
       <c r="I411" s="5"/>
       <c r="J411" s="5"/>
-      <c r="K411" s="5"/>
-      <c r="L411" s="5"/>
+      <c r="K411" s="5">
+        <v>1</v>
+      </c>
+      <c r="L411" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M411" s="5"/>
     </row>
     <row r="412" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B412" s="2"/>
-      <c r="C412" s="3"/>
-      <c r="D412" s="5"/>
-      <c r="E412" s="5"/>
+      <c r="B412" s="2">
+        <v>408</v>
+      </c>
+      <c r="C412" s="3">
+        <v>43540</v>
+      </c>
+      <c r="D412" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E412" s="5" t="s">
+        <v>1356</v>
+      </c>
       <c r="F412" s="5"/>
-      <c r="G412" s="5"/>
+      <c r="G412" s="5" t="s">
+        <v>1378</v>
+      </c>
       <c r="H412" s="5"/>
       <c r="I412" s="5"/>
       <c r="J412" s="5"/>
-      <c r="K412" s="5"/>
-      <c r="L412" s="5"/>
+      <c r="K412" s="5">
+        <v>1</v>
+      </c>
+      <c r="L412" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M412" s="5"/>
     </row>
     <row r="413" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B413" s="2"/>
-      <c r="C413" s="3"/>
-      <c r="D413" s="5"/>
-      <c r="E413" s="5"/>
+      <c r="B413" s="2">
+        <v>409</v>
+      </c>
+      <c r="C413" s="3">
+        <v>43540</v>
+      </c>
+      <c r="D413" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E413" s="5" t="s">
+        <v>1357</v>
+      </c>
       <c r="F413" s="5"/>
-      <c r="G413" s="5"/>
+      <c r="G413" s="5" t="s">
+        <v>1379</v>
+      </c>
       <c r="H413" s="5"/>
       <c r="I413" s="5"/>
       <c r="J413" s="5"/>
-      <c r="K413" s="5"/>
-      <c r="L413" s="5"/>
+      <c r="K413" s="5">
+        <v>1</v>
+      </c>
+      <c r="L413" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M413" s="5"/>
     </row>
     <row r="414" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B414" s="2"/>
-      <c r="C414" s="3"/>
-      <c r="D414" s="5"/>
-      <c r="E414" s="5"/>
+      <c r="B414" s="2">
+        <v>410</v>
+      </c>
+      <c r="C414" s="3">
+        <v>43540</v>
+      </c>
+      <c r="D414" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E414" s="5" t="s">
+        <v>1358</v>
+      </c>
       <c r="F414" s="5"/>
-      <c r="G414" s="5"/>
+      <c r="G414" s="5" t="s">
+        <v>1380</v>
+      </c>
       <c r="H414" s="5"/>
       <c r="I414" s="5"/>
       <c r="J414" s="5"/>
-      <c r="K414" s="5"/>
-      <c r="L414" s="5"/>
+      <c r="K414" s="5">
+        <v>1</v>
+      </c>
+      <c r="L414" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M414" s="5"/>
     </row>
     <row r="415" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B415" s="2"/>
-      <c r="C415" s="3"/>
-      <c r="D415" s="5"/>
-      <c r="E415" s="5"/>
+      <c r="B415" s="2">
+        <v>411</v>
+      </c>
+      <c r="C415" s="3">
+        <v>43540</v>
+      </c>
+      <c r="D415" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E415" s="5" t="s">
+        <v>1359</v>
+      </c>
       <c r="F415" s="5"/>
-      <c r="G415" s="5"/>
+      <c r="G415" s="5" t="s">
+        <v>1381</v>
+      </c>
       <c r="H415" s="5"/>
       <c r="I415" s="5"/>
       <c r="J415" s="5"/>
-      <c r="K415" s="5"/>
-      <c r="L415" s="5"/>
+      <c r="K415" s="5">
+        <v>1</v>
+      </c>
+      <c r="L415" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M415" s="5"/>
     </row>
     <row r="416" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B416" s="2"/>
-      <c r="C416" s="3"/>
-      <c r="D416" s="5"/>
-      <c r="E416" s="5"/>
+      <c r="B416" s="2">
+        <v>412</v>
+      </c>
+      <c r="C416" s="3">
+        <v>43540</v>
+      </c>
+      <c r="D416" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E416" s="5" t="s">
+        <v>1360</v>
+      </c>
       <c r="F416" s="5"/>
-      <c r="G416" s="5"/>
+      <c r="G416" s="5" t="s">
+        <v>1382</v>
+      </c>
       <c r="H416" s="5"/>
       <c r="I416" s="5"/>
       <c r="J416" s="5"/>
-      <c r="K416" s="5"/>
-      <c r="L416" s="5"/>
+      <c r="K416" s="5">
+        <v>1</v>
+      </c>
+      <c r="L416" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M416" s="5"/>
     </row>
     <row r="417" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B417" s="2"/>
-      <c r="C417" s="3"/>
-      <c r="D417" s="5"/>
-      <c r="E417" s="5"/>
+      <c r="B417" s="2">
+        <v>413</v>
+      </c>
+      <c r="C417" s="3">
+        <v>43540</v>
+      </c>
+      <c r="D417" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E417" s="5" t="s">
+        <v>1361</v>
+      </c>
       <c r="F417" s="5"/>
-      <c r="G417" s="5"/>
+      <c r="G417" s="5" t="s">
+        <v>1383</v>
+      </c>
       <c r="H417" s="5"/>
       <c r="I417" s="5"/>
       <c r="J417" s="5"/>
-      <c r="K417" s="5"/>
-      <c r="L417" s="5"/>
+      <c r="K417" s="5">
+        <v>1</v>
+      </c>
+      <c r="L417" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M417" s="5"/>
     </row>
     <row r="418" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B418" s="2"/>
-      <c r="C418" s="3"/>
-      <c r="D418" s="5"/>
-      <c r="E418" s="5"/>
+      <c r="B418" s="2">
+        <v>414</v>
+      </c>
+      <c r="C418" s="3">
+        <v>43540</v>
+      </c>
+      <c r="D418" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E418" s="5" t="s">
+        <v>1362</v>
+      </c>
       <c r="F418" s="5"/>
-      <c r="G418" s="5"/>
+      <c r="G418" s="5" t="s">
+        <v>1384</v>
+      </c>
       <c r="H418" s="5"/>
       <c r="I418" s="5"/>
       <c r="J418" s="5"/>
-      <c r="K418" s="5"/>
-      <c r="L418" s="5"/>
+      <c r="K418" s="5">
+        <v>1</v>
+      </c>
+      <c r="L418" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M418" s="5"/>
     </row>
     <row r="419" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B419" s="2"/>
-      <c r="C419" s="3"/>
-      <c r="D419" s="5"/>
-      <c r="E419" s="5"/>
+      <c r="B419" s="2">
+        <v>415</v>
+      </c>
+      <c r="C419" s="3">
+        <v>43540</v>
+      </c>
+      <c r="D419" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E419" s="5" t="s">
+        <v>1363</v>
+      </c>
       <c r="F419" s="5"/>
-      <c r="G419" s="5"/>
+      <c r="G419" s="5" t="s">
+        <v>1385</v>
+      </c>
       <c r="H419" s="5"/>
       <c r="I419" s="5"/>
       <c r="J419" s="5"/>
-      <c r="K419" s="5"/>
-      <c r="L419" s="5"/>
+      <c r="K419" s="5">
+        <v>1</v>
+      </c>
+      <c r="L419" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M419" s="5"/>
     </row>
     <row r="420" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B420" s="2"/>
-      <c r="C420" s="3"/>
-      <c r="D420" s="5"/>
-      <c r="E420" s="5"/>
+      <c r="B420" s="2">
+        <v>416</v>
+      </c>
+      <c r="C420" s="3">
+        <v>43540</v>
+      </c>
+      <c r="D420" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E420" s="5" t="s">
+        <v>1364</v>
+      </c>
       <c r="F420" s="5"/>
-      <c r="G420" s="5"/>
+      <c r="G420" s="5" t="s">
+        <v>1386</v>
+      </c>
       <c r="H420" s="5"/>
       <c r="I420" s="5"/>
       <c r="J420" s="5"/>
-      <c r="K420" s="5"/>
-      <c r="L420" s="5"/>
+      <c r="K420" s="5">
+        <v>1</v>
+      </c>
+      <c r="L420" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M420" s="5"/>
     </row>
     <row r="421" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B421" s="2"/>
-      <c r="C421" s="3"/>
-      <c r="D421" s="5"/>
-      <c r="E421" s="5"/>
+      <c r="B421" s="2">
+        <v>417</v>
+      </c>
+      <c r="C421" s="3">
+        <v>43540</v>
+      </c>
+      <c r="D421" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E421" s="5" t="s">
+        <v>1365</v>
+      </c>
       <c r="F421" s="5"/>
-      <c r="G421" s="5"/>
+      <c r="G421" s="5" t="s">
+        <v>1387</v>
+      </c>
       <c r="H421" s="5"/>
       <c r="I421" s="5"/>
       <c r="J421" s="5"/>
-      <c r="K421" s="5"/>
-      <c r="L421" s="5"/>
+      <c r="K421" s="5">
+        <v>1</v>
+      </c>
+      <c r="L421" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M421" s="5"/>
     </row>
     <row r="422" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B422" s="2"/>
-      <c r="C422" s="3"/>
-      <c r="D422" s="5"/>
-      <c r="E422" s="5"/>
+      <c r="B422" s="2">
+        <v>418</v>
+      </c>
+      <c r="C422" s="3">
+        <v>43540</v>
+      </c>
+      <c r="D422" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E422" s="5" t="s">
+        <v>1366</v>
+      </c>
       <c r="F422" s="5"/>
-      <c r="G422" s="5"/>
+      <c r="G422" s="5" t="s">
+        <v>1388</v>
+      </c>
       <c r="H422" s="5"/>
       <c r="I422" s="5"/>
       <c r="J422" s="5"/>
-      <c r="K422" s="5"/>
-      <c r="L422" s="5"/>
+      <c r="K422" s="5">
+        <v>1</v>
+      </c>
+      <c r="L422" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M422" s="5"/>
     </row>
     <row r="423" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B423" s="2"/>
-      <c r="C423" s="3"/>
-      <c r="D423" s="5"/>
-      <c r="E423" s="5"/>
+      <c r="B423" s="2">
+        <v>419</v>
+      </c>
+      <c r="C423" s="3">
+        <v>43540</v>
+      </c>
+      <c r="D423" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E423" s="5" t="s">
+        <v>1367</v>
+      </c>
       <c r="F423" s="5"/>
-      <c r="G423" s="5"/>
+      <c r="G423" s="5" t="s">
+        <v>1389</v>
+      </c>
       <c r="H423" s="5"/>
       <c r="I423" s="5"/>
       <c r="J423" s="5"/>
-      <c r="K423" s="5"/>
-      <c r="L423" s="5"/>
+      <c r="K423" s="5">
+        <v>1</v>
+      </c>
+      <c r="L423" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M423" s="5"/>
     </row>
     <row r="424" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B424" s="2"/>
-      <c r="C424" s="3"/>
-      <c r="D424" s="5"/>
-      <c r="E424" s="5"/>
+      <c r="B424" s="2">
+        <v>420</v>
+      </c>
+      <c r="C424" s="3">
+        <v>43540</v>
+      </c>
+      <c r="D424" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E424" s="5" t="s">
+        <v>1368</v>
+      </c>
       <c r="F424" s="5"/>
-      <c r="G424" s="5"/>
+      <c r="G424" s="5" t="s">
+        <v>1390</v>
+      </c>
       <c r="H424" s="5"/>
       <c r="I424" s="5"/>
       <c r="J424" s="5"/>
-      <c r="K424" s="5"/>
-      <c r="L424" s="5"/>
+      <c r="K424" s="5">
+        <v>1</v>
+      </c>
+      <c r="L424" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="M424" s="5"/>
     </row>
     <row r="425" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
@@ -16287,53 +17952,25 @@
       <c r="L518" s="5"/>
       <c r="M518" s="5"/>
     </row>
-    <row r="519" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B519" s="2"/>
-      <c r="C519" s="3"/>
-      <c r="D519" s="5"/>
-      <c r="E519" s="5"/>
-      <c r="F519" s="5"/>
-      <c r="G519" s="5"/>
-      <c r="H519" s="5"/>
-      <c r="I519" s="5"/>
-      <c r="J519" s="5"/>
-      <c r="K519" s="5"/>
-      <c r="L519" s="5"/>
-      <c r="M519" s="5"/>
-    </row>
-    <row r="520" spans="2:13" ht="29.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B520" s="2"/>
-      <c r="C520" s="3"/>
-      <c r="D520" s="5"/>
-      <c r="E520" s="5"/>
-      <c r="F520" s="5"/>
-      <c r="G520" s="5"/>
-      <c r="H520" s="5"/>
-      <c r="I520" s="5"/>
-      <c r="J520" s="5"/>
-      <c r="K520" s="5"/>
-      <c r="L520" s="5"/>
-      <c r="M520" s="5"/>
-    </row>
   </sheetData>
-  <autoFilter ref="B4:M190"/>
+  <autoFilter ref="B4:M424"/>
   <mergeCells count="1">
     <mergeCell ref="B2:L2"/>
   </mergeCells>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D115 D343:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D115 D425:D1048576">
       <formula1>"Likeshuo,TOEFL,TPO"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D116:D257">
       <formula1>"Likeshuo,TOEFL,TPO, 500 setns"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D258:D342">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D258:D424">
       <formula1>"Likeshuo,TOEFL,TPO, 500 setns, NCE4"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L5:L520">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L5:L518">
       <formula1>"Input, Renew, Understood, Reviewed, Forgot"</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C520">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C518">
       <formula1>43508</formula1>
     </dataValidation>
   </dataValidations>
@@ -16350,8 +17987,8 @@
   <dimension ref="B1:M410"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F95" sqref="F95"/>
+      <pane ySplit="4" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M2" sqref="B2:M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
@@ -16367,20 +18004,20 @@
   <sheetData>
     <row r="1" spans="2:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:13" ht="32.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="6" t="s">
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="8" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>